<commit_message>
Best SEMAINE model ready for submission.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="2"/>
@@ -12,13 +12,12 @@
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="99">
   <si>
     <t>DEVEL</t>
   </si>
@@ -162,9 +161,6 @@
   </si>
   <si>
     <t>Trained on intensity (dynamic)</t>
-  </si>
-  <si>
-    <t>Trained on intensity (dynamic, shifted)</t>
   </si>
   <si>
     <t>Corr</t>
@@ -313,12 +309,18 @@
   <si>
     <t>Static intensity geom SVM</t>
   </si>
+  <si>
+    <t>Combined SVM static geometry</t>
+  </si>
+  <si>
+    <t>Combined SVM</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,6 +505,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,7 +518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -606,7 +608,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -641,7 +642,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -817,82 +817,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:37">
+      <c r="B1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="33" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="33" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="33" t="s">
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33" t="s">
+      <c r="O1" s="32"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="33" t="s">
+      <c r="R1" s="32"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="33" t="s">
+      <c r="U1" s="32"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="33" t="s">
+      <c r="X1" s="32"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="33" t="s">
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="31" t="s">
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="31" t="s">
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="32"/>
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="33"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>0.54469999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>0.23713333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>0.53643333333333332</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>0.56054285714285712</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>0.54634285714285713</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
         <v>46</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>0.74680000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
         <v>47</v>
       </c>
@@ -2569,9 +2569,9 @@
         <v>0.71243999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="7">
         <v>0.3674</v>
@@ -2685,9 +2685,9 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="7">
         <v>0.3196</v>
@@ -2801,9 +2801,9 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="7">
         <v>0.47939999999999999</v>
@@ -2917,9 +2917,9 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="7">
         <v>0.38929999999999998</v>
@@ -3033,9 +3033,9 @@
         <v>0.59650909090909088</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="7">
         <v>0.3362</v>
@@ -3149,9 +3149,9 @@
         <v>0.5917</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="7">
         <v>0.36730000000000002</v>
@@ -3265,9 +3265,9 @@
         <v>0.61232727272727272</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="7">
         <v>0.3624</v>
@@ -3381,9 +3381,9 @@
         <v>0.58963636363636374</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="7">
         <v>0.3306</v>
@@ -3497,9 +3497,9 @@
         <v>0.57887272727272732</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="7">
         <v>0.41089999999999999</v>
@@ -3613,9 +3613,9 @@
         <v>0.60222727272727272</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="7">
         <v>0.43840000000000001</v>
@@ -3705,9 +3705,9 @@
         <v>0.57781428571428584</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="7">
         <v>0.3584</v>
@@ -3821,9 +3821,9 @@
         <v>0.60204545454545466</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37">
       <c r="A31" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="7">
         <v>0.49170000000000003</v>
@@ -3913,86 +3913,215 @@
         <v>0.57524285714285717</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37">
       <c r="A32" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="8"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="8"/>
-      <c r="AH32" s="9"/>
-      <c r="AI32" s="10"/>
-      <c r="AJ32" s="11"/>
-      <c r="AK32" s="12"/>
+        <v>84</v>
+      </c>
+      <c r="B32" s="7">
+        <v>0.36620000000000003</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0.52280000000000004</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.43070000000000003</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.31979999999999997</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0.30370000000000003</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0.3115</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0.43049999999999999</v>
+      </c>
+      <c r="I32" s="8">
+        <v>0.6452</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.51649999999999996</v>
+      </c>
+      <c r="K32" s="7">
+        <v>0.69079999999999997</v>
+      </c>
+      <c r="L32" s="8">
+        <v>0.90049999999999997</v>
+      </c>
+      <c r="M32" s="8">
+        <v>0.78180000000000005</v>
+      </c>
+      <c r="N32" s="7">
+        <v>0.64480000000000004</v>
+      </c>
+      <c r="O32" s="8">
+        <v>0.92090000000000005</v>
+      </c>
+      <c r="P32" s="8">
+        <v>0.75849999999999995</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="R32" s="8">
+        <v>0.95420000000000005</v>
+      </c>
+      <c r="S32" s="8">
+        <v>0.83040000000000003</v>
+      </c>
+      <c r="T32" s="7">
+        <v>0.8125</v>
+      </c>
+      <c r="U32" s="8">
+        <v>0.9113</v>
+      </c>
+      <c r="V32" s="8">
+        <v>0.85909999999999997</v>
+      </c>
+      <c r="W32" s="7">
+        <v>0.46850000000000003</v>
+      </c>
+      <c r="X32" s="8">
+        <v>0.90839999999999999</v>
+      </c>
+      <c r="Y32" s="8">
+        <v>0.61819999999999997</v>
+      </c>
+      <c r="Z32" s="7">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="AA32" s="8">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="AB32" s="8">
+        <v>0.3362</v>
+      </c>
+      <c r="AC32" s="7">
+        <v>0.52759999999999996</v>
+      </c>
+      <c r="AD32" s="8">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AE32" s="8">
+        <v>0.62680000000000002</v>
+      </c>
+      <c r="AF32" s="7">
+        <v>0.45629999999999998</v>
+      </c>
+      <c r="AG32" s="8">
+        <v>0.33389999999999997</v>
+      </c>
+      <c r="AH32" s="9">
+        <v>0.3856</v>
+      </c>
+      <c r="AI32" s="10">
+        <f t="shared" ref="AI32" si="6">AVERAGE(B32,E32,H32,K32,N32,Q32,T32,W32,Z32,AC32,AF32)</f>
+        <v>0.52136363636363636</v>
+      </c>
+      <c r="AJ32" s="11">
+        <f t="shared" ref="AJ32" si="7">AVERAGE(C32,F32,I32,L32,O32,R32,U32,X32,AA32,AD32,AG32)</f>
+        <v>0.68971818181818179</v>
+      </c>
+      <c r="AK32" s="12">
+        <f t="shared" ref="AK32" si="8">AVERAGE(D32,G32,J32,M32,P32,S32,V32,Y32,AB32,AE32,AH32)</f>
+        <v>0.58684545454545445</v>
+      </c>
     </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+    <row r="33" spans="1:37">
+      <c r="A33" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="7">
+        <v>0.34839999999999999</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.53639999999999999</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.4224</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.28470000000000001</v>
+      </c>
+      <c r="F33" s="8">
+        <v>0.40970000000000001</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0.38590000000000002</v>
+      </c>
+      <c r="I33" s="8">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.44729999999999998</v>
+      </c>
+      <c r="K33" s="7">
+        <v>0.68330000000000002</v>
+      </c>
+      <c r="L33" s="8">
+        <v>0.89229999999999998</v>
+      </c>
+      <c r="M33" s="8">
+        <v>0.77390000000000003</v>
+      </c>
       <c r="N33" s="7"/>
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
       <c r="Q33" s="7"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
+      <c r="T33" s="7">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="U33" s="8">
+        <v>0.90959999999999996</v>
+      </c>
+      <c r="V33" s="8">
+        <v>0.87190000000000001</v>
+      </c>
       <c r="W33" s="7"/>
       <c r="X33" s="8"/>
       <c r="Y33" s="8"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="8"/>
-      <c r="AC33" s="7"/>
-      <c r="AD33" s="8"/>
-      <c r="AE33" s="8"/>
+      <c r="Z33" s="7">
+        <v>0.34649999999999997</v>
+      </c>
+      <c r="AA33" s="8">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="AB33" s="8">
+        <v>0.44030000000000002</v>
+      </c>
+      <c r="AC33" s="7">
+        <v>0.48520000000000002</v>
+      </c>
+      <c r="AD33" s="8">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="AE33" s="8">
+        <v>0.59009999999999996</v>
+      </c>
       <c r="AF33" s="7"/>
       <c r="AG33" s="8"/>
       <c r="AH33" s="9"/>
-      <c r="AI33" s="10"/>
-      <c r="AJ33" s="11"/>
-      <c r="AK33" s="12"/>
+      <c r="AI33" s="10">
+        <f t="shared" ref="AI33" si="9">AVERAGE(B33,E33,H33,K33,N33,Q33,T33,W33,Z33,AC33,AF33)</f>
+        <v>0.48159999999999997</v>
+      </c>
+      <c r="AJ33" s="11">
+        <f t="shared" ref="AJ33" si="10">AVERAGE(C33,F33,I33,L33,O33,R33,U33,X33,AA33,AD33,AG33)</f>
+        <v>0.66241428571428584</v>
+      </c>
+      <c r="AK33" s="12">
+        <f t="shared" ref="AK33" si="11">AVERAGE(D33,G33,J33,M33,P33,S33,V33,Y33,AB33,AE33,AH33)</f>
+        <v>0.55455714285714286</v>
+      </c>
     </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37">
       <c r="B34" s="7"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
@@ -4030,7 +4159,7 @@
       <c r="AJ34" s="11"/>
       <c r="AK34" s="12"/>
     </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
@@ -4068,7 +4197,7 @@
       <c r="AJ35" s="11"/>
       <c r="AK35" s="12"/>
     </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37">
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
@@ -4106,7 +4235,7 @@
       <c r="AJ36" s="11"/>
       <c r="AK36" s="12"/>
     </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
@@ -4144,7 +4273,7 @@
       <c r="AJ37" s="11"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
@@ -4182,7 +4311,7 @@
       <c r="AJ38" s="11"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
@@ -4220,7 +4349,7 @@
       <c r="AJ39" s="11"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
@@ -4276,9 +4405,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="76">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4288,9 +4417,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="75">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4300,9 +4429,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="74">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4312,9 +4441,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="73">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4324,9 +4453,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="72">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4336,9 +4465,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="71">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4348,9 +4477,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4360,9 +4489,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4372,9 +4501,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4384,9 +4513,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4396,9 +4525,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4408,9 +4537,9 @@
   <conditionalFormatting sqref="AK3:AK40">
     <cfRule type="colorScale" priority="65">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4420,9 +4549,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="64">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4432,9 +4561,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4444,9 +4573,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4456,9 +4585,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4468,9 +4597,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4480,9 +4609,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4492,9 +4621,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4504,9 +4633,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4516,9 +4645,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4528,9 +4657,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4540,9 +4669,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4552,9 +4681,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4564,9 +4693,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4576,9 +4705,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4588,9 +4717,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4600,9 +4729,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4612,9 +4741,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4624,9 +4753,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4636,9 +4765,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4648,9 +4777,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4660,9 +4789,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4672,9 +4801,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4684,9 +4813,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4696,9 +4825,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4708,9 +4837,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4720,9 +4849,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4732,9 +4861,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4744,9 +4873,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4756,9 +4885,9 @@
   <conditionalFormatting sqref="P3:P25 P27:P40">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4768,9 +4897,9 @@
   <conditionalFormatting sqref="J3:J25 X29:X40 J27:J40">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4780,9 +4909,9 @@
   <conditionalFormatting sqref="G3:G25 G27:G40">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4792,9 +4921,9 @@
   <conditionalFormatting sqref="D3:D25 D27:D40">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4804,9 +4933,9 @@
   <conditionalFormatting sqref="AH3:AH25 AH27:AH40">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4816,9 +4945,9 @@
   <conditionalFormatting sqref="AE3:AE25 AE27:AE40">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4828,9 +4957,9 @@
   <conditionalFormatting sqref="AB3:AB25 AB27:AB40">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4840,9 +4969,9 @@
   <conditionalFormatting sqref="Y3:Y25 Y27:Y40">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4852,9 +4981,9 @@
   <conditionalFormatting sqref="M3:M25 M27:M40">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4864,9 +4993,9 @@
   <conditionalFormatting sqref="V3:V25 V27:V40">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4876,9 +5005,9 @@
   <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4888,9 +5017,9 @@
   <conditionalFormatting sqref="S26:S40">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4900,9 +5029,9 @@
   <conditionalFormatting sqref="P26:P40">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4912,9 +5041,9 @@
   <conditionalFormatting sqref="J26:J40">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4924,9 +5053,9 @@
   <conditionalFormatting sqref="G26:G40">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4936,9 +5065,9 @@
   <conditionalFormatting sqref="D26:D40">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4948,9 +5077,9 @@
   <conditionalFormatting sqref="AH26:AH40">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4960,9 +5089,9 @@
   <conditionalFormatting sqref="AE26:AE40">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4972,9 +5101,9 @@
   <conditionalFormatting sqref="AB26:AB40">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4984,9 +5113,9 @@
   <conditionalFormatting sqref="Y26:Y40">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4996,9 +5125,9 @@
   <conditionalFormatting sqref="M26:M40">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5008,9 +5137,9 @@
   <conditionalFormatting sqref="V26:V40">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5020,9 +5149,9 @@
   <conditionalFormatting sqref="AH3:AH40">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5032,9 +5161,9 @@
   <conditionalFormatting sqref="AE3:AE40">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5044,9 +5173,9 @@
   <conditionalFormatting sqref="AB3:AB40">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5056,9 +5185,9 @@
   <conditionalFormatting sqref="Y3:Y40">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5068,9 +5197,9 @@
   <conditionalFormatting sqref="V3:V40">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5080,9 +5209,9 @@
   <conditionalFormatting sqref="S3:S40">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5092,9 +5221,9 @@
   <conditionalFormatting sqref="P3:P40">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5104,9 +5233,9 @@
   <conditionalFormatting sqref="M3:M40">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5116,9 +5245,9 @@
   <conditionalFormatting sqref="J3:J40">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5128,9 +5257,9 @@
   <conditionalFormatting sqref="G3:G40">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5140,9 +5269,9 @@
   <conditionalFormatting sqref="D3:D40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5155,14 +5284,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -5183,56 +5312,56 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:34">
+      <c r="B1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="33" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="33" t="s">
+      <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="32"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="33" t="s">
+      <c r="R1" s="32"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34"/>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="34"/>
-      <c r="AF1" s="34"/>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="34"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5300,9 +5429,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="10">
         <v>0.46100000000000002</v>
@@ -5359,7 +5488,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -5418,9 +5547,9 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="10">
         <v>0.16</v>
@@ -5477,9 +5606,9 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="10">
         <v>0.40400000000000003</v>
@@ -5536,7 +5665,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -5607,7 +5736,7 @@
         <v>0.28861666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -5678,7 +5807,7 @@
         <v>0.32611666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -5749,7 +5878,7 @@
         <v>0.30031666666666662</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -5820,7 +5949,7 @@
         <v>0.33934999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
@@ -5873,7 +6002,7 @@
         <v>0.26416666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -5926,7 +6055,7 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -5979,7 +6108,7 @@
         <v>0.28023333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -6032,7 +6161,7 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -6091,7 +6220,7 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
@@ -6150,7 +6279,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
@@ -6221,7 +6350,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -6292,7 +6421,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -6363,7 +6492,7 @@
         <v>0.21026666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -6434,9 +6563,9 @@
         <v>0.33863333333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22">
       <c r="A21" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="7">
         <v>0.26500000000000001</v>
@@ -6505,9 +6634,9 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="7">
         <v>0.4204</v>
@@ -6576,9 +6705,9 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="7">
         <v>0.18329999999999999</v>
@@ -6647,9 +6776,9 @@
         <v>0.2364333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22">
       <c r="A24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="7">
         <v>0.52569999999999995</v>
@@ -6718,9 +6847,9 @@
         <v>0.36651666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22">
       <c r="A25" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="7">
         <v>0.1444</v>
@@ -6777,9 +6906,9 @@
         <v>0.36202499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22">
       <c r="A26" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="7">
         <v>0.1961</v>
@@ -6836,9 +6965,9 @@
         <v>0.38167500000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22">
       <c r="A27" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="7">
         <v>0.5837</v>
@@ -6907,9 +7036,9 @@
         <v>0.3566833333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22">
       <c r="A28" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="7">
         <v>0.26919999999999999</v>
@@ -6978,9 +7107,9 @@
         <v>0.31143333333333334</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22">
       <c r="A29" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" s="7">
         <v>0.21</v>
@@ -7028,9 +7157,9 @@
       <c r="U29" s="8"/>
       <c r="V29" s="9"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22">
       <c r="A30" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B30" s="7">
         <v>0.60299999999999998</v>
@@ -7078,9 +7207,9 @@
       <c r="U30" s="8"/>
       <c r="V30" s="9"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22">
       <c r="A31" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B31" s="7">
         <v>0.26519999999999999</v>
@@ -7122,9 +7251,9 @@
       <c r="U31" s="8"/>
       <c r="V31" s="9"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22">
       <c r="A32" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="7">
         <v>0.1608</v>
@@ -7166,9 +7295,9 @@
       <c r="U32" s="8"/>
       <c r="V32" s="9"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22">
       <c r="A33" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="7">
         <v>0.30349999999999999</v>
@@ -7216,9 +7345,9 @@
       <c r="U33" s="8"/>
       <c r="V33" s="9"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22">
       <c r="A34" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" s="7">
         <v>0.63</v>
@@ -7266,7 +7395,7 @@
       <c r="U34" s="8"/>
       <c r="V34" s="9"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22">
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
@@ -7291,24 +7420,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7318,9 +7447,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7330,9 +7459,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7342,9 +7471,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7354,9 +7483,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7366,9 +7495,9 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7378,9 +7507,9 @@
   <conditionalFormatting sqref="V3:V35">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7390,9 +7519,9 @@
   <conditionalFormatting sqref="D3:D35">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7402,9 +7531,9 @@
   <conditionalFormatting sqref="G3:G35">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7414,9 +7543,9 @@
   <conditionalFormatting sqref="J3:J35">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7426,9 +7555,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7438,9 +7567,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7450,9 +7579,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7462,9 +7591,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7474,9 +7603,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7486,9 +7615,9 @@
   <conditionalFormatting sqref="M4:M21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7498,9 +7627,9 @@
   <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7510,9 +7639,9 @@
   <conditionalFormatting sqref="S4:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7522,9 +7651,9 @@
   <conditionalFormatting sqref="M3:M35">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7534,9 +7663,9 @@
   <conditionalFormatting sqref="P3:P35">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7546,9 +7675,9 @@
   <conditionalFormatting sqref="S3:S35">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7561,14 +7690,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -7585,71 +7714,71 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="33" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="G1" s="33"/>
+      <c r="H1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="33" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="33" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="32"/>
+      <c r="M1" s="33"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="F2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="27" t="s">
+      <c r="H2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="J2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" s="27" t="s">
+      <c r="L2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
         <v>46</v>
       </c>
@@ -7697,7 +7826,7 @@
         <v>1.0845751025000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -7745,9 +7874,9 @@
         <v>1.3607243325</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="7">
         <v>0.73160000000000003</v>
@@ -7793,9 +7922,9 @@
         <v>1.1540821750000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="7">
         <v>0.71699999999999997</v>
@@ -7841,25 +7970,25 @@
         <v>1.4101859700000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="35">
+        <v>96</v>
+      </c>
+      <c r="B7" s="31">
         <v>0.76639999999999997</v>
       </c>
       <c r="C7">
         <f>0.9145*0.9145</f>
         <v>0.83631024999999992</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="31">
         <v>0.74380000000000002</v>
       </c>
       <c r="E7">
         <f>1.004*1.004</f>
         <v>1.008016</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="31">
         <v>0.8518</v>
       </c>
       <c r="G7">
@@ -7869,16 +7998,23 @@
       <c r="L7" s="7"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
-        <v>48</v>
+        <v>98</v>
+      </c>
+      <c r="B8" s="31">
+        <v>0.7651</v>
+      </c>
+      <c r="C8">
+        <f>0.934*0.934</f>
+        <v>0.87235600000000013</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="28">
         <v>0.76449999999999996</v>
@@ -7917,9 +8053,9 @@
         <v>0.942025</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>0.75980000000000003</v>
@@ -7960,9 +8096,9 @@
         <v>0.93589999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="30">
         <v>0.76670000000000005</v>
@@ -7991,9 +8127,9 @@
         <v>0.73710000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="30">
         <v>0.75880000000000003</v>
@@ -8022,16 +8158,16 @@
         <v>0.73635000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -8046,9 +8182,9 @@
   <conditionalFormatting sqref="M3:M12">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8058,9 +8194,9 @@
   <conditionalFormatting sqref="L3:L12">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8070,9 +8206,9 @@
   <conditionalFormatting sqref="B3:B6 B9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8082,9 +8218,9 @@
   <conditionalFormatting sqref="D3:D6 D9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8094,9 +8230,9 @@
   <conditionalFormatting sqref="F3:F6 F9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8106,9 +8242,9 @@
   <conditionalFormatting sqref="H3:H7 H9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8118,9 +8254,9 @@
   <conditionalFormatting sqref="J3:J7 J9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8130,9 +8266,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8142,9 +8278,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8154,9 +8290,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8166,9 +8302,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8178,9 +8314,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8190,9 +8326,9 @@
   <conditionalFormatting sqref="B3:B12">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8202,9 +8338,9 @@
   <conditionalFormatting sqref="C3:C12">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8214,9 +8350,9 @@
   <conditionalFormatting sqref="D3:D11">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8226,9 +8362,9 @@
   <conditionalFormatting sqref="E3:E11">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8238,9 +8374,9 @@
   <conditionalFormatting sqref="F3:F12">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8250,9 +8386,9 @@
   <conditionalFormatting sqref="G3:G12">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8262,9 +8398,9 @@
   <conditionalFormatting sqref="H3:H11">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8274,9 +8410,9 @@
   <conditionalFormatting sqref="I3:I11">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8286,9 +8422,9 @@
   <conditionalFormatting sqref="J3:J12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8298,9 +8434,9 @@
   <conditionalFormatting sqref="K3:K12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8313,14 +8449,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="31" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -8329,74 +8465,74 @@
     <col min="38" max="40" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="1:40">
+      <c r="B1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="33" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="33" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="33" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="33" t="s">
+      <c r="R1" s="32"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" s="32"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="31"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="33" t="s">
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="33"/>
+      <c r="AF1" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG1" s="32"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="32"/>
-      <c r="AI1" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="32"/>
-      <c r="AL1" s="31" t="s">
+      <c r="AJ1" s="32"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="32"/>
+      <c r="AM1" s="32"/>
+      <c r="AN1" s="33"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -8518,9 +8654,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40">
       <c r="A3" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="10">
         <v>0.38469999999999999</v>
@@ -8631,21 +8767,21 @@
         <v>0.63719999999999999</v>
       </c>
       <c r="AL3" s="17">
-        <f>AVERAGE(B3,E3,H3,N3,Q3,T3,W3,Z3,AC3,AF3,AI3)</f>
+        <f t="shared" ref="AL3:AN4" si="0">AVERAGE(B3,E3,H3,N3,Q3,T3,W3,Z3,AC3,AF3,AI3)</f>
         <v>0.4328727272727273</v>
       </c>
       <c r="AM3" s="18">
-        <f>AVERAGE(C3,F3,I3,O3,R3,U3,X3,AA3,AD3,AG3,AJ3)</f>
+        <f t="shared" si="0"/>
         <v>0.52852727272727273</v>
       </c>
       <c r="AN3" s="19">
-        <f>AVERAGE(D3,G3,J3,P3,S3,V3,Y3,AB3,AE3,AH3,AK3)</f>
+        <f t="shared" si="0"/>
         <v>0.45634545454545455</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40">
       <c r="A4" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="10">
         <v>0.56200000000000006</v>
@@ -8756,21 +8892,21 @@
         <v>0.59219999999999995</v>
       </c>
       <c r="AL4" s="10">
-        <f>AVERAGE(B4,E4,H4,N4,Q4,T4,W4,Z4,AC4,AF4,AI4)</f>
+        <f t="shared" si="0"/>
         <v>0.59123636363636367</v>
       </c>
       <c r="AM4" s="11">
-        <f>AVERAGE(C4,F4,I4,O4,R4,U4,X4,AA4,AD4,AG4,AJ4)</f>
+        <f t="shared" si="0"/>
         <v>0.47882727272727271</v>
       </c>
       <c r="AN4" s="12">
-        <f>AVERAGE(D4,G4,J4,P4,S4,V4,Y4,AB4,AE4,AH4,AK4)</f>
+        <f t="shared" si="0"/>
         <v>0.49341818181818181</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40">
       <c r="A5" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="10">
         <v>0.27739999999999998</v>
@@ -8881,21 +9017,21 @@
         <v>0.65649999999999997</v>
       </c>
       <c r="AL5" s="10">
-        <f t="shared" ref="AL5:AL9" si="0">AVERAGE(B5,E5,H5,N5,Q5,T5,W5,Z5,AC5,AF5,AI5)</f>
+        <f t="shared" ref="AL5:AL6" si="1">AVERAGE(B5,E5,H5,N5,Q5,T5,W5,Z5,AC5,AF5,AI5)</f>
         <v>0.37953636363636362</v>
       </c>
       <c r="AM5" s="11">
-        <f t="shared" ref="AM5:AM9" si="1">AVERAGE(C5,F5,I5,O5,R5,U5,X5,AA5,AD5,AG5,AJ5)</f>
+        <f t="shared" ref="AM5:AM6" si="2">AVERAGE(C5,F5,I5,O5,R5,U5,X5,AA5,AD5,AG5,AJ5)</f>
         <v>0.59595454545454551</v>
       </c>
       <c r="AN5" s="12">
-        <f t="shared" ref="AN5:AN9" si="2">AVERAGE(D5,G5,J5,P5,S5,V5,Y5,AB5,AE5,AH5,AK5)</f>
+        <f t="shared" ref="AN5:AN6" si="3">AVERAGE(D5,G5,J5,P5,S5,V5,Y5,AB5,AE5,AH5,AK5)</f>
         <v>0.4236454545454546</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="10">
         <v>0.3236</v>
@@ -9006,19 +9142,19 @@
         <v>0.66720000000000002</v>
       </c>
       <c r="AL6" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.54188181818181813</v>
       </c>
       <c r="AM6" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.51207272727272724</v>
       </c>
       <c r="AN6" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.51095454545454555</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40">
       <c r="A7" s="5"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -9060,7 +9196,7 @@
       <c r="AM7" s="11"/>
       <c r="AN7" s="12"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40">
       <c r="A8" s="5"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -9102,7 +9238,7 @@
       <c r="AM8" s="11"/>
       <c r="AN8" s="12"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40">
       <c r="A9" s="5"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -9163,9 +9299,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9175,9 +9311,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9187,9 +9323,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9199,9 +9335,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9211,9 +9347,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9223,9 +9359,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9235,9 +9371,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9247,9 +9383,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9259,9 +9395,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9271,9 +9407,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9283,9 +9419,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9295,9 +9431,9 @@
   <conditionalFormatting sqref="AN3:AN9">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9307,9 +9443,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9319,9 +9455,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9331,9 +9467,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9343,9 +9479,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9355,9 +9491,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9367,9 +9503,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9379,9 +9515,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9391,9 +9527,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9403,9 +9539,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9415,9 +9551,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9427,9 +9563,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9439,9 +9575,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9451,9 +9587,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9463,9 +9599,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9475,9 +9611,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9487,9 +9623,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9499,9 +9635,9 @@
   <conditionalFormatting sqref="AE4:AE9">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9511,9 +9647,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9523,9 +9659,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9535,9 +9671,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9547,9 +9683,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9559,9 +9695,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9571,9 +9707,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9583,9 +9719,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9595,9 +9731,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9607,9 +9743,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9619,9 +9755,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="25">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9631,9 +9767,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9643,9 +9779,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9655,9 +9791,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9667,9 +9803,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9679,9 +9815,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9691,9 +9827,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9703,9 +9839,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9715,9 +9851,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9727,9 +9863,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9739,9 +9875,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9751,9 +9887,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9763,9 +9899,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9775,9 +9911,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9787,9 +9923,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9799,9 +9935,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9811,9 +9947,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9823,9 +9959,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9835,9 +9971,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9847,9 +9983,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9859,9 +9995,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9871,9 +10007,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9883,9 +10019,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9895,9 +10031,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9907,9 +10043,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>

<commit_message>
Starting point for new results. Good snapshot for going back.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="BP4D_int_seg" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="102">
   <si>
     <t>DEVEL</t>
   </si>
@@ -315,6 +316,15 @@
   <si>
     <t>Combined SVM</t>
   </si>
+  <si>
+    <t>Best actual (v2)</t>
+  </si>
+  <si>
+    <t>Results submitted v2</t>
+  </si>
+  <si>
+    <t>Submitted</t>
+  </si>
 </sst>
 </file>
 
@@ -463,7 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -506,6 +516,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -820,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -831,66 +847,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="34" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="34" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="34" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="34" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="34" t="s">
+      <c r="R1" s="34"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="34" t="s">
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="34" t="s">
+      <c r="X1" s="34"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="34" t="s">
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="32" t="s">
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="32" t="s">
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="33"/>
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="35"/>
     </row>
     <row r="2" spans="1:37">
       <c r="A2" t="s">
@@ -2008,18 +2024,9 @@
       <c r="AF12" s="8"/>
       <c r="AG12" s="8"/>
       <c r="AH12" s="9"/>
-      <c r="AI12" s="10">
-        <f t="shared" si="3"/>
-        <v>0.43243333333333328</v>
-      </c>
-      <c r="AJ12" s="11">
-        <f t="shared" si="4"/>
-        <v>0.85666666666666658</v>
-      </c>
-      <c r="AK12" s="12">
-        <f t="shared" si="5"/>
-        <v>0.54469999999999996</v>
-      </c>
+      <c r="AI12" s="10"/>
+      <c r="AJ12" s="11"/>
+      <c r="AK12" s="12"/>
     </row>
     <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
@@ -2076,18 +2083,9 @@
       <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
       <c r="AH13" s="9"/>
-      <c r="AI13" s="10">
-        <f t="shared" si="3"/>
-        <v>0.57389999999999997</v>
-      </c>
-      <c r="AJ13" s="11">
-        <f t="shared" si="4"/>
-        <v>0.15646666666666667</v>
-      </c>
-      <c r="AK13" s="12">
-        <f t="shared" si="5"/>
-        <v>0.23713333333333333</v>
-      </c>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="11"/>
+      <c r="AK13" s="12"/>
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
@@ -2144,18 +2142,9 @@
       <c r="AF14" s="8"/>
       <c r="AG14" s="8"/>
       <c r="AH14" s="9"/>
-      <c r="AI14" s="10">
-        <f t="shared" si="3"/>
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="AJ14" s="11">
-        <f t="shared" si="4"/>
-        <v>0.83816666666666662</v>
-      </c>
-      <c r="AK14" s="12">
-        <f t="shared" si="5"/>
-        <v>0.53643333333333332</v>
-      </c>
+      <c r="AI14" s="10"/>
+      <c r="AJ14" s="11"/>
+      <c r="AK14" s="12"/>
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
@@ -2212,18 +2201,9 @@
       <c r="AF15" s="8"/>
       <c r="AG15" s="8"/>
       <c r="AH15" s="9"/>
-      <c r="AI15" s="10">
-        <f t="shared" si="3"/>
-        <v>0.57640000000000002</v>
-      </c>
-      <c r="AJ15" s="11">
-        <f t="shared" si="4"/>
-        <v>0.16486666666666666</v>
-      </c>
-      <c r="AK15" s="12">
-        <f t="shared" si="5"/>
-        <v>0.24983333333333335</v>
-      </c>
+      <c r="AI15" s="10"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="12"/>
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
@@ -2304,18 +2284,9 @@
       <c r="AF16" s="8"/>
       <c r="AG16" s="8"/>
       <c r="AH16" s="9"/>
-      <c r="AI16" s="10">
-        <f t="shared" si="3"/>
-        <v>0.49852857142857143</v>
-      </c>
-      <c r="AJ16" s="11">
-        <f t="shared" si="4"/>
-        <v>0.65727142857142862</v>
-      </c>
-      <c r="AK16" s="12">
-        <f t="shared" si="5"/>
-        <v>0.56054285714285712</v>
-      </c>
+      <c r="AI16" s="10"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="12"/>
     </row>
     <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
@@ -2396,18 +2367,9 @@
       <c r="AF17" s="8"/>
       <c r="AG17" s="8"/>
       <c r="AH17" s="9"/>
-      <c r="AI17" s="10">
-        <f t="shared" si="3"/>
-        <v>0.51452857142857134</v>
-      </c>
-      <c r="AJ17" s="11">
-        <f t="shared" si="4"/>
-        <v>0.59250000000000003</v>
-      </c>
-      <c r="AK17" s="12">
-        <f t="shared" si="5"/>
-        <v>0.54634285714285713</v>
-      </c>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="11"/>
+      <c r="AK17" s="12"/>
     </row>
     <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
@@ -2476,18 +2438,9 @@
       <c r="AF18" s="8"/>
       <c r="AG18" s="8"/>
       <c r="AH18" s="9"/>
-      <c r="AI18" s="10">
-        <f t="shared" si="3"/>
-        <v>0.70147999999999999</v>
-      </c>
-      <c r="AJ18" s="11">
-        <f t="shared" si="4"/>
-        <v>0.81576000000000004</v>
-      </c>
-      <c r="AK18" s="12">
-        <f t="shared" si="5"/>
-        <v>0.74680000000000002</v>
-      </c>
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="11"/>
+      <c r="AK18" s="12"/>
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
@@ -2556,18 +2509,9 @@
       <c r="AF19" s="8"/>
       <c r="AG19" s="8"/>
       <c r="AH19" s="9"/>
-      <c r="AI19" s="10">
-        <f t="shared" si="3"/>
-        <v>0.61221999999999999</v>
-      </c>
-      <c r="AJ19" s="11">
-        <f t="shared" si="4"/>
-        <v>0.87799999999999989</v>
-      </c>
-      <c r="AK19" s="12">
-        <f t="shared" si="5"/>
-        <v>0.71243999999999996</v>
-      </c>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="12"/>
     </row>
     <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
@@ -3692,18 +3636,9 @@
       <c r="AF29" s="7"/>
       <c r="AG29" s="8"/>
       <c r="AH29" s="9"/>
-      <c r="AI29" s="10">
-        <f t="shared" si="3"/>
-        <v>0.5716</v>
-      </c>
-      <c r="AJ29" s="11">
-        <f t="shared" si="4"/>
-        <v>0.60124285714285719</v>
-      </c>
-      <c r="AK29" s="12">
-        <f t="shared" si="5"/>
-        <v>0.57781428571428584</v>
-      </c>
+      <c r="AI29" s="10"/>
+      <c r="AJ29" s="11"/>
+      <c r="AK29" s="12"/>
     </row>
     <row r="30" spans="1:37">
       <c r="A30" s="25" t="s">
@@ -3900,18 +3835,9 @@
       <c r="AF31" s="7"/>
       <c r="AG31" s="8"/>
       <c r="AH31" s="9"/>
-      <c r="AI31" s="10">
-        <f t="shared" si="3"/>
-        <v>0.57911428571428569</v>
-      </c>
-      <c r="AJ31" s="11">
-        <f t="shared" si="4"/>
-        <v>0.59078571428571425</v>
-      </c>
-      <c r="AK31" s="12">
-        <f t="shared" si="5"/>
-        <v>0.57524285714285717</v>
-      </c>
+      <c r="AI31" s="10"/>
+      <c r="AJ31" s="11"/>
+      <c r="AK31" s="12"/>
     </row>
     <row r="32" spans="1:37">
       <c r="A32" s="25" t="s">
@@ -4108,56 +4034,125 @@
       <c r="AF33" s="7"/>
       <c r="AG33" s="8"/>
       <c r="AH33" s="9"/>
-      <c r="AI33" s="10">
-        <f t="shared" ref="AI33" si="9">AVERAGE(B33,E33,H33,K33,N33,Q33,T33,W33,Z33,AC33,AF33)</f>
-        <v>0.48159999999999997</v>
-      </c>
-      <c r="AJ33" s="11">
-        <f t="shared" ref="AJ33" si="10">AVERAGE(C33,F33,I33,L33,O33,R33,U33,X33,AA33,AD33,AG33)</f>
-        <v>0.66241428571428584</v>
-      </c>
-      <c r="AK33" s="12">
-        <f t="shared" ref="AK33" si="11">AVERAGE(D33,G33,J33,M33,P33,S33,V33,Y33,AB33,AE33,AH33)</f>
-        <v>0.55455714285714286</v>
-      </c>
+      <c r="AI33" s="10"/>
+      <c r="AJ33" s="11"/>
+      <c r="AK33" s="12"/>
     </row>
     <row r="34" spans="1:37">
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="7"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="7"/>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="8"/>
-      <c r="AC34" s="7"/>
-      <c r="AD34" s="8"/>
-      <c r="AE34" s="8"/>
-      <c r="AF34" s="7"/>
-      <c r="AG34" s="8"/>
-      <c r="AH34" s="9"/>
-      <c r="AI34" s="10"/>
-      <c r="AJ34" s="11"/>
-      <c r="AK34" s="12"/>
+      <c r="A34" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" s="7">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="C34" s="8">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="F34" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="I34" s="8">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="K34" s="7">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="L34" s="8">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="M34" s="8">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="N34" s="7">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="O34" s="8">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="P34" s="8">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="R34" s="8">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="S34" s="8">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="T34" s="7">
+        <v>0.83699999999999997</v>
+      </c>
+      <c r="U34" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="V34" s="8">
+        <v>0.872</v>
+      </c>
+      <c r="W34" s="7">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="X34" s="8">
+        <v>0.876</v>
+      </c>
+      <c r="Y34" s="8">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="Z34" s="7">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="AA34" s="8">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="AB34" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="AC34" s="7">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="AD34" s="8">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="AE34" s="8">
+        <v>0.622</v>
+      </c>
+      <c r="AF34" s="7">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="AG34" s="8">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="AH34" s="9">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="AI34" s="10">
+        <f t="shared" ref="AI34" si="9">AVERAGE(B34,E34,H34,K34,N34,Q34,T34,W34,Z34,AC34,AF34)</f>
+        <v>0.51727272727272733</v>
+      </c>
+      <c r="AJ34" s="11">
+        <f t="shared" ref="AJ34" si="10">AVERAGE(C34,F34,I34,L34,O34,R34,U34,X34,AA34,AD34,AG34)</f>
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="AK34" s="12">
+        <f t="shared" ref="AK34" si="11">AVERAGE(D34,G34,J34,M34,P34,S34,V34,Y34,AB34,AE34,AH34)</f>
+        <v>0.60236363636363643</v>
+      </c>
     </row>
     <row r="35" spans="1:37">
       <c r="B35" s="7"/>
@@ -5287,8 +5282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AH35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5313,53 +5308,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="34" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="34" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="34" t="s">
+      <c r="R1" s="34"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35"/>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
     </row>
     <row r="2" spans="1:34">
       <c r="A2" t="s">
@@ -7153,9 +7148,18 @@
       <c r="Q29" s="7"/>
       <c r="R29" s="8"/>
       <c r="S29" s="9"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="9"/>
+      <c r="T29" s="7">
+        <f t="shared" ref="T29:T35" si="4">AVERAGE(B29,E29,H29,K29,N29,Q29)</f>
+        <v>0.2475</v>
+      </c>
+      <c r="U29" s="8">
+        <f t="shared" ref="U29:U35" si="5">AVERAGE(C29,F29,I29,L29,O29,R29)</f>
+        <v>0.76</v>
+      </c>
+      <c r="V29" s="9">
+        <f t="shared" ref="V29:V35" si="6">AVERAGE(D29,G29,J29,M29,P29,S29)</f>
+        <v>0.36</v>
+      </c>
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="25" t="s">
@@ -7203,9 +7207,18 @@
       <c r="Q30" s="7"/>
       <c r="R30" s="8"/>
       <c r="S30" s="9"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="9"/>
+      <c r="T30" s="7">
+        <f t="shared" si="4"/>
+        <v>0.44499999999999995</v>
+      </c>
+      <c r="U30" s="8">
+        <f t="shared" si="5"/>
+        <v>0.44249999999999995</v>
+      </c>
+      <c r="V30" s="9">
+        <f t="shared" si="6"/>
+        <v>0.35099999999999998</v>
+      </c>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="25" t="s">
@@ -7247,9 +7260,18 @@
       <c r="Q31" s="7"/>
       <c r="R31" s="8"/>
       <c r="S31" s="9"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="9"/>
+      <c r="T31" s="7">
+        <f t="shared" si="4"/>
+        <v>0.2208333333333333</v>
+      </c>
+      <c r="U31" s="8">
+        <f t="shared" si="5"/>
+        <v>0.76846666666666674</v>
+      </c>
+      <c r="V31" s="9">
+        <f t="shared" si="6"/>
+        <v>0.31570000000000004</v>
+      </c>
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="25" t="s">
@@ -7291,9 +7313,18 @@
       <c r="Q32" s="7"/>
       <c r="R32" s="8"/>
       <c r="S32" s="9"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="9"/>
+      <c r="T32" s="7">
+        <f t="shared" si="4"/>
+        <v>0.18646666666666667</v>
+      </c>
+      <c r="U32" s="8">
+        <f t="shared" si="5"/>
+        <v>0.92316666666666658</v>
+      </c>
+      <c r="V32" s="9">
+        <f t="shared" si="6"/>
+        <v>0.29619999999999996</v>
+      </c>
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="25" t="s">
@@ -7341,9 +7372,18 @@
       <c r="Q33" s="7"/>
       <c r="R33" s="8"/>
       <c r="S33" s="9"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="9"/>
+      <c r="T33" s="7">
+        <f t="shared" si="4"/>
+        <v>0.35575000000000001</v>
+      </c>
+      <c r="U33" s="8">
+        <f t="shared" si="5"/>
+        <v>0.55970000000000009</v>
+      </c>
+      <c r="V33" s="9">
+        <f t="shared" si="6"/>
+        <v>0.42807499999999998</v>
+      </c>
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="25" t="s">
@@ -7391,46 +7431,103 @@
       <c r="Q34" s="7"/>
       <c r="R34" s="8"/>
       <c r="S34" s="9"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="8"/>
-      <c r="V34" s="9"/>
+      <c r="T34" s="7">
+        <f t="shared" si="4"/>
+        <v>0.38384999999999997</v>
+      </c>
+      <c r="U34" s="8">
+        <f t="shared" si="5"/>
+        <v>0.48897499999999994</v>
+      </c>
+      <c r="V34" s="9">
+        <f t="shared" si="6"/>
+        <v>0.41767499999999996</v>
+      </c>
     </row>
     <row r="35" spans="1:22">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="9"/>
+      <c r="A35" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="L35" s="8">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0.43</v>
+      </c>
+      <c r="N35" s="7">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="O35" s="8">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="P35" s="9">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>0.32</v>
+      </c>
+      <c r="R35" s="8">
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="S35" s="9">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="T35" s="7">
+        <f t="shared" si="4"/>
+        <v>0.47583333333333333</v>
+      </c>
+      <c r="U35" s="8">
+        <f t="shared" si="5"/>
+        <v>0.45366666666666666</v>
+      </c>
+      <c r="V35" s="9">
+        <f t="shared" si="6"/>
+        <v>0.43949999999999995</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
@@ -7693,8 +7790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7715,30 +7812,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="34" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34" t="s">
+      <c r="K1" s="35"/>
+      <c r="L1" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="33"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
@@ -8063,12 +8160,6 @@
       <c r="C10">
         <v>0.82220000000000004</v>
       </c>
-      <c r="D10">
-        <v>0.75629999999999997</v>
-      </c>
-      <c r="E10">
-        <v>0.94450000000000001</v>
-      </c>
       <c r="F10">
         <v>0.86309999999999998</v>
       </c>
@@ -8089,11 +8180,11 @@
       </c>
       <c r="L10" s="7">
         <f t="shared" ref="L10:M12" si="1">AVERAGE(D10,F10,H10,J10)</f>
-        <v>0.65042500000000003</v>
+        <v>0.61513333333333342</v>
       </c>
       <c r="M10" s="9">
         <f t="shared" si="1"/>
-        <v>0.93589999999999995</v>
+        <v>0.93303333333333338</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -8159,7 +8250,47 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="1"/>
+      <c r="A13" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="30">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="G13" s="30">
+        <v>0.84</v>
+      </c>
+      <c r="H13">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="I13">
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="J13">
+        <v>0.503</v>
+      </c>
+      <c r="K13">
+        <v>1.2629999999999999</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" ref="L13" si="2">AVERAGE(D13,F13,H13,J13)</f>
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" ref="M13" si="3">AVERAGE(E13,G13,I13,K13)</f>
+        <v>1.1484999999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1"/>
@@ -8179,7 +8310,7 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="M3:M12">
+  <conditionalFormatting sqref="M3:M13">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8191,7 +8322,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L12">
+  <conditionalFormatting sqref="L3:L13">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8323,7 +8454,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B12">
+  <conditionalFormatting sqref="B3:B13">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8335,7 +8466,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C12">
+  <conditionalFormatting sqref="C3:C13">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8347,7 +8478,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D11">
+  <conditionalFormatting sqref="D3:D13">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8359,7 +8490,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E11">
+  <conditionalFormatting sqref="E3:E13">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8371,7 +8502,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F12">
+  <conditionalFormatting sqref="F3:F13">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8383,7 +8514,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G12">
+  <conditionalFormatting sqref="G3:G13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8395,7 +8526,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H11">
+  <conditionalFormatting sqref="H3:H13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8407,7 +8538,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I11">
+  <conditionalFormatting sqref="I3:I13">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8419,7 +8550,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J12">
+  <conditionalFormatting sqref="J3:J13">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8431,7 +8562,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K12">
+  <conditionalFormatting sqref="K3:K13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -8449,6 +8580,305 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="34"/>
+      <c r="F1" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="35"/>
+      <c r="J1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="35"/>
+      <c r="L1" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="30">
+        <v>0.65</v>
+      </c>
+      <c r="C3">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="D3">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="E3">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="G3" s="30">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="H3">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="K3">
+        <v>1.1080000000000001</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:M3" si="0">AVERAGE(D3,F3,H3,J3)</f>
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="M3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.65325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN9"/>
   <sheetViews>
@@ -8466,71 +8896,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="34" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="34" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="34" t="s">
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="34" t="s">
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="32"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="34" t="s">
+      <c r="R1" s="34"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="34" t="s">
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="34" t="s">
+      <c r="X1" s="34"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="34" t="s">
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="34" t="s">
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="AG1" s="32"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="32" t="s">
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="AJ1" s="32"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="32" t="s">
+      <c r="AJ1" s="34"/>
+      <c r="AK1" s="35"/>
+      <c r="AL1" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="32"/>
-      <c r="AN1" s="33"/>
+      <c r="AM1" s="34"/>
+      <c r="AN1" s="35"/>
     </row>
     <row r="2" spans="1:40">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Initial geometry experiment results.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="BP4D_int_seg" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="125725" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="106">
   <si>
     <t>DEVEL</t>
   </si>
@@ -325,12 +325,24 @@
   <si>
     <t>Submitted</t>
   </si>
+  <si>
+    <t>Pure geom static (params)</t>
+  </si>
+  <si>
+    <t>Pure geom dynamic (params)</t>
+  </si>
+  <si>
+    <t>Pure geom dyn (actual locs)</t>
+  </si>
+  <si>
+    <t>Pure geom stat (actual locs)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +636,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -658,6 +671,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -833,20 +847,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
@@ -908,7 +922,7 @@
       <c r="AJ1" s="34"/>
       <c r="AK1" s="35"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -1137,7 +1151,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1229,7 +1243,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1321,7 +1335,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1427,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1505,7 +1519,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1621,7 +1635,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1737,7 +1751,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1841,7 +1855,7 @@
         <v>0.44040000000000001</v>
       </c>
       <c r="AI10" s="10">
-        <f t="shared" ref="AI10:AI31" si="3">AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10,AF10)</f>
+        <f t="shared" ref="AI10:AI30" si="3">AVERAGE(B10,E10,H10,K10,N10,Q10,T10,W10,Z10,AC10,AF10)</f>
         <v>0.5429272727272727</v>
       </c>
       <c r="AJ10" s="11">
@@ -1853,7 +1867,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -1961,15 +1975,15 @@
         <v>0.5331999999999999</v>
       </c>
       <c r="AJ11" s="11">
-        <f t="shared" ref="AJ11:AJ31" si="4">AVERAGE(C11,F11,I11,L11,O11,R11,U11,X11,AA11,AD11,AG11)</f>
+        <f t="shared" ref="AJ11:AJ30" si="4">AVERAGE(C11,F11,I11,L11,O11,R11,U11,X11,AA11,AD11,AG11)</f>
         <v>0.69535454545454545</v>
       </c>
       <c r="AK11" s="12">
-        <f t="shared" ref="AK11:AK31" si="5">AVERAGE(D11,G11,J11,M11,P11,S11,V11,Y11,AB11,AE11,AH11)</f>
+        <f t="shared" ref="AK11:AK30" si="5">AVERAGE(D11,G11,J11,M11,P11,S11,V11,Y11,AB11,AE11,AH11)</f>
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2028,7 +2042,7 @@
       <c r="AJ12" s="11"/>
       <c r="AK12" s="12"/>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2087,7 +2101,7 @@
       <c r="AJ13" s="11"/>
       <c r="AK13" s="12"/>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -2146,7 +2160,7 @@
       <c r="AJ14" s="11"/>
       <c r="AK14" s="12"/>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -2205,7 +2219,7 @@
       <c r="AJ15" s="11"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2288,7 +2302,7 @@
       <c r="AJ16" s="11"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
@@ -2371,7 +2385,7 @@
       <c r="AJ17" s="11"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>46</v>
       </c>
@@ -2442,7 +2456,7 @@
       <c r="AJ18" s="11"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>47</v>
       </c>
@@ -2513,7 +2527,7 @@
       <c r="AJ19" s="11"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>52</v>
       </c>
@@ -2629,7 +2643,7 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>53</v>
       </c>
@@ -2745,7 +2759,7 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>54</v>
       </c>
@@ -2861,7 +2875,7 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>55</v>
       </c>
@@ -2977,7 +2991,7 @@
         <v>0.59650909090909088</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>56</v>
       </c>
@@ -3093,7 +3107,7 @@
         <v>0.5917</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>60</v>
       </c>
@@ -3209,7 +3223,7 @@
         <v>0.61232727272727272</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>65</v>
       </c>
@@ -3325,7 +3339,7 @@
         <v>0.58963636363636374</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>67</v>
       </c>
@@ -3441,7 +3455,7 @@
         <v>0.57887272727272732</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>69</v>
       </c>
@@ -3557,7 +3571,7 @@
         <v>0.60222727272727272</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>70</v>
       </c>
@@ -3640,7 +3654,7 @@
       <c r="AJ29" s="11"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>76</v>
       </c>
@@ -3756,7 +3770,7 @@
         <v>0.60204545454545466</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>77</v>
       </c>
@@ -3839,7 +3853,7 @@
       <c r="AJ31" s="11"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>84</v>
       </c>
@@ -3955,7 +3969,7 @@
         <v>0.58684545454545445</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>97</v>
       </c>
@@ -4038,7 +4052,7 @@
       <c r="AJ33" s="11"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>100</v>
       </c>
@@ -4154,83 +4168,239 @@
         <v>0.60236363636363643</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="7"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="7"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="7"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="8"/>
-      <c r="AC35" s="7"/>
-      <c r="AD35" s="8"/>
-      <c r="AE35" s="8"/>
-      <c r="AF35" s="7"/>
-      <c r="AG35" s="8"/>
-      <c r="AH35" s="9"/>
-      <c r="AI35" s="10"/>
-      <c r="AJ35" s="11"/>
-      <c r="AK35" s="12"/>
-    </row>
-    <row r="36" spans="1:37">
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="7"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="7"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="7"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="8"/>
-      <c r="AC36" s="7"/>
-      <c r="AD36" s="8"/>
-      <c r="AE36" s="8"/>
-      <c r="AF36" s="7"/>
-      <c r="AG36" s="8"/>
-      <c r="AH36" s="9"/>
-      <c r="AI36" s="10"/>
-      <c r="AJ36" s="11"/>
-      <c r="AK36" s="12"/>
-    </row>
-    <row r="37" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0.2984</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.62509999999999999</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0.41710000000000003</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0.34279999999999999</v>
+      </c>
+      <c r="I35" s="8">
+        <v>0.60470000000000002</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.43759999999999999</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0.64439999999999997</v>
+      </c>
+      <c r="L35" s="8">
+        <v>0.87890000000000001</v>
+      </c>
+      <c r="M35" s="8">
+        <v>0.74360000000000004</v>
+      </c>
+      <c r="N35" s="7">
+        <v>0.626</v>
+      </c>
+      <c r="O35" s="8">
+        <v>0.9093</v>
+      </c>
+      <c r="P35" s="8">
+        <v>0.74150000000000005</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>0.73209999999999997</v>
+      </c>
+      <c r="R35" s="8">
+        <v>0.93830000000000002</v>
+      </c>
+      <c r="S35" s="8">
+        <v>0.82240000000000002</v>
+      </c>
+      <c r="T35" s="7">
+        <v>0.77769999999999995</v>
+      </c>
+      <c r="U35" s="8">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="V35" s="8">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="W35" s="7">
+        <v>0.42549999999999999</v>
+      </c>
+      <c r="X35" s="8">
+        <v>0.97829999999999995</v>
+      </c>
+      <c r="Y35" s="8">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="Z35" s="7">
+        <v>0.18729999999999999</v>
+      </c>
+      <c r="AA35" s="8">
+        <v>0.31219999999999998</v>
+      </c>
+      <c r="AB35" s="8">
+        <v>0.2341</v>
+      </c>
+      <c r="AC35" s="7">
+        <v>0.43980000000000002</v>
+      </c>
+      <c r="AD35" s="8">
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="AE35" s="8">
+        <v>0.58409999999999995</v>
+      </c>
+      <c r="AF35" s="7">
+        <v>0.21</v>
+      </c>
+      <c r="AG35" s="8">
+        <v>0.54320000000000002</v>
+      </c>
+      <c r="AH35" s="9">
+        <v>0.3029</v>
+      </c>
+      <c r="AI35" s="10">
+        <f t="shared" ref="AI35" si="12">AVERAGE(B35,E35,H35,K35,N35,Q35,T35,W35,Z35,AC35,AF35)</f>
+        <v>0.45699090909090906</v>
+      </c>
+      <c r="AJ35" s="11">
+        <f t="shared" ref="AJ35" si="13">AVERAGE(C35,F35,I35,L35,O35,R35,U35,X35,AA35,AD35,AG35)</f>
+        <v>0.73686363636363628</v>
+      </c>
+      <c r="AK35" s="12">
+        <f t="shared" ref="AK35" si="14">AVERAGE(D35,G35,J35,M35,P35,S35,V35,Y35,AB35,AE35,AH35)</f>
+        <v>0.55642727272727277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.4365</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.4909</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.2079</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.59860000000000002</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0.30859999999999999</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0.32229999999999998</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0.63160000000000005</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.42680000000000001</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0.6855</v>
+      </c>
+      <c r="L36" s="8">
+        <v>0.80630000000000002</v>
+      </c>
+      <c r="M36" s="8">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="N36" s="7">
+        <v>0.68479999999999996</v>
+      </c>
+      <c r="O36" s="8">
+        <v>0.88519999999999999</v>
+      </c>
+      <c r="P36" s="8">
+        <v>0.7722</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0.74670000000000003</v>
+      </c>
+      <c r="R36" s="8">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="S36" s="8">
+        <v>0.81489999999999996</v>
+      </c>
+      <c r="T36" s="7">
+        <v>0.755</v>
+      </c>
+      <c r="U36" s="8">
+        <v>0.88970000000000005</v>
+      </c>
+      <c r="V36" s="8">
+        <v>0.81689999999999996</v>
+      </c>
+      <c r="W36" s="7">
+        <v>0.43769999999999998</v>
+      </c>
+      <c r="X36" s="8">
+        <v>0.92069999999999996</v>
+      </c>
+      <c r="Y36" s="8">
+        <v>0.59330000000000005</v>
+      </c>
+      <c r="Z36" s="7">
+        <v>0.1623</v>
+      </c>
+      <c r="AA36" s="8">
+        <v>0.29049999999999998</v>
+      </c>
+      <c r="AB36" s="8">
+        <v>0.20830000000000001</v>
+      </c>
+      <c r="AC36" s="7">
+        <v>0.48010000000000003</v>
+      </c>
+      <c r="AD36" s="8">
+        <v>0.74350000000000005</v>
+      </c>
+      <c r="AE36" s="8">
+        <v>0.58350000000000002</v>
+      </c>
+      <c r="AF36" s="7">
+        <v>0.20960000000000001</v>
+      </c>
+      <c r="AG36" s="8">
+        <v>0.57750000000000001</v>
+      </c>
+      <c r="AH36" s="9">
+        <v>0.30759999999999998</v>
+      </c>
+      <c r="AI36" s="10">
+        <f t="shared" ref="AI36" si="15">AVERAGE(B36,E36,H36,K36,N36,Q36,T36,W36,Z36,AC36,AF36)</f>
+        <v>0.46621818181818181</v>
+      </c>
+      <c r="AJ36" s="11">
+        <f t="shared" ref="AJ36" si="16">AVERAGE(C36,F36,I36,L36,O36,R36,U36,X36,AA36,AD36,AG36)</f>
+        <v>0.7092090909090909</v>
+      </c>
+      <c r="AK36" s="12">
+        <f t="shared" ref="AK36" si="17">AVERAGE(D36,G36,J36,M36,P36,S36,V36,Y36,AB36,AE36,AH36)</f>
+        <v>0.55127272727272725</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="9"/>
@@ -4268,7 +4438,7 @@
       <c r="AJ37" s="11"/>
       <c r="AK37" s="12"/>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
@@ -4306,7 +4476,7 @@
       <c r="AJ38" s="11"/>
       <c r="AK38" s="12"/>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B39" s="7"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
@@ -4344,7 +4514,7 @@
       <c r="AJ39" s="11"/>
       <c r="AK39" s="12"/>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
@@ -4400,9 +4570,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="76">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4412,9 +4582,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="75">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4424,9 +4594,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="74">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4436,9 +4606,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="73">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4448,9 +4618,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="72">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4460,9 +4630,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="71">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4472,9 +4642,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4484,9 +4654,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4496,9 +4666,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4508,9 +4678,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4520,9 +4690,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4532,9 +4702,9 @@
   <conditionalFormatting sqref="AK3:AK40">
     <cfRule type="colorScale" priority="65">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4544,9 +4714,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="64">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4556,9 +4726,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4568,9 +4738,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4580,9 +4750,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4592,9 +4762,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4604,9 +4774,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4616,9 +4786,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4628,9 +4798,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4640,9 +4810,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4652,9 +4822,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4664,9 +4834,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4676,9 +4846,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4688,9 +4858,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4700,9 +4870,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4712,9 +4882,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4724,9 +4894,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4736,9 +4906,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4748,9 +4918,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4760,9 +4930,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4772,9 +4942,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4784,9 +4954,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4796,9 +4966,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4808,9 +4978,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4820,9 +4990,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4832,9 +5002,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4844,9 +5014,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4856,9 +5026,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4868,9 +5038,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4880,9 +5050,9 @@
   <conditionalFormatting sqref="P3:P25 P27:P40">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4892,9 +5062,9 @@
   <conditionalFormatting sqref="J3:J25 X29:X40 J27:J40">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4904,9 +5074,9 @@
   <conditionalFormatting sqref="G3:G25 G27:G40">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4916,9 +5086,9 @@
   <conditionalFormatting sqref="D3:D25 D27:D40">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4928,9 +5098,9 @@
   <conditionalFormatting sqref="AH3:AH25 AH27:AH40">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4940,9 +5110,9 @@
   <conditionalFormatting sqref="AE3:AE25 AE27:AE40">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4952,9 +5122,9 @@
   <conditionalFormatting sqref="AB3:AB25 AB27:AB40">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4964,9 +5134,9 @@
   <conditionalFormatting sqref="Y3:Y25 Y27:Y40">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4976,9 +5146,9 @@
   <conditionalFormatting sqref="M3:M25 M27:M40">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -4988,9 +5158,9 @@
   <conditionalFormatting sqref="V3:V25 V27:V40">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5000,9 +5170,9 @@
   <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5012,9 +5182,9 @@
   <conditionalFormatting sqref="S26:S40">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5024,9 +5194,9 @@
   <conditionalFormatting sqref="P26:P40">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5036,9 +5206,9 @@
   <conditionalFormatting sqref="J26:J40">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5048,9 +5218,9 @@
   <conditionalFormatting sqref="G26:G40">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5060,9 +5230,9 @@
   <conditionalFormatting sqref="D26:D40">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5072,9 +5242,9 @@
   <conditionalFormatting sqref="AH26:AH40">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5084,9 +5254,9 @@
   <conditionalFormatting sqref="AE26:AE40">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5096,9 +5266,9 @@
   <conditionalFormatting sqref="AB26:AB40">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5108,9 +5278,9 @@
   <conditionalFormatting sqref="Y26:Y40">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5120,9 +5290,9 @@
   <conditionalFormatting sqref="M26:M40">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5132,9 +5302,9 @@
   <conditionalFormatting sqref="V26:V40">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5144,9 +5314,9 @@
   <conditionalFormatting sqref="AH3:AH40">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5156,9 +5326,9 @@
   <conditionalFormatting sqref="AE3:AE40">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5168,9 +5338,9 @@
   <conditionalFormatting sqref="AB3:AB40">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5180,9 +5350,9 @@
   <conditionalFormatting sqref="Y3:Y40">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5192,9 +5362,9 @@
   <conditionalFormatting sqref="V3:V40">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5204,9 +5374,9 @@
   <conditionalFormatting sqref="S3:S40">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5216,9 +5386,9 @@
   <conditionalFormatting sqref="P3:P40">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5228,9 +5398,9 @@
   <conditionalFormatting sqref="M3:M40">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5240,9 +5410,9 @@
   <conditionalFormatting sqref="J3:J40">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5252,9 +5422,9 @@
   <conditionalFormatting sqref="G3:G40">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5264,9 +5434,9 @@
   <conditionalFormatting sqref="D3:D40">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5279,14 +5449,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -5307,7 +5477,7 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>3</v>
       </c>
@@ -5356,7 +5526,7 @@
       <c r="AG1" s="37"/>
       <c r="AH1" s="37"/>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5424,7 +5594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
@@ -5483,7 +5653,7 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -5542,7 +5712,7 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1">
+    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>59</v>
       </c>
@@ -5601,7 +5771,7 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1">
+    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>58</v>
       </c>
@@ -5660,7 +5830,7 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -5731,7 +5901,7 @@
         <v>0.28861666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
@@ -5802,7 +5972,7 @@
         <v>0.32611666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -5873,7 +6043,7 @@
         <v>0.30031666666666662</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -5944,7 +6114,7 @@
         <v>0.33934999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>40</v>
       </c>
@@ -5997,7 +6167,7 @@
         <v>0.26416666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>41</v>
       </c>
@@ -6050,7 +6220,7 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>38</v>
       </c>
@@ -6103,7 +6273,7 @@
         <v>0.28023333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
@@ -6156,7 +6326,7 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
@@ -6215,7 +6385,7 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>43</v>
       </c>
@@ -6274,7 +6444,7 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
@@ -6345,7 +6515,7 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>45</v>
       </c>
@@ -6416,7 +6586,7 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -6487,7 +6657,7 @@
         <v>0.21026666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>33</v>
       </c>
@@ -6558,7 +6728,7 @@
         <v>0.33863333333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>61</v>
       </c>
@@ -6629,7 +6799,7 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>62</v>
       </c>
@@ -6700,7 +6870,7 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
@@ -6771,7 +6941,7 @@
         <v>0.2364333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>64</v>
       </c>
@@ -6842,7 +7012,7 @@
         <v>0.36651666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>73</v>
       </c>
@@ -6901,7 +7071,7 @@
         <v>0.36202499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>74</v>
       </c>
@@ -6960,7 +7130,7 @@
         <v>0.38167500000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>75</v>
       </c>
@@ -7031,7 +7201,7 @@
         <v>0.3566833333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>80</v>
       </c>
@@ -7102,7 +7272,7 @@
         <v>0.31143333333333334</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>85</v>
       </c>
@@ -7161,7 +7331,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>81</v>
       </c>
@@ -7220,7 +7390,7 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>82</v>
       </c>
@@ -7273,7 +7443,7 @@
         <v>0.31570000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>83</v>
       </c>
@@ -7326,7 +7496,7 @@
         <v>0.29619999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>86</v>
       </c>
@@ -7385,7 +7555,7 @@
         <v>0.42807499999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>87</v>
       </c>
@@ -7444,7 +7614,7 @@
         <v>0.41767499999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>99</v>
       </c>
@@ -7515,26 +7685,402 @@
         <v>0.43949999999999995</v>
       </c>
     </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0.39340000000000003</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.4955</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.2021</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="G36" s="9">
+        <v>0.57150000000000001</v>
+      </c>
+      <c r="H36" s="7">
+        <v>0.2412</v>
+      </c>
+      <c r="I36" s="8">
+        <v>0.3876</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.29730000000000001</v>
+      </c>
+      <c r="K36" s="7">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="L36" s="8">
+        <v>0.54679999999999995</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0.45350000000000001</v>
+      </c>
+      <c r="N36" s="7">
+        <v>0.13850000000000001</v>
+      </c>
+      <c r="O36" s="8">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="P36" s="9">
+        <v>0.19650000000000001</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>0.29998999999999998</v>
+      </c>
+      <c r="R36" s="8">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="S36" s="9">
+        <v>0.39789999999999998</v>
+      </c>
+      <c r="T36" s="7">
+        <f t="shared" ref="T36" si="7">AVERAGE(B36,E36,H36,K36,N36,Q36)</f>
+        <v>0.277115</v>
+      </c>
+      <c r="U36" s="8">
+        <f t="shared" ref="U36" si="8">AVERAGE(C36,F36,I36,L36,O36,R36)</f>
+        <v>0.53256666666666674</v>
+      </c>
+      <c r="V36" s="9">
+        <f t="shared" ref="V36" si="9">AVERAGE(D36,G36,J36,M36,P36,S36)</f>
+        <v>0.4020333333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0.30640000000000001</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.60750000000000004</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.4073</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.59370000000000001</v>
+      </c>
+      <c r="F37" s="8">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="G37" s="9">
+        <v>0.51</v>
+      </c>
+      <c r="H37" s="7">
+        <v>5.6599999999999998E-2</v>
+      </c>
+      <c r="I37" s="8">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="J37" s="9">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="K37" s="7">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="L37" s="8">
+        <v>0.4239</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0.3997</v>
+      </c>
+      <c r="N37" s="7">
+        <v>0.1658</v>
+      </c>
+      <c r="O37" s="8">
+        <v>0.24079999999999999</v>
+      </c>
+      <c r="P37" s="9">
+        <v>0.19639999999999999</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>0.24859999999999999</v>
+      </c>
+      <c r="R37" s="8">
+        <v>0.56730000000000003</v>
+      </c>
+      <c r="S37" s="9">
+        <v>0.34570000000000001</v>
+      </c>
+      <c r="T37" s="7">
+        <f t="shared" ref="T37" si="10">AVERAGE(B37,E37,H37,K37,N37,Q37)</f>
+        <v>0.29154999999999998</v>
+      </c>
+      <c r="U37" s="8">
+        <f t="shared" ref="U37" si="11">AVERAGE(C37,F37,I37,L37,O37,R37)</f>
+        <v>0.38694999999999996</v>
+      </c>
+      <c r="V37" s="9">
+        <f t="shared" ref="V37" si="12">AVERAGE(D37,G37,J37,M37,P37,S37)</f>
+        <v>0.31708333333333333</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="7">
+        <v>0.49180000000000001</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.58640000000000003</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.57479999999999998</v>
+      </c>
+      <c r="F38" s="8">
+        <v>0.40389999999999998</v>
+      </c>
+      <c r="G38" s="9">
+        <v>0.47439999999999999</v>
+      </c>
+      <c r="H38" s="7">
+        <v>4.48E-2</v>
+      </c>
+      <c r="I38" s="8">
+        <v>0.999</v>
+      </c>
+      <c r="J38" s="9">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="K38" s="7">
+        <v>0.28320000000000001</v>
+      </c>
+      <c r="L38" s="8">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="M38" s="9">
+        <v>0.42170000000000002</v>
+      </c>
+      <c r="N38" s="7">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="O38" s="8">
+        <v>0.3327</v>
+      </c>
+      <c r="P38" s="9">
+        <v>0.189</v>
+      </c>
+      <c r="Q38" s="7">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="R38" s="8">
+        <v>0.55459999999999998</v>
+      </c>
+      <c r="S38" s="9">
+        <v>0.39439999999999997</v>
+      </c>
+      <c r="T38" s="7">
+        <f t="shared" ref="T38:T39" si="13">AVERAGE(B38,E38,H38,K38,N38,Q38)</f>
+        <v>0.30543333333333339</v>
+      </c>
+      <c r="U38" s="8">
+        <f t="shared" ref="U38:U39" si="14">AVERAGE(C38,F38,I38,L38,O38,R38)</f>
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="V38" s="9">
+        <f t="shared" ref="V38:V39" si="15">AVERAGE(D38,G38,J38,M38,P38,S38)</f>
+        <v>0.35005000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39" s="7">
+        <v>0.3049</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.58640000000000003</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0.4012</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.53310000000000002</v>
+      </c>
+      <c r="F39" s="8">
+        <v>0.46879999999999999</v>
+      </c>
+      <c r="G39" s="9">
+        <v>0.49890000000000001</v>
+      </c>
+      <c r="H39" s="7">
+        <v>2.2100000000000002E-2</v>
+      </c>
+      <c r="I39" s="8">
+        <v>1.5299999999999999E-2</v>
+      </c>
+      <c r="J39" s="9">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="K39" s="7">
+        <v>0.2414</v>
+      </c>
+      <c r="L39" s="8">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0.38829999999999998</v>
+      </c>
+      <c r="N39" s="7">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="O39" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P39" s="9">
+        <v>3.7900000000000003E-2</v>
+      </c>
+      <c r="Q39" s="7">
+        <v>0.25659999999999999</v>
+      </c>
+      <c r="R39" s="8">
+        <v>0.52539999999999998</v>
+      </c>
+      <c r="S39" s="9">
+        <v>0.3448</v>
+      </c>
+      <c r="T39" s="7">
+        <f t="shared" si="13"/>
+        <v>0.23321666666666666</v>
+      </c>
+      <c r="U39" s="8">
+        <f t="shared" si="14"/>
+        <v>0.43710000000000004</v>
+      </c>
+      <c r="V39" s="9">
+        <f t="shared" si="15"/>
+        <v>0.28153333333333336</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="8"/>
+      <c r="V40" s="9"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="9"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="9"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7544,9 +8090,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7556,9 +8102,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7568,9 +8114,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7580,9 +8126,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7592,57 +8138,57 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V43">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D43">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G43">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J43">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7652,9 +8198,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7664,9 +8210,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7676,9 +8222,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7688,9 +8234,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7700,9 +8246,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7712,9 +8258,9 @@
   <conditionalFormatting sqref="M4:M21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7724,9 +8270,9 @@
   <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7736,45 +8282,45 @@
   <conditionalFormatting sqref="S4:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M43">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P43">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S35">
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S43">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -7787,14 +8333,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -7811,7 +8357,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
@@ -7837,7 +8383,7 @@
       </c>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
         <v>48</v>
       </c>
@@ -7875,7 +8421,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>46</v>
       </c>
@@ -7923,7 +8469,7 @@
         <v>1.0845751025000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -7971,7 +8517,7 @@
         <v>1.3607243325</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>50</v>
       </c>
@@ -8019,7 +8565,7 @@
         <v>1.1540821750000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>51</v>
       </c>
@@ -8067,7 +8613,7 @@
         <v>1.4101859700000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>96</v>
       </c>
@@ -8095,7 +8641,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>98</v>
       </c>
@@ -8109,7 +8655,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>68</v>
       </c>
@@ -8150,7 +8696,7 @@
         <v>0.942025</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>71</v>
       </c>
@@ -8187,7 +8733,7 @@
         <v>0.93303333333333338</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>78</v>
       </c>
@@ -8218,7 +8764,7 @@
         <v>0.73710000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>79</v>
       </c>
@@ -8249,7 +8795,7 @@
         <v>0.73635000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>101</v>
       </c>
@@ -8292,13 +8838,13 @@
         <v>1.1484999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -8313,9 +8859,9 @@
   <conditionalFormatting sqref="M3:M13">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8325,9 +8871,9 @@
   <conditionalFormatting sqref="L3:L13">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8337,9 +8883,9 @@
   <conditionalFormatting sqref="B3:B6 B9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8349,9 +8895,9 @@
   <conditionalFormatting sqref="D3:D6 D9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8361,9 +8907,9 @@
   <conditionalFormatting sqref="F3:F6 F9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8373,9 +8919,9 @@
   <conditionalFormatting sqref="H3:H7 H9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8385,9 +8931,9 @@
   <conditionalFormatting sqref="J3:J7 J9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8397,9 +8943,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8409,9 +8955,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8421,9 +8967,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8433,9 +8979,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8445,9 +8991,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8457,9 +9003,9 @@
   <conditionalFormatting sqref="B3:B13">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8469,9 +9015,9 @@
   <conditionalFormatting sqref="C3:C13">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8481,9 +9027,9 @@
   <conditionalFormatting sqref="D3:D13">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8493,9 +9039,9 @@
   <conditionalFormatting sqref="E3:E13">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8505,9 +9051,9 @@
   <conditionalFormatting sqref="F3:F13">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8517,9 +9063,9 @@
   <conditionalFormatting sqref="G3:G13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8529,9 +9075,9 @@
   <conditionalFormatting sqref="H3:H13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8541,9 +9087,9 @@
   <conditionalFormatting sqref="I3:I13">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8553,9 +9099,9 @@
   <conditionalFormatting sqref="J3:J13">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8565,9 +9111,9 @@
   <conditionalFormatting sqref="K3:K13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8580,14 +9126,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -8604,7 +9150,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
@@ -8630,7 +9176,7 @@
       </c>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" s="33" t="s">
         <v>48</v>
       </c>
@@ -8668,7 +9214,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>101</v>
       </c>
@@ -8711,30 +9257,30 @@
         <v>0.65325</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L1:M1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="M3">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8744,9 +9290,9 @@
   <conditionalFormatting sqref="L3">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8756,9 +9302,9 @@
   <conditionalFormatting sqref="B3">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8768,9 +9314,9 @@
   <conditionalFormatting sqref="C3">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8780,9 +9326,9 @@
   <conditionalFormatting sqref="D3">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8792,9 +9338,9 @@
   <conditionalFormatting sqref="E3">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8804,9 +9350,9 @@
   <conditionalFormatting sqref="F3">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8816,9 +9362,9 @@
   <conditionalFormatting sqref="G3">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8828,9 +9374,9 @@
   <conditionalFormatting sqref="H3">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8840,9 +9386,9 @@
   <conditionalFormatting sqref="I3">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8852,9 +9398,9 @@
   <conditionalFormatting sqref="J3">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -8864,9 +9410,9 @@
   <conditionalFormatting sqref="K3">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -8879,14 +9425,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="31" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -8895,7 +9441,7 @@
     <col min="38" max="40" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
@@ -8962,7 +9508,7 @@
       <c r="AM1" s="34"/>
       <c r="AN1" s="35"/>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9084,7 +9630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>92</v>
       </c>
@@ -9209,7 +9755,7 @@
         <v>0.45634545454545455</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>93</v>
       </c>
@@ -9334,7 +9880,7 @@
         <v>0.49341818181818181</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>94</v>
       </c>
@@ -9459,7 +10005,7 @@
         <v>0.4236454545454546</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>95</v>
       </c>
@@ -9584,7 +10130,7 @@
         <v>0.51095454545454555</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -9626,7 +10172,7 @@
       <c r="AM7" s="11"/>
       <c r="AN7" s="12"/>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -9668,7 +10214,7 @@
       <c r="AM8" s="11"/>
       <c r="AN8" s="12"/>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -9729,9 +10275,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9741,9 +10287,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9753,9 +10299,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9765,9 +10311,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9777,9 +10323,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9789,9 +10335,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9801,9 +10347,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9813,9 +10359,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9825,9 +10371,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9837,9 +10383,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9849,9 +10395,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9861,9 +10407,9 @@
   <conditionalFormatting sqref="AN3:AN9">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9873,9 +10419,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9885,9 +10431,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9897,9 +10443,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9909,9 +10455,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9921,9 +10467,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9933,9 +10479,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9945,9 +10491,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9957,9 +10503,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9969,9 +10515,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9981,9 +10527,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9993,9 +10539,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10005,9 +10551,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10017,9 +10563,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10029,9 +10575,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10041,9 +10587,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10053,9 +10599,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10065,9 +10611,9 @@
   <conditionalFormatting sqref="AE4:AE9">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10077,9 +10623,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10089,9 +10635,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10101,9 +10647,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10113,9 +10659,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10125,9 +10671,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10137,9 +10683,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10149,9 +10695,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10161,9 +10707,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10173,9 +10719,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10185,9 +10731,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="25">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10197,9 +10743,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10209,9 +10755,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10221,9 +10767,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10233,9 +10779,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10245,9 +10791,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10257,9 +10803,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10269,9 +10815,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10281,9 +10827,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10293,9 +10839,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10305,9 +10851,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10317,9 +10863,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10329,9 +10875,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10341,9 +10887,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10353,9 +10899,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10365,9 +10911,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10377,9 +10923,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10389,9 +10935,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10401,9 +10947,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10413,9 +10959,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10425,9 +10971,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10437,9 +10983,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10449,9 +10995,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10461,9 +11007,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10473,9 +11019,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>

<commit_message>
Getting DISFA ready for this.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800"/>
@@ -11,14 +11,14 @@
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
     <sheet name="BP4D_int_seg" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
+    <sheet name="DISFA" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="128">
   <si>
     <t>DEVEL</t>
   </si>
@@ -218,9 +218,6 @@
     <t>BP4D MLP scale</t>
   </si>
   <si>
-    <t>AU28 *might need sep model</t>
-  </si>
-  <si>
     <t>BP4D MLP dynamic</t>
   </si>
   <si>
@@ -363,13 +360,55 @@
   </si>
   <si>
     <t>BP4D SVM SMOTE</t>
+  </si>
+  <si>
+    <t>App, geom, different weights (scikit learn)</t>
+  </si>
+  <si>
+    <t>BP4D weights</t>
+  </si>
+  <si>
+    <t>App geom, ensemble dynamic</t>
+  </si>
+  <si>
+    <t>App, geom old undersampling, 1-1 dynamic</t>
+  </si>
+  <si>
+    <t>App, geom old undersampling, 1-1 static</t>
+  </si>
+  <si>
+    <t>DISFA SVM sampled stat</t>
+  </si>
+  <si>
+    <t>DISFA SVM sampled dyn</t>
+  </si>
+  <si>
+    <t>BP4D SVM sampled dyn</t>
+  </si>
+  <si>
+    <t>BP4D SVM sampled stat</t>
+  </si>
+  <si>
+    <t>Combined SVM sampled stat</t>
+  </si>
+  <si>
+    <t>Combined SVM sampled dyn v sem</t>
+  </si>
+  <si>
+    <t>AU28</t>
+  </si>
+  <si>
+    <t>BP4D SVM static, caelum 101</t>
+  </si>
+  <si>
+    <t>BP4D SVM dynamic, caelum 101</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -507,12 +546,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -572,6 +622,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -663,7 +720,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -698,7 +754,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -874,20 +929,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41.5703125" customWidth="1"/>
     <col min="2" max="37" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
@@ -949,7 +1004,7 @@
       <c r="AJ1" s="34"/>
       <c r="AK1" s="35"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
@@ -1178,7 +1233,7 @@
         <v>0.26816666666666661</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1270,7 +1325,7 @@
         <v>0.25200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
@@ -1362,7 +1417,7 @@
         <v>0.23471428571428571</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" ht="16.5" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
@@ -1454,7 +1509,7 @@
         <v>0.3408571428571428</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1546,7 +1601,7 @@
         <v>0.21928571428571431</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -1662,7 +1717,7 @@
         <v>0.60526363636363623</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
@@ -1778,7 +1833,7 @@
         <v>0.59264545454545459</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
@@ -1894,7 +1949,7 @@
         <v>0.59812727272727273</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -2010,7 +2065,7 @@
         <v>0.59751818181818195</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>
@@ -2069,7 +2124,7 @@
       <c r="AJ12" s="11"/>
       <c r="AK12" s="12"/>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
@@ -2128,7 +2183,7 @@
       <c r="AJ13" s="11"/>
       <c r="AK13" s="12"/>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="5" t="s">
         <v>34</v>
       </c>
@@ -2187,7 +2242,7 @@
       <c r="AJ14" s="11"/>
       <c r="AK14" s="12"/>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="5" t="s">
         <v>35</v>
       </c>
@@ -2246,7 +2301,7 @@
       <c r="AJ15" s="11"/>
       <c r="AK15" s="12"/>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2329,7 +2384,7 @@
       <c r="AJ16" s="11"/>
       <c r="AK16" s="12"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
@@ -2412,7 +2467,7 @@
       <c r="AJ17" s="11"/>
       <c r="AK17" s="12"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="25" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2538,7 @@
       <c r="AJ18" s="11"/>
       <c r="AK18" s="12"/>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="25" t="s">
         <v>47</v>
       </c>
@@ -2554,7 +2609,7 @@
       <c r="AJ19" s="11"/>
       <c r="AK19" s="12"/>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="25" t="s">
         <v>52</v>
       </c>
@@ -2670,7 +2725,7 @@
         <v>0.57558181818181819</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="25" t="s">
         <v>53</v>
       </c>
@@ -2786,7 +2841,7 @@
         <v>0.58974545454545457</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="25" t="s">
         <v>54</v>
       </c>
@@ -2902,7 +2957,7 @@
         <v>0.58663636363636362</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" s="25" t="s">
         <v>55</v>
       </c>
@@ -3018,7 +3073,7 @@
         <v>0.59650909090909088</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" s="25" t="s">
         <v>56</v>
       </c>
@@ -3134,7 +3189,7 @@
         <v>0.5917</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="25" t="s">
         <v>60</v>
       </c>
@@ -3250,7 +3305,7 @@
         <v>0.61232727272727272</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="25" t="s">
         <v>65</v>
       </c>
@@ -3366,9 +3421,9 @@
         <v>0.58963636363636374</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="7">
         <v>0.3306</v>
@@ -3482,9 +3537,9 @@
         <v>0.57887272727272732</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="7">
         <v>0.41089999999999999</v>
@@ -3598,9 +3653,9 @@
         <v>0.60222727272727272</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="7">
         <v>0.43840000000000001</v>
@@ -3681,9 +3736,9 @@
       <c r="AJ29" s="11"/>
       <c r="AK29" s="12"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" s="7">
         <v>0.3584</v>
@@ -3797,9 +3852,9 @@
         <v>0.60204545454545466</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37">
       <c r="A31" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="7">
         <v>0.49170000000000003</v>
@@ -3880,9 +3935,9 @@
       <c r="AJ31" s="11"/>
       <c r="AK31" s="12"/>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37">
       <c r="A32" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B32" s="7">
         <v>0.36620000000000003</v>
@@ -3996,9 +4051,9 @@
         <v>0.58684545454545445</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37">
       <c r="A33" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="7">
         <v>0.34839999999999999</v>
@@ -4079,9 +4134,9 @@
       <c r="AJ33" s="11"/>
       <c r="AK33" s="12"/>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37">
       <c r="A34" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="7">
         <v>0.34799999999999998</v>
@@ -4195,9 +4250,9 @@
         <v>0.60236363636363643</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37">
       <c r="A35" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" s="7">
         <v>0.2984</v>
@@ -4311,9 +4366,9 @@
         <v>0.55642727272727277</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37">
       <c r="A36" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B36" s="7">
         <v>0.4365</v>
@@ -4427,9 +4482,9 @@
         <v>0.55127272727272725</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37">
       <c r="A37" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="7">
         <v>0.33360000000000001</v>
@@ -4543,9 +4598,9 @@
         <v>0.55403636363636355</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37">
       <c r="A38" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B38" s="7">
         <v>0.32329999999999998</v>
@@ -4659,9 +4714,9 @@
         <v>0.54439090909090904</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37">
       <c r="A39" s="25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B39" s="7">
         <v>0.40389999999999998</v>
@@ -4775,9 +4830,9 @@
         <v>0.60190909090909095</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37">
       <c r="A40" s="25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B40" s="7">
         <v>0.36620000000000003</v>
@@ -4891,9 +4946,9 @@
         <v>0.60019999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37">
       <c r="A41" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B41" s="7">
         <v>0.37190000000000001</v>
@@ -5007,45 +5062,126 @@
         <v>0.60027272727272729</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="T42" s="7"/>
-      <c r="U42" s="8"/>
-      <c r="V42" s="8"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="8"/>
-      <c r="Y42" s="8"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="8"/>
-      <c r="AB42" s="8"/>
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="8"/>
-      <c r="AE42" s="8"/>
-      <c r="AF42" s="7"/>
-      <c r="AG42" s="8"/>
-      <c r="AH42" s="9"/>
-      <c r="AI42" s="10"/>
-      <c r="AJ42" s="11"/>
-      <c r="AK42" s="12"/>
-    </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37">
+      <c r="A42" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0.34820000000000001</v>
+      </c>
+      <c r="C42" s="8">
+        <v>0.50519999999999998</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.4123</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.29270000000000002</v>
+      </c>
+      <c r="F42" s="8">
+        <v>0.42320000000000002</v>
+      </c>
+      <c r="G42" s="9">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0.34439999999999998</v>
+      </c>
+      <c r="I42" s="8">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="J42" s="9">
+        <v>0.43709999999999999</v>
+      </c>
+      <c r="K42" s="7">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="L42" s="8">
+        <v>0.76780000000000004</v>
+      </c>
+      <c r="M42" s="8">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="N42" s="7">
+        <v>0.75529999999999997</v>
+      </c>
+      <c r="O42" s="8">
+        <v>0.74070000000000003</v>
+      </c>
+      <c r="P42" s="8">
+        <v>0.74790000000000001</v>
+      </c>
+      <c r="Q42" s="7">
+        <v>0.87770000000000004</v>
+      </c>
+      <c r="R42" s="8">
+        <v>0.78510000000000002</v>
+      </c>
+      <c r="S42" s="8">
+        <v>0.82879999999999998</v>
+      </c>
+      <c r="T42" s="7">
+        <v>0.88739999999999997</v>
+      </c>
+      <c r="U42" s="8">
+        <v>0.83720000000000006</v>
+      </c>
+      <c r="V42" s="8">
+        <v>0.86160000000000003</v>
+      </c>
+      <c r="W42" s="7">
+        <v>0.6149</v>
+      </c>
+      <c r="X42" s="8">
+        <v>0.7258</v>
+      </c>
+      <c r="Y42" s="8">
+        <v>0.66579999999999995</v>
+      </c>
+      <c r="Z42" s="7">
+        <v>0.317</v>
+      </c>
+      <c r="AA42" s="8">
+        <v>0.69079999999999997</v>
+      </c>
+      <c r="AB42" s="8">
+        <v>0.43459999999999999</v>
+      </c>
+      <c r="AC42" s="7">
+        <v>0.52639999999999998</v>
+      </c>
+      <c r="AD42" s="8">
+        <v>0.76060000000000005</v>
+      </c>
+      <c r="AE42" s="8">
+        <v>0.62219999999999998</v>
+      </c>
+      <c r="AF42" s="7">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="AG42" s="8">
+        <v>0.64129999999999998</v>
+      </c>
+      <c r="AH42" s="9">
+        <v>0.43830000000000002</v>
+      </c>
+      <c r="AI42" s="10">
+        <f t="shared" ref="AI42" si="18">AVERAGE(B42,E42,H42,K42,N42,Q42,T42,W42,Z42,AC42,AF42)</f>
+        <v>0.55155454545454552</v>
+      </c>
+      <c r="AJ42" s="11">
+        <f t="shared" ref="AJ42" si="19">AVERAGE(C42,F42,I42,L42,O42,R42,U42,X42,AA42,AD42,AG42)</f>
+        <v>0.67960909090909094</v>
+      </c>
+      <c r="AK42" s="12">
+        <f t="shared" ref="AK42" si="20">AVERAGE(D42,G42,J42,M42,P42,S42,V42,Y42,AB42,AE42,AH42)</f>
+        <v>0.59669090909090905</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="A43" s="25" t="s">
+        <v>126</v>
+      </c>
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="9"/>
@@ -5083,7 +5219,10 @@
       <c r="AJ43" s="11"/>
       <c r="AK43" s="12"/>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37">
+      <c r="A44" s="25" t="s">
+        <v>127</v>
+      </c>
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
@@ -5121,7 +5260,7 @@
       <c r="AJ44" s="11"/>
       <c r="AK44" s="12"/>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37">
       <c r="B45" s="7"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
@@ -5159,7 +5298,7 @@
       <c r="AJ45" s="11"/>
       <c r="AK45" s="12"/>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37">
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
@@ -5197,7 +5336,7 @@
       <c r="AJ46" s="11"/>
       <c r="AK46" s="12"/>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37">
       <c r="B47" s="7"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
@@ -5253,9 +5392,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="76">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5265,9 +5404,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="75">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5277,9 +5416,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="74">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5289,9 +5428,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="73">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5301,9 +5440,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="72">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5313,9 +5452,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="71">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5325,9 +5464,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="70">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5337,9 +5476,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="69">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5349,9 +5488,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="68">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5361,9 +5500,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="67">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5373,9 +5512,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="66">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5385,9 +5524,9 @@
   <conditionalFormatting sqref="AK3:AK47">
     <cfRule type="colorScale" priority="65">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5397,9 +5536,9 @@
   <conditionalFormatting sqref="D3:D17">
     <cfRule type="colorScale" priority="64">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5409,9 +5548,9 @@
   <conditionalFormatting sqref="G3:G11">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5421,9 +5560,9 @@
   <conditionalFormatting sqref="J3:J11">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5433,9 +5572,9 @@
   <conditionalFormatting sqref="M3:M11">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5445,9 +5584,9 @@
   <conditionalFormatting sqref="P3:P11">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5457,9 +5596,9 @@
   <conditionalFormatting sqref="S3:S11">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5469,9 +5608,9 @@
   <conditionalFormatting sqref="V3:V11">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5481,9 +5620,9 @@
   <conditionalFormatting sqref="Y3:Y11">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5493,9 +5632,9 @@
   <conditionalFormatting sqref="AB3:AB11">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5505,9 +5644,9 @@
   <conditionalFormatting sqref="AE3:AE11">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5517,9 +5656,9 @@
   <conditionalFormatting sqref="AH3:AH11">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5529,9 +5668,9 @@
   <conditionalFormatting sqref="G3:G21">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5541,9 +5680,9 @@
   <conditionalFormatting sqref="V3:V21">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5553,9 +5692,9 @@
   <conditionalFormatting sqref="AE3:AE19 AE21">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5565,9 +5704,9 @@
   <conditionalFormatting sqref="J3:J17">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5577,9 +5716,9 @@
   <conditionalFormatting sqref="M3:M17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5589,9 +5728,9 @@
   <conditionalFormatting sqref="AB4:AB17">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5601,9 +5740,9 @@
   <conditionalFormatting sqref="S8:S18">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5613,9 +5752,9 @@
   <conditionalFormatting sqref="Y8:Y18">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5625,9 +5764,9 @@
   <conditionalFormatting sqref="Y8:Y19">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5637,9 +5776,9 @@
   <conditionalFormatting sqref="S8:S19">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5649,9 +5788,9 @@
   <conditionalFormatting sqref="M3:M19">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5661,9 +5800,9 @@
   <conditionalFormatting sqref="M3:M20">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5673,9 +5812,9 @@
   <conditionalFormatting sqref="AH8:AH20">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5685,9 +5824,9 @@
   <conditionalFormatting sqref="AE3:AE21">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5697,9 +5836,9 @@
   <conditionalFormatting sqref="AB3:AB20">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5709,9 +5848,9 @@
   <conditionalFormatting sqref="Y8:Y20">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5721,9 +5860,9 @@
   <conditionalFormatting sqref="S3:S24">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5733,9 +5872,9 @@
   <conditionalFormatting sqref="P3:P25 P27:P47">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5745,9 +5884,9 @@
   <conditionalFormatting sqref="J3:J25 X29:X47 J27:J47">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5757,9 +5896,9 @@
   <conditionalFormatting sqref="G3:G25 G27:G47">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5769,9 +5908,9 @@
   <conditionalFormatting sqref="D3:D25 D27:D47">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5781,9 +5920,9 @@
   <conditionalFormatting sqref="AH3:AH25 AH27:AH47">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5793,9 +5932,9 @@
   <conditionalFormatting sqref="AE3:AE25 AE27:AE47">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5805,9 +5944,9 @@
   <conditionalFormatting sqref="AB3:AB25 AB27:AB47">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5817,9 +5956,9 @@
   <conditionalFormatting sqref="Y3:Y25 Y27:Y47">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5829,9 +5968,9 @@
   <conditionalFormatting sqref="M3:M25 M27:M47">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5841,9 +5980,9 @@
   <conditionalFormatting sqref="V3:V25 V27:V47">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5853,9 +5992,9 @@
   <conditionalFormatting sqref="S3:S25">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5865,9 +6004,9 @@
   <conditionalFormatting sqref="S26:S47">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5877,9 +6016,9 @@
   <conditionalFormatting sqref="P26:P47">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5889,9 +6028,9 @@
   <conditionalFormatting sqref="J26:J47">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5901,9 +6040,9 @@
   <conditionalFormatting sqref="G26:G47">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5913,9 +6052,9 @@
   <conditionalFormatting sqref="D26:D47">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5925,9 +6064,9 @@
   <conditionalFormatting sqref="AH26:AH47">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5937,9 +6076,9 @@
   <conditionalFormatting sqref="AE26:AE47">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5949,9 +6088,9 @@
   <conditionalFormatting sqref="AB26:AB47">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5961,9 +6100,9 @@
   <conditionalFormatting sqref="Y26:Y47">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5973,9 +6112,9 @@
   <conditionalFormatting sqref="M26:M47">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5985,9 +6124,9 @@
   <conditionalFormatting sqref="V26:V47">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -5997,9 +6136,9 @@
   <conditionalFormatting sqref="AH3:AH47">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6009,9 +6148,9 @@
   <conditionalFormatting sqref="AE3:AE47">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6021,9 +6160,9 @@
   <conditionalFormatting sqref="AB3:AB47">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6033,9 +6172,9 @@
   <conditionalFormatting sqref="Y3:Y47">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6045,9 +6184,9 @@
   <conditionalFormatting sqref="V3:V47">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6057,9 +6196,9 @@
   <conditionalFormatting sqref="S3:S47">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6069,9 +6208,9 @@
   <conditionalFormatting sqref="P3:P47">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6081,9 +6220,9 @@
   <conditionalFormatting sqref="M3:M47">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6093,9 +6232,9 @@
   <conditionalFormatting sqref="J3:J47">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6105,9 +6244,9 @@
   <conditionalFormatting sqref="G3:G47">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6117,9 +6256,9 @@
   <conditionalFormatting sqref="D3:D47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -6132,14 +6271,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AH55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" customWidth="1"/>
@@ -6160,7 +6299,7 @@
     <col min="22" max="22" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34">
       <c r="B1" s="36" t="s">
         <v>3</v>
       </c>
@@ -6182,7 +6321,7 @@
       <c r="L1" s="34"/>
       <c r="M1" s="35"/>
       <c r="N1" s="36" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="O1" s="34"/>
       <c r="P1" s="35"/>
@@ -6209,8 +6348,8 @@
       <c r="AG1" s="37"/>
       <c r="AH1" s="37"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:34">
+      <c r="A2" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -6277,8 +6416,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:34" ht="17.25" customHeight="1">
+      <c r="A3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="10">
@@ -6336,8 +6475,8 @@
         <v>0.40849999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:34">
+      <c r="A4" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="10">
@@ -6395,8 +6534,8 @@
         <v>0.42475000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:34" ht="15" customHeight="1">
+      <c r="A5" s="39" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="10">
@@ -6454,8 +6593,8 @@
         <v>0.27600000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:34" ht="15" customHeight="1">
+      <c r="A6" s="39" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="10">
@@ -6513,8 +6652,8 @@
         <v>0.42574999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:34">
+      <c r="A7" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="10">
@@ -6584,8 +6723,8 @@
         <v>0.28861666666666669</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:34">
+      <c r="A8" s="39" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="15">
@@ -6655,8 +6794,8 @@
         <v>0.32611666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:34">
+      <c r="A9" s="39" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="7">
@@ -6726,8 +6865,8 @@
         <v>0.30031666666666662</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:34">
+      <c r="A10" s="39" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="7">
@@ -6797,8 +6936,8 @@
         <v>0.33934999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:34">
+      <c r="A11" s="39" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="7">
@@ -6850,8 +6989,8 @@
         <v>0.26416666666666666</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:34">
+      <c r="A12" s="39" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="7">
@@ -6903,8 +7042,8 @@
         <v>0.30256666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:34">
+      <c r="A13" s="39" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="7">
@@ -6956,8 +7095,8 @@
         <v>0.28023333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+    <row r="14" spans="1:34">
+      <c r="A14" s="39" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="7">
@@ -7009,8 +7148,8 @@
         <v>0.28770000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:34">
+      <c r="A15" s="39" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="7">
@@ -7068,8 +7207,8 @@
         <v>0.40457500000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:34">
+      <c r="A16" s="40" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="7">
@@ -7127,8 +7266,8 @@
         <v>0.44357500000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:22">
+      <c r="A17" s="40" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="7">
@@ -7198,8 +7337,8 @@
         <v>0.24411666666666668</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:22">
+      <c r="A18" s="40" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="7">
@@ -7269,8 +7408,8 @@
         <v>0.29361666666666664</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:22">
+      <c r="A19" s="39" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="7">
@@ -7340,8 +7479,8 @@
         <v>0.21026666666666669</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:22">
+      <c r="A20" s="39" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="7">
@@ -7411,8 +7550,8 @@
         <v>0.33863333333333334</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:22">
+      <c r="A21" s="39" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="7">
@@ -7482,8 +7621,8 @@
         <v>0.26086666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:22">
+      <c r="A22" s="39" t="s">
         <v>62</v>
       </c>
       <c r="B22" s="7">
@@ -7553,8 +7692,8 @@
         <v>0.24983333333333335</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+    <row r="23" spans="1:22">
+      <c r="A23" s="39" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="7">
@@ -7624,8 +7763,8 @@
         <v>0.2364333333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+    <row r="24" spans="1:22">
+      <c r="A24" s="39" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="7">
@@ -7695,9 +7834,9 @@
         <v>0.36651666666666666</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>73</v>
+    <row r="25" spans="1:22">
+      <c r="A25" s="39" t="s">
+        <v>72</v>
       </c>
       <c r="B25" s="7">
         <v>0.1444</v>
@@ -7754,9 +7893,9 @@
         <v>0.36202499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>74</v>
+    <row r="26" spans="1:22">
+      <c r="A26" s="39" t="s">
+        <v>73</v>
       </c>
       <c r="B26" s="7">
         <v>0.1961</v>
@@ -7813,9 +7952,9 @@
         <v>0.38167500000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>75</v>
+    <row r="27" spans="1:22">
+      <c r="A27" s="39" t="s">
+        <v>74</v>
       </c>
       <c r="B27" s="7">
         <v>0.5837</v>
@@ -7884,9 +8023,9 @@
         <v>0.3566833333333333</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>80</v>
+    <row r="28" spans="1:22">
+      <c r="A28" s="39" t="s">
+        <v>79</v>
       </c>
       <c r="B28" s="7">
         <v>0.26919999999999999</v>
@@ -7955,9 +8094,9 @@
         <v>0.31143333333333334</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
-        <v>85</v>
+    <row r="29" spans="1:22">
+      <c r="A29" s="40" t="s">
+        <v>84</v>
       </c>
       <c r="B29" s="7">
         <v>0.21</v>
@@ -8014,9 +8153,9 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>81</v>
+    <row r="30" spans="1:22">
+      <c r="A30" s="40" t="s">
+        <v>80</v>
       </c>
       <c r="B30" s="7">
         <v>0.60299999999999998</v>
@@ -8073,9 +8212,9 @@
         <v>0.35099999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>82</v>
+    <row r="31" spans="1:22">
+      <c r="A31" s="40" t="s">
+        <v>81</v>
       </c>
       <c r="B31" s="7">
         <v>0.26519999999999999</v>
@@ -8126,9 +8265,9 @@
         <v>0.31570000000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>83</v>
+    <row r="32" spans="1:22">
+      <c r="A32" s="40" t="s">
+        <v>82</v>
       </c>
       <c r="B32" s="7">
         <v>0.1608</v>
@@ -8179,9 +8318,9 @@
         <v>0.29619999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
-        <v>86</v>
+    <row r="33" spans="1:22">
+      <c r="A33" s="40" t="s">
+        <v>85</v>
       </c>
       <c r="B33" s="7">
         <v>0.30349999999999999</v>
@@ -8238,9 +8377,9 @@
         <v>0.42807499999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
-        <v>87</v>
+    <row r="34" spans="1:22">
+      <c r="A34" s="40" t="s">
+        <v>86</v>
       </c>
       <c r="B34" s="7">
         <v>0.63</v>
@@ -8297,9 +8436,9 @@
         <v>0.41767499999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
-        <v>113</v>
+    <row r="35" spans="1:22">
+      <c r="A35" s="40" t="s">
+        <v>112</v>
       </c>
       <c r="B35" s="7">
         <v>0.63500000000000001</v>
@@ -8368,9 +8507,9 @@
         <v>0.43949999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>102</v>
+    <row r="36" spans="1:22">
+      <c r="A36" s="40" t="s">
+        <v>101</v>
       </c>
       <c r="B36" s="7">
         <v>0.39340000000000003</v>
@@ -8439,9 +8578,9 @@
         <v>0.4020333333333333</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
-        <v>101</v>
+    <row r="37" spans="1:22">
+      <c r="A37" s="40" t="s">
+        <v>100</v>
       </c>
       <c r="B37" s="7">
         <v>0.30640000000000001</v>
@@ -8510,9 +8649,9 @@
         <v>0.31708333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>103</v>
+    <row r="38" spans="1:22">
+      <c r="A38" s="40" t="s">
+        <v>102</v>
       </c>
       <c r="B38" s="7">
         <v>0.49180000000000001</v>
@@ -8581,9 +8720,9 @@
         <v>0.35005000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
-        <v>104</v>
+    <row r="39" spans="1:22">
+      <c r="A39" s="40" t="s">
+        <v>103</v>
       </c>
       <c r="B39" s="7">
         <v>0.3049</v>
@@ -8652,9 +8791,9 @@
         <v>0.28153333333333336</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A40" s="25" t="s">
-        <v>107</v>
+    <row r="40" spans="1:22">
+      <c r="A40" s="40" t="s">
+        <v>106</v>
       </c>
       <c r="B40" s="7">
         <v>0.62919999999999998</v>
@@ -8723,9 +8862,9 @@
         <v>0.4820166666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A41" s="25" t="s">
-        <v>108</v>
+    <row r="41" spans="1:22">
+      <c r="A41" s="40" t="s">
+        <v>107</v>
       </c>
       <c r="B41" s="7">
         <v>0.28489999999999999</v>
@@ -8794,9 +8933,9 @@
         <v>0.37363333333333332</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A42" s="25" t="s">
-        <v>110</v>
+    <row r="42" spans="1:22">
+      <c r="A42" s="40" t="s">
+        <v>109</v>
       </c>
       <c r="B42" s="7">
         <v>0.49840000000000001</v>
@@ -8865,9 +9004,9 @@
         <v>0.47994999999999993</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
-        <v>112</v>
+    <row r="43" spans="1:22">
+      <c r="A43" s="40" t="s">
+        <v>111</v>
       </c>
       <c r="B43" s="7">
         <v>0.47760000000000002</v>
@@ -8936,99 +9075,294 @@
         <v>0.48656666666666665</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="7"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="9"/>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="9"/>
-      <c r="T45" s="7"/>
-      <c r="U45" s="8"/>
-      <c r="V45" s="9"/>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="8"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="7"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="7"/>
-      <c r="U46" s="8"/>
-      <c r="V46" s="9"/>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="7"/>
-      <c r="R47" s="8"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="7"/>
-      <c r="U47" s="8"/>
-      <c r="V47" s="9"/>
-    </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22">
+      <c r="A44" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0.48120000000000002</v>
+      </c>
+      <c r="C44" s="8">
+        <v>0.65690000000000004</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.55179999999999996</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.5907</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.61580000000000001</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0.50370000000000004</v>
+      </c>
+      <c r="I44" s="8">
+        <v>0.37740000000000001</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0.43149999999999999</v>
+      </c>
+      <c r="K44" s="7">
+        <v>0.43909999999999999</v>
+      </c>
+      <c r="L44" s="8">
+        <v>0.51380000000000003</v>
+      </c>
+      <c r="M44" s="9">
+        <v>0.47349999999999998</v>
+      </c>
+      <c r="N44" s="7">
+        <v>0.52759999999999996</v>
+      </c>
+      <c r="O44" s="8">
+        <v>0.3266</v>
+      </c>
+      <c r="P44" s="9">
+        <v>0.40350000000000003</v>
+      </c>
+      <c r="Q44" s="7">
+        <v>0.313</v>
+      </c>
+      <c r="R44" s="8">
+        <v>0.64029999999999998</v>
+      </c>
+      <c r="S44" s="9">
+        <v>0.42049999999999998</v>
+      </c>
+      <c r="T44" s="7">
+        <f t="shared" ref="T44:T47" si="16">AVERAGE(B44,E44,H44,K44,N44,Q44)</f>
+        <v>0.47588333333333338</v>
+      </c>
+      <c r="U44" s="8">
+        <f t="shared" ref="U44:U47" si="17">AVERAGE(C44,F44,I44,L44,O44,R44)</f>
+        <v>0.52179999999999993</v>
+      </c>
+      <c r="V44" s="9">
+        <f t="shared" ref="V44:V47" si="18">AVERAGE(D44,G44,J44,M44,P44,S44)</f>
+        <v>0.4806333333333333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B45" s="7">
+        <v>0.4773</v>
+      </c>
+      <c r="C45" s="8">
+        <v>0.6764</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.55969999999999998</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.57750000000000001</v>
+      </c>
+      <c r="F45" s="8">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="G45" s="9">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="H45" s="7">
+        <v>0.4551</v>
+      </c>
+      <c r="I45" s="8">
+        <v>0.41049999999999998</v>
+      </c>
+      <c r="J45" s="9">
+        <v>0.43159999999999998</v>
+      </c>
+      <c r="K45" s="7">
+        <v>0.44919999999999999</v>
+      </c>
+      <c r="L45" s="8">
+        <v>0.495</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="N45" s="7">
+        <v>0.52849999999999997</v>
+      </c>
+      <c r="O45" s="8">
+        <v>0.317</v>
+      </c>
+      <c r="P45" s="9">
+        <v>0.39629999999999999</v>
+      </c>
+      <c r="Q45" s="7">
+        <v>0.31080000000000002</v>
+      </c>
+      <c r="R45" s="8">
+        <v>0.64949999999999997</v>
+      </c>
+      <c r="S45" s="9">
+        <v>0.4204</v>
+      </c>
+      <c r="T45" s="7">
+        <f t="shared" si="16"/>
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="U45" s="8">
+        <f t="shared" si="17"/>
+        <v>0.52951666666666675</v>
+      </c>
+      <c r="V45" s="9">
+        <f t="shared" si="18"/>
+        <v>0.48016666666666663</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="7">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="C46" s="8">
+        <v>0.66149999999999998</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.55969999999999998</v>
+      </c>
+      <c r="E46" s="7">
+        <v>0.57979999999999998</v>
+      </c>
+      <c r="F46" s="8">
+        <v>0.62649999999999995</v>
+      </c>
+      <c r="G46" s="9">
+        <v>0.60229999999999995</v>
+      </c>
+      <c r="H46" s="7">
+        <v>0.4627</v>
+      </c>
+      <c r="I46" s="8">
+        <v>0.40129999999999999</v>
+      </c>
+      <c r="J46" s="9">
+        <v>0.42980000000000002</v>
+      </c>
+      <c r="K46" s="7">
+        <v>0.42409999999999998</v>
+      </c>
+      <c r="L46" s="8">
+        <v>0.51949999999999996</v>
+      </c>
+      <c r="M46" s="9">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="N46" s="7">
+        <v>0.46289999999999998</v>
+      </c>
+      <c r="O46" s="8">
+        <v>0.3327</v>
+      </c>
+      <c r="P46" s="9">
+        <v>0.38719999999999999</v>
+      </c>
+      <c r="Q46" s="7">
+        <v>0.30669999999999997</v>
+      </c>
+      <c r="R46" s="8">
+        <v>0.65539999999999998</v>
+      </c>
+      <c r="S46" s="9">
+        <v>0.4178</v>
+      </c>
+      <c r="T46" s="7">
+        <f t="shared" si="16"/>
+        <v>0.45353333333333329</v>
+      </c>
+      <c r="U46" s="8">
+        <f t="shared" si="17"/>
+        <v>0.53281666666666661</v>
+      </c>
+      <c r="V46" s="9">
+        <f t="shared" si="18"/>
+        <v>0.4773</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="7">
+        <v>0.21079999999999999</v>
+      </c>
+      <c r="C47" s="8">
+        <v>0.60509999999999997</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0.31269999999999998</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.4985</v>
+      </c>
+      <c r="F47" s="8">
+        <v>0.68510000000000004</v>
+      </c>
+      <c r="G47" s="9">
+        <v>0.57709999999999995</v>
+      </c>
+      <c r="H47" s="7">
+        <v>0.1978</v>
+      </c>
+      <c r="I47" s="8">
+        <v>9.9900000000000003E-2</v>
+      </c>
+      <c r="J47" s="9">
+        <v>0.1328</v>
+      </c>
+      <c r="K47" s="7">
+        <v>0.376</v>
+      </c>
+      <c r="L47" s="8">
+        <v>0.5958</v>
+      </c>
+      <c r="M47" s="9">
+        <v>0.46110000000000001</v>
+      </c>
+      <c r="N47" s="7">
+        <v>0.59450000000000003</v>
+      </c>
+      <c r="O47" s="8">
+        <v>0.34150000000000003</v>
+      </c>
+      <c r="P47" s="9">
+        <v>0.43380000000000002</v>
+      </c>
+      <c r="Q47" s="7">
+        <v>0.23910000000000001</v>
+      </c>
+      <c r="R47" s="8">
+        <v>0.6956</v>
+      </c>
+      <c r="S47" s="9">
+        <v>0.35589999999999999</v>
+      </c>
+      <c r="T47" s="7">
+        <f t="shared" si="16"/>
+        <v>0.35278333333333339</v>
+      </c>
+      <c r="U47" s="8">
+        <f t="shared" si="17"/>
+        <v>0.50383333333333324</v>
+      </c>
+      <c r="V47" s="9">
+        <f t="shared" si="18"/>
+        <v>0.37890000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48" s="40" t="s">
+        <v>119</v>
+      </c>
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
@@ -9051,7 +9385,10 @@
       <c r="U48" s="8"/>
       <c r="V48" s="9"/>
     </row>
-    <row r="49" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22">
+      <c r="A49" s="40" t="s">
+        <v>120</v>
+      </c>
       <c r="B49" s="7"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
@@ -9074,7 +9411,10 @@
       <c r="U49" s="8"/>
       <c r="V49" s="9"/>
     </row>
-    <row r="50" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:22">
+      <c r="A50" s="40" t="s">
+        <v>121</v>
+      </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
@@ -9097,7 +9437,10 @@
       <c r="U50" s="8"/>
       <c r="V50" s="9"/>
     </row>
-    <row r="51" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22">
+      <c r="A51" s="40" t="s">
+        <v>122</v>
+      </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
@@ -9120,26 +9463,124 @@
       <c r="U51" s="8"/>
       <c r="V51" s="9"/>
     </row>
+    <row r="52" spans="1:22">
+      <c r="A52" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="9"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="9"/>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B53" s="7"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="9"/>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="9"/>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="B55" s="7"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="8"/>
+      <c r="V55" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9149,9 +9590,9 @@
   <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9161,9 +9602,9 @@
   <conditionalFormatting sqref="J3:J10">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9173,9 +9614,9 @@
   <conditionalFormatting sqref="M3:M10">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9185,9 +9626,9 @@
   <conditionalFormatting sqref="P7:P10">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9197,57 +9638,57 @@
   <conditionalFormatting sqref="S7:S10">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V3:V55">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D55">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G55">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J55">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9257,9 +9698,9 @@
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9269,9 +9710,9 @@
   <conditionalFormatting sqref="M3:M16">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9281,9 +9722,9 @@
   <conditionalFormatting sqref="M3:M18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9293,9 +9734,9 @@
   <conditionalFormatting sqref="P7:P18">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9305,9 +9746,9 @@
   <conditionalFormatting sqref="S7:S18">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9317,9 +9758,9 @@
   <conditionalFormatting sqref="M4:M21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9329,9 +9770,9 @@
   <conditionalFormatting sqref="P4:P21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9341,45 +9782,45 @@
   <conditionalFormatting sqref="S4:S21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M55">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P55">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S51">
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S55">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9392,14 +9833,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -9416,7 +9857,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
@@ -9442,12 +9883,12 @@
       </c>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="27" t="s">
         <v>48</v>
@@ -9480,7 +9921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
         <v>46</v>
       </c>
@@ -9528,7 +9969,7 @@
         <v>1.0845751025000001</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="25" t="s">
         <v>47</v>
       </c>
@@ -9576,7 +10017,7 @@
         <v>1.3607243325</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="25" t="s">
         <v>50</v>
       </c>
@@ -9624,7 +10065,7 @@
         <v>1.1540821750000001</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="25" t="s">
         <v>51</v>
       </c>
@@ -9672,9 +10113,9 @@
         <v>1.4101859700000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B7" s="31">
         <v>0.76639999999999997</v>
@@ -9700,9 +10141,9 @@
       <c r="L7" s="7"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="31">
         <v>0.7651</v>
@@ -9714,9 +10155,9 @@
       <c r="L8" s="7"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="28">
         <v>0.76449999999999996</v>
@@ -9755,9 +10196,9 @@
         <v>0.942025</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>0.75980000000000003</v>
@@ -9792,9 +10233,9 @@
         <v>0.93303333333333338</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="30">
         <v>0.76670000000000005</v>
@@ -9823,9 +10264,9 @@
         <v>0.73710000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="30">
         <v>0.75880000000000003</v>
@@ -9854,9 +10295,9 @@
         <v>0.73635000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="30">
         <v>0.76100000000000001</v>
@@ -9897,13 +10338,13 @@
         <v>1.1484999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
     </row>
   </sheetData>
@@ -9918,9 +10359,9 @@
   <conditionalFormatting sqref="M3:M13">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -9930,9 +10371,9 @@
   <conditionalFormatting sqref="L3:L13">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9942,9 +10383,9 @@
   <conditionalFormatting sqref="B3:B6 B9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9954,9 +10395,9 @@
   <conditionalFormatting sqref="D3:D6 D9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9966,9 +10407,9 @@
   <conditionalFormatting sqref="F3:F6 F9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9978,9 +10419,9 @@
   <conditionalFormatting sqref="H3:H7 H9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -9990,9 +10431,9 @@
   <conditionalFormatting sqref="J3:J7 J9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10002,9 +10443,9 @@
   <conditionalFormatting sqref="C3:C6">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10014,9 +10455,9 @@
   <conditionalFormatting sqref="E3:E6">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10026,9 +10467,9 @@
   <conditionalFormatting sqref="G3:G7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10038,9 +10479,9 @@
   <conditionalFormatting sqref="I3:I6">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10050,9 +10491,9 @@
   <conditionalFormatting sqref="K3:K6">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10062,9 +10503,9 @@
   <conditionalFormatting sqref="B3:B13">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10074,9 +10515,9 @@
   <conditionalFormatting sqref="C3:C13">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10086,9 +10527,9 @@
   <conditionalFormatting sqref="D3:D13">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10098,9 +10539,9 @@
   <conditionalFormatting sqref="E3:E13">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10110,9 +10551,9 @@
   <conditionalFormatting sqref="F3:F13">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10122,9 +10563,9 @@
   <conditionalFormatting sqref="G3:G13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10134,9 +10575,9 @@
   <conditionalFormatting sqref="H3:H13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10146,9 +10587,9 @@
   <conditionalFormatting sqref="I3:I13">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10158,9 +10599,9 @@
   <conditionalFormatting sqref="J3:J13">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10170,9 +10611,9 @@
   <conditionalFormatting sqref="K3:K13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10185,14 +10626,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
@@ -10209,7 +10650,7 @@
     <col min="13" max="13" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="B1" s="36" t="s">
         <v>5</v>
       </c>
@@ -10235,12 +10676,12 @@
       </c>
       <c r="M1" s="35"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="B2" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>48</v>
@@ -10273,9 +10714,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="30">
         <v>0.65</v>
@@ -10316,13 +10757,13 @@
         <v>0.65325</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="1"/>
     </row>
   </sheetData>
@@ -10337,9 +10778,9 @@
   <conditionalFormatting sqref="M3">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10349,9 +10790,9 @@
   <conditionalFormatting sqref="L3">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10361,9 +10802,9 @@
   <conditionalFormatting sqref="B3">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10373,9 +10814,9 @@
   <conditionalFormatting sqref="C3">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10385,9 +10826,9 @@
   <conditionalFormatting sqref="D3">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10397,9 +10838,9 @@
   <conditionalFormatting sqref="E3">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10409,9 +10850,9 @@
   <conditionalFormatting sqref="F3">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10421,9 +10862,9 @@
   <conditionalFormatting sqref="G3">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10433,9 +10874,9 @@
   <conditionalFormatting sqref="H3">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10445,9 +10886,9 @@
   <conditionalFormatting sqref="I3">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10457,9 +10898,9 @@
   <conditionalFormatting sqref="J3">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -10469,9 +10910,9 @@
   <conditionalFormatting sqref="K3">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -10484,14 +10925,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="31" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -10500,7 +10941,7 @@
     <col min="38" max="40" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40">
       <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
@@ -10517,7 +10958,7 @@
       <c r="I1" s="34"/>
       <c r="J1" s="34"/>
       <c r="K1" s="36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L1" s="34"/>
       <c r="M1" s="34"/>
@@ -10527,7 +10968,7 @@
       <c r="O1" s="34"/>
       <c r="P1" s="34"/>
       <c r="Q1" s="36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R1" s="34"/>
       <c r="S1" s="35"/>
@@ -10547,7 +10988,7 @@
       <c r="AA1" s="34"/>
       <c r="AB1" s="35"/>
       <c r="AC1" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AD1" s="34"/>
       <c r="AE1" s="35"/>
@@ -10557,7 +10998,7 @@
       <c r="AG1" s="34"/>
       <c r="AH1" s="35"/>
       <c r="AI1" s="34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AJ1" s="34"/>
       <c r="AK1" s="35"/>
@@ -10567,7 +11008,7 @@
       <c r="AM1" s="34"/>
       <c r="AN1" s="35"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -10689,9 +11130,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40">
       <c r="A3" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="10">
         <v>0.38469999999999999</v>
@@ -10814,9 +11255,9 @@
         <v>0.45634545454545455</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="10">
         <v>0.56200000000000006</v>
@@ -10939,9 +11380,9 @@
         <v>0.49341818181818181</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="10">
         <v>0.27739999999999998</v>
@@ -11064,9 +11505,9 @@
         <v>0.4236454545454546</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40">
       <c r="A6" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" s="10">
         <v>0.3236</v>
@@ -11189,7 +11630,7 @@
         <v>0.51095454545454555</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40">
       <c r="A7" s="5"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
@@ -11231,7 +11672,7 @@
       <c r="AM7" s="11"/>
       <c r="AN7" s="12"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40">
       <c r="A8" s="5"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -11273,7 +11714,7 @@
       <c r="AM8" s="11"/>
       <c r="AN8" s="12"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40">
       <c r="A9" s="5"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -11334,9 +11775,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="63">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11346,9 +11787,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="62">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11358,9 +11799,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="61">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11370,9 +11811,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="60">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11382,9 +11823,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="59">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11394,9 +11835,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="58">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11406,9 +11847,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="57">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11418,9 +11859,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="56">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11430,9 +11871,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="55">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11442,9 +11883,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="54">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11454,9 +11895,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="53">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11466,9 +11907,9 @@
   <conditionalFormatting sqref="AN3:AN9">
     <cfRule type="colorScale" priority="52">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11478,9 +11919,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="51">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11490,9 +11931,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="50">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11502,9 +11943,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11514,9 +11955,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="48">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11526,9 +11967,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="47">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11538,9 +11979,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="46">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11550,9 +11991,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="45">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11562,9 +12003,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="44">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11574,9 +12015,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="43">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11586,9 +12027,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="42">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11598,9 +12039,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="41">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11610,9 +12051,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="40">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11622,9 +12063,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="39">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11634,9 +12075,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="38">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11646,9 +12087,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="37">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11658,9 +12099,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="36">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11670,9 +12111,9 @@
   <conditionalFormatting sqref="AE4:AE9">
     <cfRule type="colorScale" priority="35">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11682,9 +12123,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="34">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11694,9 +12135,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="33">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11706,9 +12147,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="32">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11718,9 +12159,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="31">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11730,9 +12171,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="30">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11742,9 +12183,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="29">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11754,9 +12195,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="28">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11766,9 +12207,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="27">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11778,9 +12219,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="26">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11790,9 +12231,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="25">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11802,9 +12243,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="24">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11814,9 +12255,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="23">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11826,9 +12267,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="22">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11838,9 +12279,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="21">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11850,9 +12291,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11862,9 +12303,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11874,9 +12315,9 @@
   <conditionalFormatting sqref="AK3:AK9">
     <cfRule type="colorScale" priority="18">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11886,9 +12327,9 @@
   <conditionalFormatting sqref="AH3:AH9">
     <cfRule type="colorScale" priority="17">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11898,9 +12339,9 @@
   <conditionalFormatting sqref="AE3:AE9">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11910,9 +12351,9 @@
   <conditionalFormatting sqref="AB3:AB9">
     <cfRule type="colorScale" priority="15">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11922,9 +12363,9 @@
   <conditionalFormatting sqref="Y3:Y9">
     <cfRule type="colorScale" priority="14">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11934,9 +12375,9 @@
   <conditionalFormatting sqref="V3:V9">
     <cfRule type="colorScale" priority="13">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11946,9 +12387,9 @@
   <conditionalFormatting sqref="S3:S9">
     <cfRule type="colorScale" priority="12">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11958,9 +12399,9 @@
   <conditionalFormatting sqref="P3:P9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11970,9 +12411,9 @@
   <conditionalFormatting sqref="J3:J9">
     <cfRule type="colorScale" priority="10">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11982,9 +12423,9 @@
   <conditionalFormatting sqref="G3:G9">
     <cfRule type="colorScale" priority="9">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -11994,9 +12435,9 @@
   <conditionalFormatting sqref="D3:D9">
     <cfRule type="colorScale" priority="8">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12006,9 +12447,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="7">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12018,9 +12459,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="6">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12030,9 +12471,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="5">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12042,9 +12483,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12054,9 +12495,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="3">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12066,9 +12507,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
@@ -12078,9 +12519,9 @@
   <conditionalFormatting sqref="M3:M9">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>

<commit_message>
More results, cleverer sampling.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="130">
   <si>
     <t>DEVEL</t>
   </si>
@@ -402,6 +402,12 @@
   </si>
   <si>
     <t>BP4D SVM dynamic, caelum 101</t>
+  </si>
+  <si>
+    <t>SVM static rebalanced (c104)</t>
+  </si>
+  <si>
+    <t>SVM dynamic rebalanced (c104)</t>
   </si>
 </sst>
 </file>
@@ -611,6 +617,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -622,13 +635,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -932,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -943,66 +949,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="36" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="36" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="36" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="34"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="36" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="36" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="34"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="36" t="s">
+      <c r="U1" s="37"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="36" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="36" t="s">
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="34" t="s">
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="34" t="s">
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="35"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="38"/>
     </row>
     <row r="2" spans="1:37">
       <c r="A2" t="s">
@@ -6300,56 +6306,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="36" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="O1" s="34"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="36" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="36" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="34"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="40"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
+      <c r="AA1" s="40"/>
+      <c r="AB1" s="40"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
     </row>
     <row r="2" spans="1:34">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -6417,7 +6423,7 @@
       </c>
     </row>
     <row r="3" spans="1:34" ht="17.25" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="10">
@@ -6476,7 +6482,7 @@
       </c>
     </row>
     <row r="4" spans="1:34">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="10">
@@ -6535,7 +6541,7 @@
       </c>
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="35" t="s">
         <v>59</v>
       </c>
       <c r="B5" s="10">
@@ -6594,7 +6600,7 @@
       </c>
     </row>
     <row r="6" spans="1:34" ht="15" customHeight="1">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="35" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="10">
@@ -6653,7 +6659,7 @@
       </c>
     </row>
     <row r="7" spans="1:34">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="35" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="10">
@@ -6724,7 +6730,7 @@
       </c>
     </row>
     <row r="8" spans="1:34">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="15">
@@ -6795,7 +6801,7 @@
       </c>
     </row>
     <row r="9" spans="1:34">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="7">
@@ -6866,7 +6872,7 @@
       </c>
     </row>
     <row r="10" spans="1:34">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="35" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="7">
@@ -6937,7 +6943,7 @@
       </c>
     </row>
     <row r="11" spans="1:34">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="35" t="s">
         <v>40</v>
       </c>
       <c r="B11" s="7">
@@ -6990,7 +6996,7 @@
       </c>
     </row>
     <row r="12" spans="1:34">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="35" t="s">
         <v>41</v>
       </c>
       <c r="B12" s="7">
@@ -7043,7 +7049,7 @@
       </c>
     </row>
     <row r="13" spans="1:34">
-      <c r="A13" s="39" t="s">
+      <c r="A13" s="35" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="7">
@@ -7096,7 +7102,7 @@
       </c>
     </row>
     <row r="14" spans="1:34">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B14" s="7">
@@ -7149,7 +7155,7 @@
       </c>
     </row>
     <row r="15" spans="1:34">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="35" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="7">
@@ -7208,7 +7214,7 @@
       </c>
     </row>
     <row r="16" spans="1:34">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="36" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="7">
@@ -7267,7 +7273,7 @@
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="7">
@@ -7338,7 +7344,7 @@
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="36" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="7">
@@ -7409,7 +7415,7 @@
       </c>
     </row>
     <row r="19" spans="1:22">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="35" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="7">
@@ -7480,7 +7486,7 @@
       </c>
     </row>
     <row r="20" spans="1:22">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="35" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="7">
@@ -7551,7 +7557,7 @@
       </c>
     </row>
     <row r="21" spans="1:22">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="7">
@@ -7622,7 +7628,7 @@
       </c>
     </row>
     <row r="22" spans="1:22">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="35" t="s">
         <v>62</v>
       </c>
       <c r="B22" s="7">
@@ -7693,7 +7699,7 @@
       </c>
     </row>
     <row r="23" spans="1:22">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B23" s="7">
@@ -7764,7 +7770,7 @@
       </c>
     </row>
     <row r="24" spans="1:22">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="35" t="s">
         <v>64</v>
       </c>
       <c r="B24" s="7">
@@ -7835,7 +7841,7 @@
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="35" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="7">
@@ -7894,7 +7900,7 @@
       </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="35" t="s">
         <v>73</v>
       </c>
       <c r="B26" s="7">
@@ -7953,7 +7959,7 @@
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B27" s="7">
@@ -8024,7 +8030,7 @@
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="35" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="7">
@@ -8095,7 +8101,7 @@
       </c>
     </row>
     <row r="29" spans="1:22">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="36" t="s">
         <v>84</v>
       </c>
       <c r="B29" s="7">
@@ -8154,7 +8160,7 @@
       </c>
     </row>
     <row r="30" spans="1:22">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="36" t="s">
         <v>80</v>
       </c>
       <c r="B30" s="7">
@@ -8213,7 +8219,7 @@
       </c>
     </row>
     <row r="31" spans="1:22">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="36" t="s">
         <v>81</v>
       </c>
       <c r="B31" s="7">
@@ -8266,7 +8272,7 @@
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="36" t="s">
         <v>82</v>
       </c>
       <c r="B32" s="7">
@@ -8319,7 +8325,7 @@
       </c>
     </row>
     <row r="33" spans="1:22">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="36" t="s">
         <v>85</v>
       </c>
       <c r="B33" s="7">
@@ -8378,7 +8384,7 @@
       </c>
     </row>
     <row r="34" spans="1:22">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="36" t="s">
         <v>86</v>
       </c>
       <c r="B34" s="7">
@@ -8437,7 +8443,7 @@
       </c>
     </row>
     <row r="35" spans="1:22">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="36" t="s">
         <v>112</v>
       </c>
       <c r="B35" s="7">
@@ -8508,7 +8514,7 @@
       </c>
     </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="40" t="s">
+      <c r="A36" s="36" t="s">
         <v>101</v>
       </c>
       <c r="B36" s="7">
@@ -8579,7 +8585,7 @@
       </c>
     </row>
     <row r="37" spans="1:22">
-      <c r="A37" s="40" t="s">
+      <c r="A37" s="36" t="s">
         <v>100</v>
       </c>
       <c r="B37" s="7">
@@ -8650,7 +8656,7 @@
       </c>
     </row>
     <row r="38" spans="1:22">
-      <c r="A38" s="40" t="s">
+      <c r="A38" s="36" t="s">
         <v>102</v>
       </c>
       <c r="B38" s="7">
@@ -8721,7 +8727,7 @@
       </c>
     </row>
     <row r="39" spans="1:22">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="36" t="s">
         <v>103</v>
       </c>
       <c r="B39" s="7">
@@ -8792,7 +8798,7 @@
       </c>
     </row>
     <row r="40" spans="1:22">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="36" t="s">
         <v>106</v>
       </c>
       <c r="B40" s="7">
@@ -8863,7 +8869,7 @@
       </c>
     </row>
     <row r="41" spans="1:22">
-      <c r="A41" s="40" t="s">
+      <c r="A41" s="36" t="s">
         <v>107</v>
       </c>
       <c r="B41" s="7">
@@ -8934,7 +8940,7 @@
       </c>
     </row>
     <row r="42" spans="1:22">
-      <c r="A42" s="40" t="s">
+      <c r="A42" s="36" t="s">
         <v>109</v>
       </c>
       <c r="B42" s="7">
@@ -9005,7 +9011,7 @@
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="36" t="s">
         <v>111</v>
       </c>
       <c r="B43" s="7">
@@ -9076,7 +9082,7 @@
       </c>
     </row>
     <row r="44" spans="1:22">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="36" t="s">
         <v>114</v>
       </c>
       <c r="B44" s="7">
@@ -9147,7 +9153,7 @@
       </c>
     </row>
     <row r="45" spans="1:22">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="36" t="s">
         <v>116</v>
       </c>
       <c r="B45" s="7">
@@ -9218,7 +9224,7 @@
       </c>
     </row>
     <row r="46" spans="1:22">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="36" t="s">
         <v>117</v>
       </c>
       <c r="B46" s="7">
@@ -9289,7 +9295,7 @@
       </c>
     </row>
     <row r="47" spans="1:22">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="36" t="s">
         <v>118</v>
       </c>
       <c r="B47" s="7">
@@ -9360,7 +9366,7 @@
       </c>
     </row>
     <row r="48" spans="1:22">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="36" t="s">
         <v>119</v>
       </c>
       <c r="B48" s="7"/>
@@ -9386,7 +9392,7 @@
       <c r="V48" s="9"/>
     </row>
     <row r="49" spans="1:22">
-      <c r="A49" s="40" t="s">
+      <c r="A49" s="36" t="s">
         <v>120</v>
       </c>
       <c r="B49" s="7"/>
@@ -9412,7 +9418,7 @@
       <c r="V49" s="9"/>
     </row>
     <row r="50" spans="1:22">
-      <c r="A50" s="40" t="s">
+      <c r="A50" s="36" t="s">
         <v>121</v>
       </c>
       <c r="B50" s="7"/>
@@ -9438,7 +9444,7 @@
       <c r="V50" s="9"/>
     </row>
     <row r="51" spans="1:22">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="36" t="s">
         <v>122</v>
       </c>
       <c r="B51" s="7"/>
@@ -9464,7 +9470,7 @@
       <c r="V51" s="9"/>
     </row>
     <row r="52" spans="1:22">
-      <c r="A52" s="40" t="s">
+      <c r="A52" s="36" t="s">
         <v>123</v>
       </c>
       <c r="B52" s="7"/>
@@ -9490,7 +9496,7 @@
       <c r="V52" s="9"/>
     </row>
     <row r="53" spans="1:22">
-      <c r="A53" s="40" t="s">
+      <c r="A53" s="36" t="s">
         <v>124</v>
       </c>
       <c r="B53" s="7"/>
@@ -9563,17 +9569,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="21">
@@ -9858,30 +9864,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="36" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="35"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="27" t="s">
@@ -10651,30 +10657,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="37"/>
+      <c r="F1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="36" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="36" t="s">
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="35"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="33" t="s">
@@ -10928,13 +10934,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="31" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="34" width="4.5703125" customWidth="1"/>
     <col min="35" max="37" width="4.5703125" bestFit="1" customWidth="1"/>
@@ -10942,71 +10948,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="36" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="36" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="36" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="36" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="R1" s="34"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="36" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="U1" s="34"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="36" t="s">
+      <c r="U1" s="37"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="34"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="36" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="34"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="36" t="s">
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="36" t="s">
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="AG1" s="34"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="34" t="s">
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="AJ1" s="34"/>
-      <c r="AK1" s="35"/>
-      <c r="AL1" s="34" t="s">
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="AM1" s="34"/>
-      <c r="AN1" s="35"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="38"/>
     </row>
     <row r="2" spans="1:40">
       <c r="A2" t="s">
@@ -11630,8 +11636,10 @@
         <v>0.51095454545454555</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:40" ht="23.25">
+      <c r="A7" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="B7" s="10"/>
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
@@ -11673,7 +11681,9 @@
       <c r="AN7" s="12"/>
     </row>
     <row r="8" spans="1:40">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
       <c r="D8" s="12"/>

</xml_diff>

<commit_message>
Intensity underampling (helps), together with attmpted synthetic gen and undersampling results.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
     <sheet name="SEMAINE" sheetId="2" r:id="rId2"/>
-    <sheet name="BP4D_intensity" sheetId="3" r:id="rId3"/>
-    <sheet name="BP4D_int_seg" sheetId="5" r:id="rId4"/>
-    <sheet name="DISFA" sheetId="4" r:id="rId5"/>
+    <sheet name="DISFA" sheetId="4" r:id="rId3"/>
+    <sheet name="BP4D_intensity" sheetId="3" r:id="rId4"/>
+    <sheet name="BP4D_int_seg" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="133">
   <si>
     <t>DEVEL</t>
   </si>
@@ -398,16 +398,25 @@
     <t>AU28</t>
   </si>
   <si>
-    <t>BP4D SVM static, caelum 101</t>
-  </si>
-  <si>
-    <t>BP4D SVM dynamic, caelum 101</t>
-  </si>
-  <si>
-    <t>SVM static rebalanced (c104)</t>
-  </si>
-  <si>
-    <t>SVM dynamic rebalanced (c104)</t>
+    <t>SVM static rebalanced</t>
+  </si>
+  <si>
+    <t>SVM dynamic rebalanced</t>
+  </si>
+  <si>
+    <t>App, geom old undersampling, 1-1 dynamic clever</t>
+  </si>
+  <si>
+    <t>App, geom old undersampling, 1-1 static clever</t>
+  </si>
+  <si>
+    <t>BP4D SVM static</t>
+  </si>
+  <si>
+    <t>BP4D SVM static clever sampling</t>
+  </si>
+  <si>
+    <t>SVM appearance balanced</t>
   </si>
 </sst>
 </file>
@@ -938,7 +947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
@@ -5172,99 +5181,249 @@
         <v>0.43830000000000002</v>
       </c>
       <c r="AI42" s="10">
-        <f t="shared" ref="AI42" si="18">AVERAGE(B42,E42,H42,K42,N42,Q42,T42,W42,Z42,AC42,AF42)</f>
+        <f t="shared" ref="AI42:AI44" si="18">AVERAGE(B42,E42,H42,K42,N42,Q42,T42,W42,Z42,AC42,AF42)</f>
         <v>0.55155454545454552</v>
       </c>
       <c r="AJ42" s="11">
-        <f t="shared" ref="AJ42" si="19">AVERAGE(C42,F42,I42,L42,O42,R42,U42,X42,AA42,AD42,AG42)</f>
+        <f t="shared" ref="AJ42:AJ44" si="19">AVERAGE(C42,F42,I42,L42,O42,R42,U42,X42,AA42,AD42,AG42)</f>
         <v>0.67960909090909094</v>
       </c>
       <c r="AK42" s="12">
-        <f t="shared" ref="AK42" si="20">AVERAGE(D42,G42,J42,M42,P42,S42,V42,Y42,AB42,AE42,AH42)</f>
+        <f t="shared" ref="AK42:AK44" si="20">AVERAGE(D42,G42,J42,M42,P42,S42,V42,Y42,AB42,AE42,AH42)</f>
         <v>0.59669090909090905</v>
       </c>
     </row>
     <row r="43" spans="1:37">
       <c r="A43" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="8"/>
-      <c r="S43" s="8"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="8"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="7"/>
-      <c r="X43" s="8"/>
-      <c r="Y43" s="8"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="8"/>
-      <c r="AB43" s="8"/>
-      <c r="AC43" s="7"/>
-      <c r="AD43" s="8"/>
-      <c r="AE43" s="8"/>
-      <c r="AF43" s="7"/>
-      <c r="AG43" s="8"/>
-      <c r="AH43" s="9"/>
-      <c r="AI43" s="10"/>
-      <c r="AJ43" s="11"/>
-      <c r="AK43" s="12"/>
+        <v>130</v>
+      </c>
+      <c r="B43" s="7">
+        <v>0.35349999999999998</v>
+      </c>
+      <c r="C43" s="8">
+        <v>0.50480000000000003</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.4158</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.2913</v>
+      </c>
+      <c r="F43" s="8">
+        <v>0.43640000000000001</v>
+      </c>
+      <c r="G43" s="9">
+        <v>0.34939999999999999</v>
+      </c>
+      <c r="H43" s="7">
+        <v>0.34720000000000001</v>
+      </c>
+      <c r="I43" s="8">
+        <v>0.59030000000000005</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="K43" s="7">
+        <v>0.7863</v>
+      </c>
+      <c r="L43" s="8">
+        <v>0.75160000000000005</v>
+      </c>
+      <c r="M43" s="8">
+        <v>0.76849999999999996</v>
+      </c>
+      <c r="N43" s="7">
+        <v>0.74970000000000003</v>
+      </c>
+      <c r="O43" s="8">
+        <v>0.75439999999999996</v>
+      </c>
+      <c r="P43" s="8">
+        <v>0.75439999999999996</v>
+      </c>
+      <c r="Q43" s="7">
+        <v>0.8619</v>
+      </c>
+      <c r="R43" s="8">
+        <v>0.83069999999999999</v>
+      </c>
+      <c r="S43" s="8">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="T43" s="7">
+        <v>0.87939999999999996</v>
+      </c>
+      <c r="U43" s="8">
+        <v>0.84860000000000002</v>
+      </c>
+      <c r="V43" s="8">
+        <v>0.86370000000000002</v>
+      </c>
+      <c r="W43" s="7">
+        <v>0.60760000000000003</v>
+      </c>
+      <c r="X43" s="8">
+        <v>0.74729999999999996</v>
+      </c>
+      <c r="Y43" s="8">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="Z43" s="7">
+        <v>0.31309999999999999</v>
+      </c>
+      <c r="AA43" s="8">
+        <v>0.70369999999999999</v>
+      </c>
+      <c r="AB43" s="8">
+        <v>0.43340000000000001</v>
+      </c>
+      <c r="AC43" s="7">
+        <v>0.5262</v>
+      </c>
+      <c r="AD43" s="8">
+        <v>0.75609999999999999</v>
+      </c>
+      <c r="AE43" s="8">
+        <v>0.62050000000000005</v>
+      </c>
+      <c r="AF43" s="7">
+        <v>0.3347</v>
+      </c>
+      <c r="AG43" s="8">
+        <v>0.62039999999999995</v>
+      </c>
+      <c r="AH43" s="9">
+        <v>0.43480000000000002</v>
+      </c>
+      <c r="AI43" s="10">
+        <f t="shared" si="18"/>
+        <v>0.55008181818181812</v>
+      </c>
+      <c r="AJ43" s="11">
+        <f t="shared" si="19"/>
+        <v>0.68584545454545454</v>
+      </c>
+      <c r="AK43" s="12">
+        <f t="shared" si="20"/>
+        <v>0.59946363636363642</v>
+      </c>
     </row>
     <row r="44" spans="1:37">
       <c r="A44" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="8"/>
-      <c r="S44" s="8"/>
-      <c r="T44" s="7"/>
-      <c r="U44" s="8"/>
-      <c r="V44" s="8"/>
-      <c r="W44" s="7"/>
-      <c r="X44" s="8"/>
-      <c r="Y44" s="8"/>
-      <c r="Z44" s="7"/>
-      <c r="AA44" s="8"/>
-      <c r="AB44" s="8"/>
-      <c r="AC44" s="7"/>
-      <c r="AD44" s="8"/>
-      <c r="AE44" s="8"/>
-      <c r="AF44" s="7"/>
-      <c r="AG44" s="8"/>
-      <c r="AH44" s="9"/>
-      <c r="AI44" s="10"/>
-      <c r="AJ44" s="11"/>
-      <c r="AK44" s="12"/>
+        <v>131</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0.35470000000000002</v>
+      </c>
+      <c r="C44" s="8">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.42080000000000001</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="F44" s="8">
+        <v>0.39250000000000002</v>
+      </c>
+      <c r="G44" s="9">
+        <v>0.3392</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0.3604</v>
+      </c>
+      <c r="I44" s="8">
+        <v>0.57489999999999997</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0.44309999999999999</v>
+      </c>
+      <c r="K44" s="7">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="L44" s="8">
+        <v>0.77690000000000003</v>
+      </c>
+      <c r="M44" s="8">
+        <v>0.76880000000000004</v>
+      </c>
+      <c r="N44" s="7">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="O44" s="8">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="P44" s="8">
+        <v>0.77010000000000001</v>
+      </c>
+      <c r="Q44" s="7">
+        <v>0.86809999999999998</v>
+      </c>
+      <c r="R44" s="8">
+        <v>0.83430000000000004</v>
+      </c>
+      <c r="S44" s="8">
+        <v>0.85089999999999999</v>
+      </c>
+      <c r="T44" s="7">
+        <v>0.87450000000000006</v>
+      </c>
+      <c r="U44" s="8">
+        <v>0.86150000000000004</v>
+      </c>
+      <c r="V44" s="8">
+        <v>0.86799999999999999</v>
+      </c>
+      <c r="W44" s="7">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="X44" s="8">
+        <v>0.80069999999999997</v>
+      </c>
+      <c r="Y44" s="8">
+        <v>0.66869999999999996</v>
+      </c>
+      <c r="Z44" s="7">
+        <v>0.3216</v>
+      </c>
+      <c r="AA44" s="8">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="AB44" s="8">
+        <v>0.43580000000000002</v>
+      </c>
+      <c r="AC44" s="7">
+        <v>0.52110000000000001</v>
+      </c>
+      <c r="AD44" s="8">
+        <v>0.76559999999999995</v>
+      </c>
+      <c r="AE44" s="8">
+        <v>0.62009999999999998</v>
+      </c>
+      <c r="AF44" s="7">
+        <v>0.33090000000000003</v>
+      </c>
+      <c r="AG44" s="8">
+        <v>0.65839999999999999</v>
+      </c>
+      <c r="AH44" s="9">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="AI44" s="10">
+        <f t="shared" si="18"/>
+        <v>0.54608181818181822</v>
+      </c>
+      <c r="AJ44" s="11">
+        <f t="shared" si="19"/>
+        <v>0.69619090909090919</v>
+      </c>
+      <c r="AK44" s="12">
+        <f t="shared" si="20"/>
+        <v>0.60235454545454559</v>
+      </c>
     </row>
     <row r="45" spans="1:37">
       <c r="B45" s="7"/>
@@ -5887,7 +6046,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J25 X29:X47 J27:J47">
+  <conditionalFormatting sqref="J3:J25 J27:J47 X44:X47">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -6278,10 +6437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH55"/>
+  <dimension ref="A1:AH56"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9140,15 +9299,15 @@
         <v>0.42049999999999998</v>
       </c>
       <c r="T44" s="7">
-        <f t="shared" ref="T44:T47" si="16">AVERAGE(B44,E44,H44,K44,N44,Q44)</f>
+        <f t="shared" ref="T44:T49" si="16">AVERAGE(B44,E44,H44,K44,N44,Q44)</f>
         <v>0.47588333333333338</v>
       </c>
       <c r="U44" s="8">
-        <f t="shared" ref="U44:U47" si="17">AVERAGE(C44,F44,I44,L44,O44,R44)</f>
+        <f t="shared" ref="U44:U49" si="17">AVERAGE(C44,F44,I44,L44,O44,R44)</f>
         <v>0.52179999999999993</v>
       </c>
       <c r="V44" s="9">
-        <f t="shared" ref="V44:V47" si="18">AVERAGE(D44,G44,J44,M44,P44,S44)</f>
+        <f t="shared" ref="V44:V49" si="18">AVERAGE(D44,G44,J44,M44,P44,S44)</f>
         <v>0.4806333333333333</v>
       </c>
     </row>
@@ -9367,59 +9526,149 @@
     </row>
     <row r="48" spans="1:22">
       <c r="A48" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="7"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="7"/>
-      <c r="R48" s="8"/>
-      <c r="S48" s="9"/>
-      <c r="T48" s="7"/>
-      <c r="U48" s="8"/>
-      <c r="V48" s="9"/>
+        <v>128</v>
+      </c>
+      <c r="B48" s="7">
+        <v>0.47370000000000001</v>
+      </c>
+      <c r="C48" s="8">
+        <v>0.69130000000000003</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.56220000000000003</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.58450000000000002</v>
+      </c>
+      <c r="F48" s="8">
+        <v>0.63139999999999996</v>
+      </c>
+      <c r="G48" s="9">
+        <v>0.60709999999999997</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0.37940000000000002</v>
+      </c>
+      <c r="I48" s="8">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="J48" s="9">
+        <v>0.43590000000000001</v>
+      </c>
+      <c r="K48" s="7">
+        <v>0.43480000000000002</v>
+      </c>
+      <c r="L48" s="8">
+        <v>0.60740000000000005</v>
+      </c>
+      <c r="M48" s="9">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="N48" s="7">
+        <v>0.50939999999999996</v>
+      </c>
+      <c r="O48" s="8">
+        <v>0.34150000000000003</v>
+      </c>
+      <c r="P48" s="9">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="Q48" s="7">
+        <v>0.30520000000000003</v>
+      </c>
+      <c r="R48" s="8">
+        <v>0.68610000000000004</v>
+      </c>
+      <c r="S48" s="9">
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="T48" s="7">
+        <f t="shared" si="16"/>
+        <v>0.44783333333333336</v>
+      </c>
+      <c r="U48" s="8">
+        <f t="shared" si="17"/>
+        <v>0.57828333333333337</v>
+      </c>
+      <c r="V48" s="9">
+        <f t="shared" si="18"/>
+        <v>0.49058333333333332</v>
+      </c>
     </row>
     <row r="49" spans="1:22">
       <c r="A49" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="9"/>
-      <c r="N49" s="7"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="9"/>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="8"/>
-      <c r="S49" s="9"/>
-      <c r="T49" s="7"/>
-      <c r="U49" s="8"/>
-      <c r="V49" s="9"/>
+        <v>129</v>
+      </c>
+      <c r="B49" s="7">
+        <v>0.27379999999999999</v>
+      </c>
+      <c r="C49" s="8">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.33210000000000001</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.51170000000000004</v>
+      </c>
+      <c r="F49" s="8">
+        <v>0.68869999999999998</v>
+      </c>
+      <c r="G49" s="9">
+        <v>0.58720000000000006</v>
+      </c>
+      <c r="H49" s="7">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="I49" s="8">
+        <v>0.3034</v>
+      </c>
+      <c r="J49" s="9">
+        <v>0.1447</v>
+      </c>
+      <c r="K49" s="7">
+        <v>0.37069999999999997</v>
+      </c>
+      <c r="L49" s="8">
+        <v>0.5706</v>
+      </c>
+      <c r="M49" s="9">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="N49" s="7">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="O49" s="8">
+        <v>0.44569999999999999</v>
+      </c>
+      <c r="P49" s="9">
+        <v>0.47389999999999999</v>
+      </c>
+      <c r="Q49" s="7">
+        <v>0.24490000000000001</v>
+      </c>
+      <c r="R49" s="8">
+        <v>0.7218</v>
+      </c>
+      <c r="S49" s="9">
+        <v>0.36570000000000003</v>
+      </c>
+      <c r="T49" s="7">
+        <f t="shared" si="16"/>
+        <v>0.33368333333333333</v>
+      </c>
+      <c r="U49" s="8">
+        <f t="shared" si="17"/>
+        <v>0.52538333333333342</v>
+      </c>
+      <c r="V49" s="9">
+        <f t="shared" si="18"/>
+        <v>0.39218333333333333</v>
+      </c>
     </row>
     <row r="50" spans="1:22">
       <c r="A50" s="36" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
@@ -9445,7 +9694,7 @@
     </row>
     <row r="51" spans="1:22">
       <c r="A51" s="36" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="8"/>
@@ -9471,7 +9720,7 @@
     </row>
     <row r="52" spans="1:22">
       <c r="A52" s="36" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
@@ -9497,7 +9746,7 @@
     </row>
     <row r="53" spans="1:22">
       <c r="A53" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="8"/>
@@ -9522,6 +9771,9 @@
       <c r="V53" s="9"/>
     </row>
     <row r="54" spans="1:22">
+      <c r="A54" s="36" t="s">
+        <v>123</v>
+      </c>
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="9"/>
@@ -9545,6 +9797,9 @@
       <c r="V54" s="9"/>
     </row>
     <row r="55" spans="1:22">
+      <c r="A55" s="36" t="s">
+        <v>124</v>
+      </c>
       <c r="B55" s="7"/>
       <c r="C55" s="8"/>
       <c r="D55" s="9"/>
@@ -9567,6 +9822,29 @@
       <c r="U55" s="8"/>
       <c r="V55" s="9"/>
     </row>
+    <row r="56" spans="1:22">
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="9"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="8"/>
+      <c r="V56" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="Q1:S1"/>
@@ -9653,54 +9931,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V3:V55">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D55">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G55">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J55">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="M3:M15">
     <cfRule type="colorScale" priority="11">
       <colorScale>
@@ -9797,32 +10027,80 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M55">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P55">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S3:S55">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="V3:V56">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D56">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G56">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J56">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M56">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P56">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S3:S56">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -9840,1102 +10118,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:AN9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="B1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="38"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="B2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0.76639999999999997</v>
-      </c>
-      <c r="C3" s="9">
-        <f>0.9145*0.9145</f>
-        <v>0.83631024999999992</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0.74380000000000002</v>
-      </c>
-      <c r="E3" s="9">
-        <f>1.004*1.004</f>
-        <v>1.008016</v>
-      </c>
-      <c r="F3" s="7">
-        <v>0.8518</v>
-      </c>
-      <c r="G3" s="9">
-        <f>0.8217*0.8217</f>
-        <v>0.67519088999999999</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0.53010000000000002</v>
-      </c>
-      <c r="I3" s="9">
-        <f>1.2034*1.2034</f>
-        <v>1.44817156</v>
-      </c>
-      <c r="J3" s="7">
-        <v>0.49890000000000001</v>
-      </c>
-      <c r="K3" s="8">
-        <f>1.0986*1.0986</f>
-        <v>1.2069219600000001</v>
-      </c>
-      <c r="L3" s="7">
-        <f t="shared" ref="L3:M6" si="0">AVERAGE(D3,F3,H3,J3)</f>
-        <v>0.65615000000000001</v>
-      </c>
-      <c r="M3" s="9">
-        <f t="shared" si="0"/>
-        <v>1.0845751025000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0.74750000000000005</v>
-      </c>
-      <c r="C4" s="9">
-        <f>1.0015*1.0015</f>
-        <v>1.0030022500000002</v>
-      </c>
-      <c r="D4" s="7">
-        <v>0.60819999999999996</v>
-      </c>
-      <c r="E4" s="9">
-        <f>1.2472 *1.2472</f>
-        <v>1.5555078400000002</v>
-      </c>
-      <c r="F4" s="7">
-        <v>0.7742</v>
-      </c>
-      <c r="G4" s="9">
-        <f>1.0482*1.0482</f>
-        <v>1.09872324</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0.4163</v>
-      </c>
-      <c r="I4" s="9">
-        <f>1.4015*1.4015</f>
-        <v>1.9642022499999998</v>
-      </c>
-      <c r="J4" s="7">
-        <v>0.51639999999999997</v>
-      </c>
-      <c r="K4" s="8">
-        <f>0.908*0.908</f>
-        <v>0.82446400000000009</v>
-      </c>
-      <c r="L4" s="7">
-        <f t="shared" si="0"/>
-        <v>0.57877500000000004</v>
-      </c>
-      <c r="M4" s="9">
-        <f t="shared" si="0"/>
-        <v>1.3607243325</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="7">
-        <v>0.73160000000000003</v>
-      </c>
-      <c r="C5" s="9">
-        <f>0.9703*0.9703</f>
-        <v>0.94148209000000005</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0.7097</v>
-      </c>
-      <c r="E5" s="9">
-        <f>1.0558*1.0558</f>
-        <v>1.1147136400000002</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0.83860000000000001</v>
-      </c>
-      <c r="G5" s="9">
-        <f>0.8519*0.8519</f>
-        <v>0.72573361000000003</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0.50409999999999999</v>
-      </c>
-      <c r="I5" s="9">
-        <f>1.2313*1.2313</f>
-        <v>1.5160996900000001</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="K5" s="9">
-        <f>1.1224*1.1224</f>
-        <v>1.2597817600000001</v>
-      </c>
-      <c r="L5" s="7">
-        <f t="shared" si="0"/>
-        <v>0.63485000000000003</v>
-      </c>
-      <c r="M5" s="9">
-        <f t="shared" si="0"/>
-        <v>1.1540821750000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="7">
-        <v>0.71699999999999997</v>
-      </c>
-      <c r="C6" s="9">
-        <f>1.0332 * 1.0332</f>
-        <v>1.0675022399999998</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.5756</v>
-      </c>
-      <c r="E6" s="9">
-        <f>1.2736*1.2736</f>
-        <v>1.6220569600000001</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0.75049999999999994</v>
-      </c>
-      <c r="G6" s="9">
-        <f>1.0584*1.0584</f>
-        <v>1.1202105600000001</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0.38679999999999998</v>
-      </c>
-      <c r="I6" s="9">
-        <f>1.403*1.403</f>
-        <v>1.9684090000000001</v>
-      </c>
-      <c r="J6" s="7">
-        <v>0.43230000000000002</v>
-      </c>
-      <c r="K6" s="9">
-        <f>0.9644*0.9644</f>
-        <v>0.93006736000000012</v>
-      </c>
-      <c r="L6" s="7">
-        <f t="shared" si="0"/>
-        <v>0.5363</v>
-      </c>
-      <c r="M6" s="9">
-        <f t="shared" si="0"/>
-        <v>1.4101859700000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="31">
-        <v>0.76639999999999997</v>
-      </c>
-      <c r="C7">
-        <f>0.9145*0.9145</f>
-        <v>0.83631024999999992</v>
-      </c>
-      <c r="D7" s="31">
-        <v>0.74380000000000002</v>
-      </c>
-      <c r="E7">
-        <f>1.004*1.004</f>
-        <v>1.008016</v>
-      </c>
-      <c r="F7" s="31">
-        <v>0.8518</v>
-      </c>
-      <c r="G7">
-        <f>0.8217*0.8217</f>
-        <v>0.67519088999999999</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="31">
-        <v>0.7651</v>
-      </c>
-      <c r="C8">
-        <f>0.934*0.934</f>
-        <v>0.87235600000000013</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="28">
-        <v>0.76449999999999996</v>
-      </c>
-      <c r="C9">
-        <v>0.80910000000000004</v>
-      </c>
-      <c r="D9" s="28">
-        <v>0.751</v>
-      </c>
-      <c r="E9">
-        <v>0.9607</v>
-      </c>
-      <c r="F9" s="28">
-        <v>0.86480000000000001</v>
-      </c>
-      <c r="G9">
-        <v>0.62270000000000003</v>
-      </c>
-      <c r="H9" s="28">
-        <v>0.55569999999999997</v>
-      </c>
-      <c r="I9">
-        <v>1.2606999999999999</v>
-      </c>
-      <c r="J9" s="28">
-        <v>0.443</v>
-      </c>
-      <c r="K9">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="L9" s="7">
-        <v>0.65362500000000001</v>
-      </c>
-      <c r="M9" s="9">
-        <v>0.942025</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10">
-        <v>0.75980000000000003</v>
-      </c>
-      <c r="C10">
-        <v>0.82220000000000004</v>
-      </c>
-      <c r="F10">
-        <v>0.86309999999999998</v>
-      </c>
-      <c r="G10">
-        <v>0.63129999999999997</v>
-      </c>
-      <c r="H10">
-        <v>0.53280000000000005</v>
-      </c>
-      <c r="I10">
-        <v>1.2661</v>
-      </c>
-      <c r="J10">
-        <v>0.44950000000000001</v>
-      </c>
-      <c r="K10">
-        <v>0.90169999999999995</v>
-      </c>
-      <c r="L10" s="7">
-        <f t="shared" ref="L10:M12" si="1">AVERAGE(D10,F10,H10,J10)</f>
-        <v>0.61513333333333342</v>
-      </c>
-      <c r="M10" s="9">
-        <f t="shared" si="1"/>
-        <v>0.93303333333333338</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="30">
-        <v>0.76670000000000005</v>
-      </c>
-      <c r="C11">
-        <v>0.79520000000000002</v>
-      </c>
-      <c r="F11" s="30">
-        <v>0.8669</v>
-      </c>
-      <c r="G11">
-        <v>0.63280000000000003</v>
-      </c>
-      <c r="J11">
-        <v>0.46839999999999998</v>
-      </c>
-      <c r="K11">
-        <v>0.84140000000000004</v>
-      </c>
-      <c r="L11" s="7">
-        <f t="shared" si="1"/>
-        <v>0.66764999999999997</v>
-      </c>
-      <c r="M11" s="9">
-        <f t="shared" si="1"/>
-        <v>0.73710000000000009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="30">
-        <v>0.75880000000000003</v>
-      </c>
-      <c r="C12">
-        <v>0.83179999999999998</v>
-      </c>
-      <c r="F12" s="30">
-        <v>0.871</v>
-      </c>
-      <c r="G12" s="30">
-        <v>0.60240000000000005</v>
-      </c>
-      <c r="J12">
-        <v>0.51029999999999998</v>
-      </c>
-      <c r="K12">
-        <v>0.87029999999999996</v>
-      </c>
-      <c r="L12" s="7">
-        <f t="shared" si="1"/>
-        <v>0.69064999999999999</v>
-      </c>
-      <c r="M12" s="9">
-        <f t="shared" si="1"/>
-        <v>0.73635000000000006</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" s="30">
-        <v>0.76100000000000001</v>
-      </c>
-      <c r="C13">
-        <v>0.88700000000000001</v>
-      </c>
-      <c r="D13">
-        <v>0.76500000000000001</v>
-      </c>
-      <c r="E13">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="F13" s="30">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="G13" s="30">
-        <v>0.84</v>
-      </c>
-      <c r="H13">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="I13">
-        <v>1.5529999999999999</v>
-      </c>
-      <c r="J13">
-        <v>0.503</v>
-      </c>
-      <c r="K13">
-        <v>1.2629999999999999</v>
-      </c>
-      <c r="L13" s="7">
-        <f t="shared" ref="L13" si="2">AVERAGE(D13,F13,H13,J13)</f>
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="M13" s="9">
-        <f t="shared" ref="M13" si="3">AVERAGE(E13,G13,I13,K13)</f>
-        <v>1.1484999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="M3:M13">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:L13">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B6 B9">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D6 D9">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F6 F9">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H7 H9">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J7 J9">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C6">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E6">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G7">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I6">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K6">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B13">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C13">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D13">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E13">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F13">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G13">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H13">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I13">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J13">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K13">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" customWidth="1"/>
-    <col min="12" max="12" width="4.7109375" customWidth="1"/>
-    <col min="13" max="13" width="5.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="B1" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="38"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="B2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="30">
-        <v>0.65</v>
-      </c>
-      <c r="C3">
-        <v>0.59299999999999997</v>
-      </c>
-      <c r="D3">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="E3">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="F3" s="30">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="G3" s="30">
-        <v>0.41899999999999998</v>
-      </c>
-      <c r="H3">
-        <v>0.72299999999999998</v>
-      </c>
-      <c r="I3">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="J3">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="K3">
-        <v>1.1080000000000001</v>
-      </c>
-      <c r="L3" s="7">
-        <f t="shared" ref="L3:M3" si="0">AVERAGE(D3,F3,H3,J3)</f>
-        <v>0.65149999999999997</v>
-      </c>
-      <c r="M3" s="9">
-        <f t="shared" si="0"/>
-        <v>0.65325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="M3">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3">
-    <cfRule type="colorScale" priority="46">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F3">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J3">
-    <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="colorScale" priority="56">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AN9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10944,7 +10130,7 @@
     <col min="2" max="31" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="34" width="4.5703125" customWidth="1"/>
     <col min="35" max="37" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="40" width="7.7109375" customWidth="1"/>
+    <col min="38" max="40" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -11499,15 +10685,15 @@
         <v>0.65649999999999997</v>
       </c>
       <c r="AL5" s="10">
-        <f t="shared" ref="AL5:AL6" si="1">AVERAGE(B5,E5,H5,N5,Q5,T5,W5,Z5,AC5,AF5,AI5)</f>
+        <f t="shared" ref="AL5:AL7" si="1">AVERAGE(B5,E5,H5,N5,Q5,T5,W5,Z5,AC5,AF5,AI5)</f>
         <v>0.37953636363636362</v>
       </c>
       <c r="AM5" s="11">
-        <f t="shared" ref="AM5:AM6" si="2">AVERAGE(C5,F5,I5,O5,R5,U5,X5,AA5,AD5,AG5,AJ5)</f>
+        <f t="shared" ref="AM5:AM7" si="2">AVERAGE(C5,F5,I5,O5,R5,U5,X5,AA5,AD5,AG5,AJ5)</f>
         <v>0.59595454545454551</v>
       </c>
       <c r="AN5" s="12">
-        <f t="shared" ref="AN5:AN6" si="3">AVERAGE(D5,G5,J5,P5,S5,V5,Y5,AB5,AE5,AH5,AK5)</f>
+        <f t="shared" ref="AN5:AN7" si="3">AVERAGE(D5,G5,J5,P5,S5,V5,Y5,AB5,AE5,AH5,AK5)</f>
         <v>0.4236454545454546</v>
       </c>
     </row>
@@ -11636,93 +10822,255 @@
         <v>0.51095454545454555</v>
       </c>
     </row>
-    <row r="7" spans="1:40" ht="23.25">
+    <row r="7" spans="1:40">
       <c r="A7" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="10"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="10"/>
-      <c r="AA7" s="11"/>
-      <c r="AB7" s="12"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="16"/>
-      <c r="AF7" s="10"/>
-      <c r="AG7" s="11"/>
-      <c r="AH7" s="12"/>
-      <c r="AI7" s="11"/>
-      <c r="AJ7" s="11"/>
-      <c r="AK7" s="12"/>
-      <c r="AL7" s="10"/>
-      <c r="AM7" s="11"/>
-      <c r="AN7" s="12"/>
+        <v>126</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.51259999999999994</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.21579999999999999</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.30370000000000003</v>
+      </c>
+      <c r="E7" s="15">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.17130000000000001</v>
+      </c>
+      <c r="G7" s="11">
+        <v>0.1116</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.44059999999999999</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.82769999999999999</v>
+      </c>
+      <c r="J7" s="11">
+        <v>0.57509999999999994</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.1328</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.20269999999999999</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0.3034</v>
+      </c>
+      <c r="O7" s="11">
+        <v>0.86709999999999998</v>
+      </c>
+      <c r="P7" s="11">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>0.12429999999999999</v>
+      </c>
+      <c r="R7" s="11">
+        <v>0.84730000000000005</v>
+      </c>
+      <c r="S7" s="12">
+        <v>0.2167</v>
+      </c>
+      <c r="T7" s="10">
+        <v>0.74050000000000005</v>
+      </c>
+      <c r="U7" s="11">
+        <v>0.91039999999999999</v>
+      </c>
+      <c r="V7" s="12">
+        <v>0.81669999999999998</v>
+      </c>
+      <c r="W7" s="10">
+        <v>0.2238</v>
+      </c>
+      <c r="X7" s="11">
+        <v>0.4335</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>0.29520000000000002</v>
+      </c>
+      <c r="Z7" s="10">
+        <v>0.14230000000000001</v>
+      </c>
+      <c r="AA7" s="11">
+        <v>0.6492</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>0.23350000000000001</v>
+      </c>
+      <c r="AC7" s="10">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="AD7" s="13">
+        <v>0.49230000000000002</v>
+      </c>
+      <c r="AE7" s="16">
+        <v>0.1032</v>
+      </c>
+      <c r="AF7" s="10">
+        <v>0.84450000000000003</v>
+      </c>
+      <c r="AG7" s="11">
+        <v>0.83309999999999995</v>
+      </c>
+      <c r="AH7" s="12">
+        <v>0.83879999999999999</v>
+      </c>
+      <c r="AI7" s="11">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="AJ7" s="11">
+        <v>0.86180000000000001</v>
+      </c>
+      <c r="AK7" s="12">
+        <v>0.67</v>
+      </c>
+      <c r="AL7" s="10">
+        <f t="shared" si="1"/>
+        <v>0.36549090909090914</v>
+      </c>
+      <c r="AM7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.64631818181818179</v>
+      </c>
+      <c r="AN7" s="12">
+        <f t="shared" si="3"/>
+        <v>0.41945454545454547</v>
+      </c>
     </row>
     <row r="8" spans="1:40">
       <c r="A8" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="12"/>
-      <c r="Z8" s="10"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="12"/>
-      <c r="AC8" s="10"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="16"/>
-      <c r="AF8" s="10"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="12"/>
-      <c r="AL8" s="10"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="12"/>
+        <v>127</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.22950000000000001</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.4168</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.17749999999999999</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.35630000000000001</v>
+      </c>
+      <c r="G8" s="11">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.46229999999999999</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="J8" s="11">
+        <v>0.57979999999999998</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.62760000000000005</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0.45040000000000002</v>
+      </c>
+      <c r="O8" s="11">
+        <v>0.86029999999999995</v>
+      </c>
+      <c r="P8" s="11">
+        <v>0.59130000000000005</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>0.3458</v>
+      </c>
+      <c r="R8" s="11">
+        <v>0.85340000000000005</v>
+      </c>
+      <c r="S8" s="12">
+        <v>0.49209999999999998</v>
+      </c>
+      <c r="T8" s="10">
+        <v>0.76429999999999998</v>
+      </c>
+      <c r="U8" s="11">
+        <v>0.82320000000000004</v>
+      </c>
+      <c r="V8" s="12">
+        <v>0.79259999999999997</v>
+      </c>
+      <c r="W8" s="10">
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="X8" s="11">
+        <v>0.47060000000000002</v>
+      </c>
+      <c r="Y8" s="12">
+        <v>0.50039999999999996</v>
+      </c>
+      <c r="Z8" s="10">
+        <v>0.29720000000000002</v>
+      </c>
+      <c r="AA8" s="11">
+        <v>0.67930000000000001</v>
+      </c>
+      <c r="AB8" s="12">
+        <v>0.41349999999999998</v>
+      </c>
+      <c r="AC8" s="10">
+        <v>0.18809999999999999</v>
+      </c>
+      <c r="AD8" s="13">
+        <v>0.29530000000000001</v>
+      </c>
+      <c r="AE8" s="16">
+        <v>0.2298</v>
+      </c>
+      <c r="AF8" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="AG8" s="11">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="AH8" s="12">
+        <v>0.83379999999999999</v>
+      </c>
+      <c r="AI8" s="11">
+        <v>0.66639999999999999</v>
+      </c>
+      <c r="AJ8" s="11">
+        <v>0.68830000000000002</v>
+      </c>
+      <c r="AK8" s="12">
+        <v>0.67720000000000002</v>
+      </c>
+      <c r="AL8" s="10">
+        <f t="shared" ref="AL8" si="4">AVERAGE(B8,E8,H8,N8,Q8,T8,W8,Z8,AC8,AF8,AI8)</f>
+        <v>0.46051818181818188</v>
+      </c>
+      <c r="AM8" s="11">
+        <f t="shared" ref="AM8" si="5">AVERAGE(C8,F8,I8,O8,R8,U8,X8,AA8,AD8,AG8,AJ8)</f>
+        <v>0.63309090909090926</v>
+      </c>
+      <c r="AN8" s="12">
+        <f t="shared" ref="AN8" si="6">AVERAGE(D8,G8,J8,P8,S8,V8,Y8,AB8,AE8,AH8,AK8)</f>
+        <v>0.51304545454545458</v>
+      </c>
     </row>
     <row r="9" spans="1:40">
       <c r="A9" s="5"/>
@@ -12540,4 +11888,1146 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="37"/>
+      <c r="F1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="38"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0.76639999999999997</v>
+      </c>
+      <c r="C3" s="9">
+        <f>0.9145*0.9145</f>
+        <v>0.83631024999999992</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="E3" s="9">
+        <f>1.004*1.004</f>
+        <v>1.008016</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.8518</v>
+      </c>
+      <c r="G3" s="9">
+        <f>0.8217*0.8217</f>
+        <v>0.67519088999999999</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.53010000000000002</v>
+      </c>
+      <c r="I3" s="9">
+        <f>1.2034*1.2034</f>
+        <v>1.44817156</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.49890000000000001</v>
+      </c>
+      <c r="K3" s="8">
+        <f>1.0986*1.0986</f>
+        <v>1.2069219600000001</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:M6" si="0">AVERAGE(D3,F3,H3,J3)</f>
+        <v>0.65615000000000001</v>
+      </c>
+      <c r="M3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0845751025000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0.74750000000000005</v>
+      </c>
+      <c r="C4" s="9">
+        <f>1.0015*1.0015</f>
+        <v>1.0030022500000002</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.60819999999999996</v>
+      </c>
+      <c r="E4" s="9">
+        <f>1.2472 *1.2472</f>
+        <v>1.5555078400000002</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0.7742</v>
+      </c>
+      <c r="G4" s="9">
+        <f>1.0482*1.0482</f>
+        <v>1.09872324</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.4163</v>
+      </c>
+      <c r="I4" s="9">
+        <f>1.4015*1.4015</f>
+        <v>1.9642022499999998</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.51639999999999997</v>
+      </c>
+      <c r="K4" s="8">
+        <f>0.908*0.908</f>
+        <v>0.82446400000000009</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.57877500000000004</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3607243325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0.73160000000000003</v>
+      </c>
+      <c r="C5" s="9">
+        <f>0.9703*0.9703</f>
+        <v>0.94148209000000005</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.7097</v>
+      </c>
+      <c r="E5" s="9">
+        <f>1.0558*1.0558</f>
+        <v>1.1147136400000002</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.83860000000000001</v>
+      </c>
+      <c r="G5" s="9">
+        <f>0.8519*0.8519</f>
+        <v>0.72573361000000003</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.50409999999999999</v>
+      </c>
+      <c r="I5" s="9">
+        <f>1.2313*1.2313</f>
+        <v>1.5160996900000001</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="K5" s="9">
+        <f>1.1224*1.1224</f>
+        <v>1.2597817600000001</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.63485000000000003</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1540821750000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="C6" s="9">
+        <f>1.0332 * 1.0332</f>
+        <v>1.0675022399999998</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.5756</v>
+      </c>
+      <c r="E6" s="9">
+        <f>1.2736*1.2736</f>
+        <v>1.6220569600000001</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.75049999999999994</v>
+      </c>
+      <c r="G6" s="9">
+        <f>1.0584*1.0584</f>
+        <v>1.1202105600000001</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.38679999999999998</v>
+      </c>
+      <c r="I6" s="9">
+        <f>1.403*1.403</f>
+        <v>1.9684090000000001</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="K6" s="9">
+        <f>0.9644*0.9644</f>
+        <v>0.93006736000000012</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.5363</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4101859700000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="31">
+        <v>0.76639999999999997</v>
+      </c>
+      <c r="C7">
+        <f>0.9145*0.9145</f>
+        <v>0.83631024999999992</v>
+      </c>
+      <c r="D7" s="31">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="E7">
+        <f>1.004*1.004</f>
+        <v>1.008016</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.8518</v>
+      </c>
+      <c r="G7">
+        <f>0.8217*0.8217</f>
+        <v>0.67519088999999999</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="31">
+        <v>0.7651</v>
+      </c>
+      <c r="C8">
+        <f>0.934*0.934</f>
+        <v>0.87235600000000013</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.76449999999999996</v>
+      </c>
+      <c r="C9">
+        <v>0.80910000000000004</v>
+      </c>
+      <c r="D9" s="28">
+        <v>0.751</v>
+      </c>
+      <c r="E9">
+        <v>0.9607</v>
+      </c>
+      <c r="F9" s="28">
+        <v>0.86480000000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.62270000000000003</v>
+      </c>
+      <c r="H9" s="28">
+        <v>0.55569999999999997</v>
+      </c>
+      <c r="I9">
+        <v>1.2606999999999999</v>
+      </c>
+      <c r="J9" s="28">
+        <v>0.443</v>
+      </c>
+      <c r="K9">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.65362500000000001</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0.942025</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>0.75980000000000003</v>
+      </c>
+      <c r="C10">
+        <v>0.82220000000000004</v>
+      </c>
+      <c r="F10">
+        <v>0.86309999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.63129999999999997</v>
+      </c>
+      <c r="H10">
+        <v>0.53280000000000005</v>
+      </c>
+      <c r="I10">
+        <v>1.2661</v>
+      </c>
+      <c r="J10">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.90169999999999995</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" ref="L10:M12" si="1">AVERAGE(D10,F10,H10,J10)</f>
+        <v>0.61513333333333342</v>
+      </c>
+      <c r="M10" s="9">
+        <f t="shared" si="1"/>
+        <v>0.93303333333333338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.79520000000000002</v>
+      </c>
+      <c r="F11" s="30">
+        <v>0.8669</v>
+      </c>
+      <c r="G11">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="J11">
+        <v>0.46839999999999998</v>
+      </c>
+      <c r="K11">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.66764999999999997</v>
+      </c>
+      <c r="M11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.73710000000000009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="30">
+        <v>0.75880000000000003</v>
+      </c>
+      <c r="C12">
+        <v>0.83179999999999998</v>
+      </c>
+      <c r="F12" s="30">
+        <v>0.871</v>
+      </c>
+      <c r="G12" s="30">
+        <v>0.60240000000000005</v>
+      </c>
+      <c r="J12">
+        <v>0.51029999999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.87029999999999996</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.69064999999999999</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="1"/>
+        <v>0.73635000000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="30">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="C13">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F13" s="30">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="G13" s="30">
+        <v>0.84</v>
+      </c>
+      <c r="H13">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="I13">
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="J13">
+        <v>0.503</v>
+      </c>
+      <c r="K13">
+        <v>1.2629999999999999</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" ref="L13:L14" si="2">AVERAGE(D13,F13,H13,J13)</f>
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" ref="M13:M14" si="3">AVERAGE(E13,G13,I13,K13)</f>
+        <v>1.1484999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="30">
+        <v>0.75449999999999995</v>
+      </c>
+      <c r="C14">
+        <v>0.8508</v>
+      </c>
+      <c r="D14">
+        <v>0.76549999999999996</v>
+      </c>
+      <c r="E14">
+        <v>0.94220000000000004</v>
+      </c>
+      <c r="F14" s="30">
+        <v>0.86270000000000002</v>
+      </c>
+      <c r="G14" s="30">
+        <v>0.83450000000000002</v>
+      </c>
+      <c r="H14">
+        <v>0.54590000000000005</v>
+      </c>
+      <c r="I14">
+        <v>0.1217</v>
+      </c>
+      <c r="J14">
+        <v>0.50070000000000003</v>
+      </c>
+      <c r="K14">
+        <v>1.1496</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="2"/>
+        <v>0.66870000000000007</v>
+      </c>
+      <c r="M14" s="9">
+        <f t="shared" si="3"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1"/>
+      <c r="B15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1"/>
+      <c r="B16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M3:M16">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L16">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B6 B9">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D6 D9">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F6 F9">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H7 H9">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J7 J9">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C6">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E6">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G7">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I6">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K6">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:B16">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C16">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D16">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E16">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G16">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H16">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K16">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="4.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
+    <col min="12" max="12" width="4.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="37"/>
+      <c r="F1" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="38"/>
+      <c r="H1" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="38"/>
+      <c r="J1" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="38"/>
+      <c r="L1" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="38"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="B2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="30">
+        <v>0.65</v>
+      </c>
+      <c r="C3">
+        <v>0.59299999999999997</v>
+      </c>
+      <c r="D3">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="E3">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="G3" s="30">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="H3">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="J3">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="K3">
+        <v>1.1080000000000001</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:M3" si="0">AVERAGE(D3,F3,H3,J3)</f>
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="M3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.65325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="colorScale" priority="47">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some DISFA sampling results.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -10120,8 +10120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10824,253 +10824,166 @@
     </row>
     <row r="7" spans="1:40">
       <c r="A7" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B7" s="10">
-        <v>0.51259999999999994</v>
+        <v>0.2737</v>
       </c>
       <c r="C7" s="11">
-        <v>0.21579999999999999</v>
+        <v>0.35160000000000002</v>
       </c>
       <c r="D7" s="12">
-        <v>0.30370000000000003</v>
+        <v>0.30780000000000002</v>
       </c>
       <c r="E7" s="15">
-        <v>8.2799999999999999E-2</v>
+        <v>0.33879999999999999</v>
       </c>
       <c r="F7" s="11">
-        <v>0.17130000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="G7" s="11">
-        <v>0.1116</v>
+        <v>0.2515</v>
       </c>
       <c r="H7" s="10">
-        <v>0.44059999999999999</v>
+        <v>0.71409999999999996</v>
       </c>
       <c r="I7" s="11">
-        <v>0.82769999999999999</v>
+        <v>0.63449999999999995</v>
       </c>
       <c r="J7" s="11">
-        <v>0.57509999999999994</v>
+        <v>0.67190000000000005</v>
       </c>
       <c r="K7" s="10">
-        <v>0.1328</v>
+        <v>9.8699999999999996E-2</v>
       </c>
       <c r="L7" s="11">
-        <v>0.42799999999999999</v>
+        <v>0.52470000000000006</v>
       </c>
       <c r="M7" s="11">
-        <v>0.20269999999999999</v>
+        <v>0.16619999999999999</v>
       </c>
       <c r="N7" s="10">
-        <v>0.3034</v>
+        <v>0.67020000000000002</v>
       </c>
       <c r="O7" s="11">
-        <v>0.86709999999999998</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="P7" s="11">
-        <v>0.44950000000000001</v>
+        <v>0.65259999999999996</v>
       </c>
       <c r="Q7" s="10">
-        <v>0.12429999999999999</v>
+        <v>0.54530000000000001</v>
       </c>
       <c r="R7" s="11">
-        <v>0.84730000000000005</v>
+        <v>0.63300000000000001</v>
       </c>
       <c r="S7" s="12">
-        <v>0.2167</v>
+        <v>0.58589999999999998</v>
       </c>
       <c r="T7" s="10">
-        <v>0.74050000000000005</v>
+        <v>0.82779999999999998</v>
       </c>
       <c r="U7" s="11">
-        <v>0.91039999999999999</v>
+        <v>0.74950000000000006</v>
       </c>
       <c r="V7" s="12">
-        <v>0.81669999999999998</v>
+        <v>0.78649999999999998</v>
       </c>
       <c r="W7" s="10">
-        <v>0.2238</v>
+        <v>0.52739999999999998</v>
       </c>
       <c r="X7" s="11">
-        <v>0.4335</v>
+        <v>0.45879999999999999</v>
       </c>
       <c r="Y7" s="12">
-        <v>0.29520000000000002</v>
+        <v>0.49070000000000003</v>
       </c>
       <c r="Z7" s="10">
-        <v>0.14230000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="AA7" s="11">
-        <v>0.6492</v>
+        <v>0.55230000000000001</v>
       </c>
       <c r="AB7" s="12">
-        <v>0.23350000000000001</v>
+        <v>0.43590000000000001</v>
       </c>
       <c r="AC7" s="10">
-        <v>5.7599999999999998E-2</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="AD7" s="13">
-        <v>0.49230000000000002</v>
+        <v>0.28339999999999999</v>
       </c>
       <c r="AE7" s="16">
-        <v>0.1032</v>
+        <v>0.23860000000000001</v>
       </c>
       <c r="AF7" s="10">
-        <v>0.84450000000000003</v>
+        <v>0.93989999999999996</v>
       </c>
       <c r="AG7" s="11">
-        <v>0.83309999999999995</v>
+        <v>0.74409999999999998</v>
       </c>
       <c r="AH7" s="12">
-        <v>0.83879999999999999</v>
-      </c>
-      <c r="AI7" s="11">
-        <v>0.54800000000000004</v>
-      </c>
-      <c r="AJ7" s="11">
-        <v>0.86180000000000001</v>
-      </c>
-      <c r="AK7" s="12">
-        <v>0.67</v>
-      </c>
+        <v>0.8306</v>
+      </c>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="12"/>
       <c r="AL7" s="10">
         <f t="shared" si="1"/>
-        <v>0.36549090909090914</v>
+        <v>0.54032000000000002</v>
       </c>
       <c r="AM7" s="11">
         <f t="shared" si="2"/>
-        <v>0.64631818181818179</v>
+        <v>0.52432000000000001</v>
       </c>
       <c r="AN7" s="12">
         <f t="shared" si="3"/>
-        <v>0.41945454545454547</v>
+        <v>0.52519999999999989</v>
       </c>
     </row>
     <row r="8" spans="1:40">
       <c r="A8" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="10">
-        <v>0.22950000000000001</v>
-      </c>
-      <c r="C8" s="11">
-        <v>0.4168</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E8" s="15">
-        <v>0.17749999999999999</v>
-      </c>
-      <c r="F8" s="11">
-        <v>0.35630000000000001</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0.23699999999999999</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0.46229999999999999</v>
-      </c>
-      <c r="I8" s="11">
-        <v>0.77749999999999997</v>
-      </c>
-      <c r="J8" s="11">
-        <v>0.57979999999999998</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="L8" s="11">
-        <v>0.62760000000000005</v>
-      </c>
-      <c r="M8" s="11">
-        <v>0.17249999999999999</v>
-      </c>
-      <c r="N8" s="10">
-        <v>0.45040000000000002</v>
-      </c>
-      <c r="O8" s="11">
-        <v>0.86029999999999995</v>
-      </c>
-      <c r="P8" s="11">
-        <v>0.59130000000000005</v>
-      </c>
-      <c r="Q8" s="10">
-        <v>0.3458</v>
-      </c>
-      <c r="R8" s="11">
-        <v>0.85340000000000005</v>
-      </c>
-      <c r="S8" s="12">
-        <v>0.49209999999999998</v>
-      </c>
-      <c r="T8" s="10">
-        <v>0.76429999999999998</v>
-      </c>
-      <c r="U8" s="11">
-        <v>0.82320000000000004</v>
-      </c>
-      <c r="V8" s="12">
-        <v>0.79259999999999997</v>
-      </c>
-      <c r="W8" s="10">
-        <v>0.53420000000000001</v>
-      </c>
-      <c r="X8" s="11">
-        <v>0.47060000000000002</v>
-      </c>
-      <c r="Y8" s="12">
-        <v>0.50039999999999996</v>
-      </c>
-      <c r="Z8" s="10">
-        <v>0.29720000000000002</v>
-      </c>
-      <c r="AA8" s="11">
-        <v>0.67930000000000001</v>
-      </c>
-      <c r="AB8" s="12">
-        <v>0.41349999999999998</v>
-      </c>
-      <c r="AC8" s="10">
-        <v>0.18809999999999999</v>
-      </c>
-      <c r="AD8" s="13">
-        <v>0.29530000000000001</v>
-      </c>
-      <c r="AE8" s="16">
-        <v>0.2298</v>
-      </c>
-      <c r="AF8" s="10">
-        <v>0.95</v>
-      </c>
-      <c r="AG8" s="11">
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="AH8" s="12">
-        <v>0.83379999999999999</v>
-      </c>
-      <c r="AI8" s="11">
-        <v>0.66639999999999999</v>
-      </c>
-      <c r="AJ8" s="11">
-        <v>0.68830000000000002</v>
-      </c>
-      <c r="AK8" s="12">
-        <v>0.67720000000000002</v>
-      </c>
-      <c r="AL8" s="10">
-        <f t="shared" ref="AL8" si="4">AVERAGE(B8,E8,H8,N8,Q8,T8,W8,Z8,AC8,AF8,AI8)</f>
-        <v>0.46051818181818188</v>
-      </c>
-      <c r="AM8" s="11">
-        <f t="shared" ref="AM8" si="5">AVERAGE(C8,F8,I8,O8,R8,U8,X8,AA8,AD8,AG8,AJ8)</f>
-        <v>0.63309090909090926</v>
-      </c>
-      <c r="AN8" s="12">
-        <f t="shared" ref="AN8" si="6">AVERAGE(D8,G8,J8,P8,S8,V8,Y8,AB8,AE8,AH8,AK8)</f>
-        <v>0.51304545454545458</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="11"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="11"/>
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="12"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="11"/>
+      <c r="AN8" s="12"/>
     </row>
     <row r="9" spans="1:40">
       <c r="A9" s="5"/>
@@ -11894,7 +11807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Making sure test folds are randomised properly.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
     <t>only on one validation set, needs to be done properly? Although this does not look promissing, needs to be converted to regressor first</t>
   </si>
   <si>
-    <t>do a step by step comparison here, difficult while stuff keeps crashing</t>
+    <t>This needs to be done by randomising the test fold, but how?</t>
   </si>
 </sst>
 </file>
@@ -9006,7 +9006,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V63 S63">
+  <conditionalFormatting sqref="S63 V63">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -9018,7 +9018,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V63 S63">
+  <conditionalFormatting sqref="S63 V63">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -13871,17 +13871,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="24">
@@ -17814,7 +17814,7 @@
   <dimension ref="A1:AN23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="AP20" sqref="AP20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18502,7 +18502,7 @@
         <v>196</v>
       </c>
       <c r="B14" s="8">
-        <v>0.54690000000000005</v>
+        <v>0.55449999999999999</v>
       </c>
       <c r="C14" s="8">
         <v>0.39800000000000002</v>
@@ -18519,17 +18519,27 @@
       <c r="G14" s="8">
         <v>0.4158</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="H14" s="8">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.32569999999999999</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.34620000000000001</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0.18190000000000001</v>
+      </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8">
         <f t="shared" ref="N14:N21" si="3">AVERAGE(B14:M14)</f>
-        <v>0.47425</v>
-      </c>
-      <c r="O14" s="21"/>
+        <v>0.45322999999999991</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>206</v>
+      </c>
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
       <c r="R14" s="21"/>
@@ -18560,25 +18570,44 @@
         <v>198</v>
       </c>
       <c r="B16" s="29">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
+        <v>0.57230000000000003</v>
+      </c>
+      <c r="C16" s="29">
+        <v>0.45929999999999999</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0.59050000000000002</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0.60229999999999995</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0.51680000000000004</v>
+      </c>
+      <c r="H16" s="29">
+        <v>0.83530000000000004</v>
+      </c>
+      <c r="I16" s="29">
+        <v>0.39419999999999999</v>
+      </c>
+      <c r="J16" s="29">
+        <v>0.41820000000000002</v>
+      </c>
+      <c r="K16" s="29">
+        <v>0.2492</v>
+      </c>
+      <c r="L16" s="29">
+        <v>0.86150000000000004</v>
+      </c>
+      <c r="M16" s="29">
+        <v>0.6119</v>
+      </c>
       <c r="N16" s="29">
         <f t="shared" si="3"/>
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="O16" t="s">
-        <v>206</v>
+        <v>0.56779166666666669</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -19289,7 +19318,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="A1:I13"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19489,10 +19518,13 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="B2" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">

</xml_diff>

<commit_message>
Adding extra data and some more tests.
</commit_message>
<xml_diff>
--- a/results_v2.xlsx
+++ b/results_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="12930" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="BP4D" sheetId="1" r:id="rId1"/>
@@ -13,15 +13,16 @@
     <sheet name="BP4D_intensity" sheetId="3" r:id="rId4"/>
     <sheet name="BP4D_int_seg" sheetId="5" r:id="rId5"/>
     <sheet name="DISFA balanced split" sheetId="6" r:id="rId6"/>
-    <sheet name="SEMAINE balanced split" sheetId="7" r:id="rId7"/>
-    <sheet name="SEMAINE train DISFA test" sheetId="8" r:id="rId8"/>
+    <sheet name="SEMAINE train DISFA test" sheetId="8" r:id="rId7"/>
+    <sheet name="BP4D_train_DISFA_test" sheetId="9" r:id="rId8"/>
+    <sheet name="UNBC balanced split" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="206">
   <si>
     <t>DEVEL</t>
   </si>
@@ -636,9 +637,6 @@
   </si>
   <si>
     <t>average</t>
-  </si>
-  <si>
-    <t>only on one validation set, needs to be done properly? Although this does not look promissing, needs to be converted to regressor first</t>
   </si>
   <si>
     <t>This needs to be done by randomising the test fold, but how?</t>
@@ -1190,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK69"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1:AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9051,8 +9049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH78"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14169,7 +14167,7 @@
   <dimension ref="A1:AN13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AN2"/>
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16442,7 +16440,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17402,7 +17400,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17813,8 +17811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AP20" sqref="AP20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18502,43 +18500,47 @@
         <v>196</v>
       </c>
       <c r="B14" s="8">
-        <v>0.55449999999999999</v>
+        <v>0.54669999999999996</v>
       </c>
       <c r="C14" s="8">
-        <v>0.39800000000000002</v>
+        <v>0.4405</v>
       </c>
       <c r="D14" s="8">
-        <v>0.57040000000000002</v>
+        <v>0.58379999999999999</v>
       </c>
       <c r="E14" s="8">
-        <v>0.31469999999999998</v>
+        <v>0.35820000000000002</v>
       </c>
       <c r="F14" s="8">
-        <v>0.59970000000000001</v>
+        <v>0.56610000000000005</v>
       </c>
       <c r="G14" s="8">
-        <v>0.4158</v>
+        <v>0.4335</v>
       </c>
       <c r="H14" s="8">
-        <v>0.82540000000000002</v>
+        <v>0.82199999999999995</v>
       </c>
       <c r="I14" s="8">
-        <v>0.32569999999999999</v>
+        <v>0.26840000000000003</v>
       </c>
       <c r="J14" s="8">
-        <v>0.34620000000000001</v>
+        <v>0.30769999999999997</v>
       </c>
       <c r="K14" s="8">
-        <v>0.18190000000000001</v>
-      </c>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+        <v>0.158</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.80079999999999996</v>
+      </c>
+      <c r="M14" s="8">
+        <v>0.56040000000000001</v>
+      </c>
       <c r="N14" s="8">
         <f t="shared" ref="N14:N21" si="3">AVERAGE(B14:M14)</f>
-        <v>0.45322999999999991</v>
+        <v>0.48717499999999997</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P14" s="21"/>
       <c r="Q14" s="21"/>
@@ -18548,21 +18550,45 @@
       <c r="A15" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29" t="e">
+      <c r="B15" s="29">
+        <v>0.15659999999999999</v>
+      </c>
+      <c r="C15" s="29">
+        <v>0.10979999999999999</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0.56279999999999997</v>
+      </c>
+      <c r="E15" s="29">
+        <v>0.21029999999999999</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0.52839999999999998</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0.3337</v>
+      </c>
+      <c r="H15" s="29">
+        <v>0.80859999999999999</v>
+      </c>
+      <c r="I15" s="29">
+        <v>9.4700000000000006E-2</v>
+      </c>
+      <c r="J15" s="29">
+        <v>0.2109</v>
+      </c>
+      <c r="K15" s="29">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="L15" s="29">
+        <v>0.82950000000000002</v>
+      </c>
+      <c r="M15" s="29">
+        <v>0.44950000000000001</v>
+      </c>
+      <c r="N15" s="29">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.36328333333333324</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
@@ -18570,65 +18596,89 @@
         <v>198</v>
       </c>
       <c r="B16" s="29">
-        <v>0.57230000000000003</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="C16" s="29">
-        <v>0.45929999999999999</v>
+        <v>0.4163</v>
       </c>
       <c r="D16" s="29">
-        <v>0.70199999999999996</v>
+        <v>0.64670000000000005</v>
       </c>
       <c r="E16" s="29">
-        <v>0.59050000000000002</v>
+        <v>0.57210000000000005</v>
       </c>
       <c r="F16" s="29">
-        <v>0.60229999999999995</v>
+        <v>0.53539999999999999</v>
       </c>
       <c r="G16" s="29">
-        <v>0.51680000000000004</v>
+        <v>0.50860000000000005</v>
       </c>
       <c r="H16" s="29">
-        <v>0.83530000000000004</v>
+        <v>0.82479999999999998</v>
       </c>
       <c r="I16" s="29">
-        <v>0.39419999999999999</v>
+        <v>0.27010000000000001</v>
       </c>
       <c r="J16" s="29">
-        <v>0.41820000000000002</v>
+        <v>0.31080000000000002</v>
       </c>
       <c r="K16" s="29">
-        <v>0.2492</v>
+        <v>0.2334</v>
       </c>
       <c r="L16" s="29">
-        <v>0.86150000000000004</v>
+        <v>0.85619999999999996</v>
       </c>
       <c r="M16" s="29">
-        <v>0.6119</v>
+        <v>0.63139999999999996</v>
       </c>
       <c r="N16" s="29">
         <f t="shared" si="3"/>
-        <v>0.56779166666666669</v>
+        <v>0.53165000000000007</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-      <c r="N17" s="29" t="e">
+      <c r="B17" s="29">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="C17" s="29">
+        <v>0.39929999999999999</v>
+      </c>
+      <c r="D17" s="29">
+        <v>0.56689999999999996</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0.56510000000000005</v>
+      </c>
+      <c r="F17" s="29">
+        <v>0.54149999999999998</v>
+      </c>
+      <c r="G17" s="29">
+        <v>0.48270000000000002</v>
+      </c>
+      <c r="H17" s="29">
+        <v>0.81520000000000004</v>
+      </c>
+      <c r="I17" s="29">
+        <v>0.26590000000000003</v>
+      </c>
+      <c r="J17" s="29">
+        <v>0.29220000000000002</v>
+      </c>
+      <c r="K17" s="29">
+        <v>0.20730000000000001</v>
+      </c>
+      <c r="L17" s="29">
+        <v>0.86009999999999998</v>
+      </c>
+      <c r="M17" s="29">
+        <v>0.58260000000000001</v>
+      </c>
+      <c r="N17" s="29">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.5091500000000001</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -18733,6 +18783,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B23 C10:M11">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9 C12:C23">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -18744,7 +18806,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C9 C12:C23">
+  <conditionalFormatting sqref="D2:D9 D12:D23">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -18756,7 +18818,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D9 D12:D23">
+  <conditionalFormatting sqref="E2:E9 E12:E23">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -18768,7 +18830,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E9 E12:E23">
+  <conditionalFormatting sqref="F2:F9 F12:F16 F18:F23 F17:G17">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -18780,7 +18842,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F9 F12:F23">
+  <conditionalFormatting sqref="G2:G9 G12:G16 G18:G23">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -18792,7 +18854,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9 G12:G23">
+  <conditionalFormatting sqref="H2:H9 H12:H23">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -18804,7 +18866,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9 H12:H23">
+  <conditionalFormatting sqref="I2:I9 I12:I23">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -18816,7 +18878,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9 I12:I23">
+  <conditionalFormatting sqref="J2:J9 J12:J23">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -18828,7 +18890,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9 J12:J23">
+  <conditionalFormatting sqref="K2:K9 K12:K23">
     <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
@@ -18840,7 +18902,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K9 K12:K23">
+  <conditionalFormatting sqref="L2:L9 L12:L23">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -18852,7 +18914,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L9 L12:L23">
+  <conditionalFormatting sqref="M2:M9 M12:M23">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -18864,7 +18926,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M9 M12:M23">
+  <conditionalFormatting sqref="N2:N21">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -18876,7 +18938,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N21">
+  <conditionalFormatting sqref="B2:B25">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -18888,7 +18950,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B25">
+  <conditionalFormatting sqref="C2:C25">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -18900,7 +18962,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C25">
+  <conditionalFormatting sqref="E2:E22">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -18912,7 +18974,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E22">
+  <conditionalFormatting sqref="G2:G16 G18:G23">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -18924,7 +18986,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -18936,7 +18998,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
@@ -18948,7 +19010,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -18960,7 +19022,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="K2:K16">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -18972,7 +19034,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K16">
+  <conditionalFormatting sqref="L2:L21">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -18984,7 +19046,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L21">
+  <conditionalFormatting sqref="M2:M21">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -18996,7 +19058,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M21">
+  <conditionalFormatting sqref="B14:B17">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -19008,7 +19070,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B17">
+  <conditionalFormatting sqref="C14:C17">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -19020,7 +19082,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C17">
+  <conditionalFormatting sqref="N14:N17">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -19032,7 +19094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N14:N17">
+  <conditionalFormatting sqref="D14:D17">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -19044,7 +19106,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D17">
+  <conditionalFormatting sqref="E14:E17">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -19056,7 +19118,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14:E17">
+  <conditionalFormatting sqref="F14:F16 F17:G17">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -19068,19 +19130,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F14:F17">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F2:F13">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -19092,7 +19154,79 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G14:G16">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H13">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:H17">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I13">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:I17">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J13">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14:J17">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -19104,200 +19238,128 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K13">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14:K17">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:L17">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L13">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M13">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14:M17">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E13">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D13">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B13">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G14:G17">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H14:H17">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I17">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
     <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J14:J17">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K13">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14:K17">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L14:L17">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L13">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M13">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M14:M17">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D13">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C13">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B13">
-    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -19315,18 +19377,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -19340,291 +19405,611 @@
         <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>188</v>
       </c>
-      <c r="B2">
-        <v>0.35089999999999999</v>
-      </c>
-      <c r="C2">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="D2">
-        <v>0.2341</v>
-      </c>
-      <c r="E2">
-        <v>0.37640000000000001</v>
-      </c>
-      <c r="F2">
-        <v>8.6599999999999996E-2</v>
-      </c>
-      <c r="G2">
-        <v>0.38229999999999997</v>
-      </c>
-      <c r="H2">
-        <f>AVERAGE(B2:G2)</f>
-        <v>0.32771666666666666</v>
-      </c>
-      <c r="I2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="29">
+        <v>9.06E-2</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.62709999999999999</v>
+      </c>
+      <c r="D2" s="29">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E2" s="29">
+        <v>0.26569999999999999</v>
+      </c>
+      <c r="F2" s="29">
+        <f t="shared" ref="F2:F13" si="0">AVERAGE(B2:E2)</f>
+        <v>0.2606</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>196</v>
       </c>
-      <c r="B3">
-        <v>0.45319999999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.57169999999999999</v>
-      </c>
-      <c r="D3">
-        <v>0.36320000000000002</v>
-      </c>
-      <c r="E3">
-        <v>0.37790000000000001</v>
-      </c>
-      <c r="F3">
-        <v>0.2233</v>
-      </c>
-      <c r="G3">
-        <v>0.43180000000000002</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H13" si="0">AVERAGE(B3:G3)</f>
-        <v>0.40351666666666669</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="29">
+        <v>0.2263</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.71220000000000006</v>
+      </c>
+      <c r="D3" s="29">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E3" s="29">
+        <v>8.2400000000000001E-2</v>
+      </c>
+      <c r="F3" s="29">
+        <f t="shared" si="0"/>
+        <v>0.26972500000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>189</v>
       </c>
-      <c r="B4">
-        <v>0.36180000000000001</v>
-      </c>
-      <c r="C4">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="D4">
-        <v>0.2341</v>
-      </c>
-      <c r="E4">
-        <v>0.37640000000000001</v>
-      </c>
-      <c r="F4">
-        <v>5.8200000000000002E-2</v>
-      </c>
-      <c r="G4">
-        <v>0.38229999999999997</v>
-      </c>
-      <c r="H4">
+      <c r="B4" s="29">
+        <v>0.3387</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0.6734</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.1094</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.2235</v>
+      </c>
+      <c r="F4" s="29">
         <f t="shared" si="0"/>
-        <v>0.32480000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.33624999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>198</v>
       </c>
-      <c r="B5">
-        <v>0.36480000000000001</v>
-      </c>
-      <c r="C5">
-        <v>0.57169999999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.36320000000000002</v>
-      </c>
-      <c r="E5">
-        <v>0.37790000000000001</v>
-      </c>
-      <c r="F5">
-        <v>0.2233</v>
-      </c>
-      <c r="G5">
-        <v>0.43180000000000002</v>
-      </c>
-      <c r="H5">
+      <c r="B5" s="29">
+        <v>0.39369999999999999</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.72719999999999996</v>
+      </c>
+      <c r="D5" s="29">
+        <v>0.11360000000000001</v>
+      </c>
+      <c r="E5" s="29">
+        <v>0.1363</v>
+      </c>
+      <c r="F5" s="29">
         <f t="shared" si="0"/>
-        <v>0.38878333333333331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.3427</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>188</v>
       </c>
-      <c r="F2" t="e">
-        <f t="shared" ref="F2:F13" si="0">AVERAGE(B2:E2)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="29">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="C2" s="29">
+        <v>0.12790000000000001</v>
+      </c>
+      <c r="D2" s="29">
+        <v>0.1537</v>
+      </c>
+      <c r="E2" s="29">
+        <v>0.51129999999999998</v>
+      </c>
+      <c r="F2" s="29">
+        <v>0.8095</v>
+      </c>
+      <c r="G2" s="29">
+        <v>9.9299999999999999E-2</v>
+      </c>
+      <c r="H2" s="29">
+        <v>0.19259999999999999</v>
+      </c>
+      <c r="I2" s="29">
+        <f>AVERAGE(B2:H2)</f>
+        <v>0.28447142857142854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>196</v>
       </c>
-      <c r="F3" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="29">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="C3" s="29">
+        <v>0.17610000000000001</v>
+      </c>
+      <c r="D3" s="29">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="E3" s="29">
+        <v>0.59260000000000002</v>
+      </c>
+      <c r="F3" s="29">
+        <v>0.54549999999999998</v>
+      </c>
+      <c r="G3" s="29">
+        <v>0.1051</v>
+      </c>
+      <c r="H3" s="29">
+        <v>0.25040000000000001</v>
+      </c>
+      <c r="I3" s="29">
+        <f>AVERAGE(B3:H3)</f>
+        <v>0.32217142857142861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>189</v>
       </c>
-      <c r="F4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="29">
+        <v>0.2354</v>
+      </c>
+      <c r="C4" s="29">
+        <v>0.25469999999999998</v>
+      </c>
+      <c r="D4" s="29">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0.63480000000000003</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0.83560000000000001</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0.21190000000000001</v>
+      </c>
+      <c r="H4" s="29">
+        <v>0.42759999999999998</v>
+      </c>
+      <c r="I4" s="29">
+        <f t="shared" ref="I4:I5" si="0">AVERAGE(B4:H4)</f>
+        <v>0.41871428571428571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>198</v>
       </c>
-      <c r="F5" t="e">
+      <c r="B5" s="29">
+        <v>0.43819999999999998</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.2918</v>
+      </c>
+      <c r="D5" s="29">
+        <v>0.40839999999999999</v>
+      </c>
+      <c r="E5" s="29">
+        <v>0.63429999999999997</v>
+      </c>
+      <c r="F5" s="29">
+        <v>0.81859999999999999</v>
+      </c>
+      <c r="G5" s="29">
+        <v>0.22389999999999999</v>
+      </c>
+      <c r="H5" s="29">
+        <v>0.42570000000000002</v>
+      </c>
+      <c r="I5" s="29">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F6" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F8" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F9" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.46298571428571428</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B5">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:F5">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:H5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I5">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2">
+        <v>2.93E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.48170000000000002</v>
+      </c>
+      <c r="D2">
+        <v>0.27879999999999999</v>
+      </c>
+      <c r="E2">
+        <v>8.7099999999999997E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.1188</v>
+      </c>
+      <c r="G2">
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="H2">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.19359999999999999</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.51190000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.25819999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.123</v>
+      </c>
+      <c r="F3">
+        <v>0.25619999999999998</v>
+      </c>
+      <c r="G3">
+        <v>0.47789999999999999</v>
+      </c>
+      <c r="H3">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.19470000000000001</v>
+      </c>
+      <c r="J3">
+        <v>7.3200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.46439999999999998</v>
+      </c>
+      <c r="D4">
+        <v>0.29809999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.16209999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.1183</v>
+      </c>
+      <c r="G4">
+        <v>0.41039999999999999</v>
+      </c>
+      <c r="H4">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="I4">
+        <v>0.29630000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5">
+        <v>0.1099</v>
+      </c>
+      <c r="C5">
+        <v>0.43209999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.26550000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.22040000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.39729999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.40279999999999999</v>
+      </c>
+      <c r="H5">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.28239999999999998</v>
+      </c>
+      <c r="J5">
+        <v>9.06E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>